<commit_message>
docs: update document with encounter resource tags from the Epic CCDA xml files #1197
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="430">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -141,6 +141,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Document.component.structuredBody.component.section.entry.observation
 where </t>
     </r>
@@ -195,6 +202,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Document.component.structuredBody.component.section.entry.observation
 where </t>
     </r>
@@ -234,6 +248,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Document.component.structuredBody.component.section.entry.observation
 where Document.component.structuredBody.component.section.templateId. root = '</t>
     </r>
@@ -267,6 +288,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Document.component.structuredBody.component.section.entry.observation
 where Document.component.structuredBody.component.section.templateId. root other than  '</t>
     </r>
@@ -396,6 +424,15 @@
   </si>
   <si>
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/middle-name"</t>
+  </si>
+  <si>
+    <t>name -&gt; use</t>
+  </si>
+  <si>
+    <t>Document.recordTarget.patientRole.patient.name.use</t>
+  </si>
+  <si>
+    <t>"use" : "official",</t>
   </si>
   <si>
     <t>name -&gt; family</t>
@@ -2153,6 +2190,86 @@
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/shinny-encounter"</t>
   </si>
   <si>
+    <t>identifier -&gt; system</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.id.root</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"identifier": [
+          {
+            "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "urn:oid:1.2.840.114350.1.13.861.1.7.3.698084.8",
+            "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "10011574538"
+          }
+        ],</t>
+    </r>
+  </si>
+  <si>
+    <t>Tentatively mapped the Identifier -&gt; system</t>
+  </si>
+  <si>
+    <t>identifier -&gt; value</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.id.extension</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the Identifier -&gt; value</t>
+  </si>
+  <si>
+    <t>"finished"</t>
+  </si>
+  <si>
     <t>"status" : "finished",</t>
   </si>
   <si>
@@ -2160,6 +2277,9 @@
   </si>
   <si>
     <t>class -&gt; code</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.code.code</t>
   </si>
   <si>
     <r>
@@ -2172,7 +2292,28 @@
       </rPr>
       <t>"class" : [{
     "coding" : [{
-      "system" : "http://terminology.hl7.org/CodeSystem/v3-ActCode",
+      "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "http://terminology.hl7.org/CodeSystem/v3-ActCode",
       "code" : "</t>
     </r>
     <r>
@@ -2195,19 +2336,59 @@
         <scheme val="minor"/>
       </rPr>
       <t>",
-      "display" : "inpatient encounter"
+      "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "inpatient encounter"
     }]
   }],</t>
     </r>
   </si>
   <si>
-    <t>Path to get the class.code</t>
+    <t>Tentatively mapped the code -&gt; code</t>
+  </si>
+  <si>
+    <t>class -&gt; system</t>
+  </si>
+  <si>
+    <t>"http://terminology.hl7.org/CodeSystem/v3-ActCode"</t>
+  </si>
+  <si>
+    <t>Tentatively given the system as 
+"http://terminology.hl7.org/CodeSystem/v3-ActCode"</t>
+  </si>
+  <si>
+    <t>class -&gt; display</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.code.displayName</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the code -&gt; displayName</t>
   </si>
   <si>
     <t>type -&gt; coding -&gt; code</t>
   </si>
   <si>
-    <t>Document.componentOf.encompassingEncounter.code.value</t>
+    <t>Document.componentOf.encompassingEncounter.code.translation.code</t>
   </si>
   <si>
     <r>
@@ -2287,24 +2468,60 @@
       </rPr>
       <t>" : "Direct questioning (procedure)"
         }],
-        "text" : "Direct questioning (procedure)"
+        "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "Direct questioning (procedure)"
       }],</t>
     </r>
   </si>
   <si>
+    <t>Tentatively mapped the code -&gt; translation -&gt; code</t>
+  </si>
+  <si>
     <t>type -&gt; coding -&gt; display</t>
   </si>
   <si>
-    <t>Document.componentOf.encompassingEncounter.code.displayName</t>
+    <t>Document.componentOf.encompassingEncounter.code.translation.displayName</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the code -&gt; translation -&gt; displayName</t>
   </si>
   <si>
     <t>type -&gt; coding -&gt; system</t>
   </si>
   <si>
-    <t>"http://snomed.info/sct"</t>
-  </si>
-  <si>
-    <t>Tentatively mapped the type -&gt; system</t>
+    <t>Document.componentOf.encompassingEncounter.code.translation.codeSystem</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the code -&gt; translation -&gt; codeSystem</t>
+  </si>
+  <si>
+    <t>type -&gt; text</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.code.originalText</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the code -&gt; originalText</t>
   </si>
   <si>
     <t>period -&gt; start</t>
@@ -2376,17 +2593,327 @@
     <t>Document.componentOf.encompassingEncounter.effectiveTime.high.value</t>
   </si>
   <si>
+    <t>participant -&gt; type -&gt; coding -&gt; system</t>
+  </si>
+  <si>
+    <t>"http://terminology.hl7.org/CodeSystem/v3-ParticipationType"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"participant": [{
+            "type": [{
+                "coding": [{
+                    "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "http://terminology.hl7.org/CodeSystem/v3-ParticipationType",
+                    "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "ATND",
+                    "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "attender"
+                  }]}],
+            "individual": {
+              "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Practitioner/1000003560",
+              "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Starter Provider"
+            }}],</t>
+    </r>
+  </si>
+  <si>
+    <t>Tentatively given the system as 
+"http://terminology.hl7.org/CodeSystem/v3-ParticipationType"</t>
+  </si>
+  <si>
+    <t>participant -&gt; type -&gt; coding -&gt; code</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.encounterParticipant.typeCode</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; typeCode</t>
+  </si>
+  <si>
+    <t>participant -&gt; type -&gt; coding -&gt; display</t>
+  </si>
+  <si>
+    <t>Description for Document.componentOf.encompassingEncounter.encounterParticipant.typeCode</t>
+  </si>
+  <si>
+    <t>participant -&gt; individual -&gt; reference</t>
+  </si>
+  <si>
+    <t>"Practitioner/&lt;Document.componentOf.encompassingEncounter.encounterParticipant.assignedEntity.id.extension&gt;"</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; assignedEntity -&gt; id -&gt; extension</t>
+  </si>
+  <si>
+    <t>participant -&gt; individual -&gt; display</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.encounterParticipant.assignedEntity.assignedPerson.name.given 
+and
+Document.componentOf.encompassingEncounter.encounterParticipant.assignedEntity.assignedPerson.name.family</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; assignedEntity -&gt; assignedPerson -&gt; name -&gt; given and family</t>
+  </si>
+  <si>
     <t>location -&gt; location -&gt; reference</t>
   </si>
   <si>
-    <t>"location" : [{
-        "location" : {
-          "reference" : "Location/LocationExample-SCN"
-        }
-      }]</t>
-  </si>
-  <si>
-    <t>Path to ge the location details.</t>
+    <t>Document.componentOf.encompassingEncounter.location.healthCareFacility.id.extension</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"location": [{
+            "location": {
+              "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Location/1",
+              "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Initial Department"
+            }}],</t>
+    </r>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; location -&gt; healthCareFacility -&gt; id -&gt; extension</t>
+  </si>
+  <si>
+    <t>location -&gt; location -&gt; display</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.location.healthCareFacility.location.name</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; location -&gt; healthCareFacility -&gt; location -&gt; name</t>
+  </si>
+  <si>
+    <t>serviceProvider -&gt; reference</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.location.healthCareFacility.serviceProviderOrganization.id.extension</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"serviceProvider": {
+          "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Organization/1",
+          "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Facility"
+        }</t>
+    </r>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; location -&gt; healthCareFacility -&gt; serviceProviderOrganization -&gt; id -&gt; extension</t>
+  </si>
+  <si>
+    <t>serviceProvider -&gt; display</t>
+  </si>
+  <si>
+    <t>Document.componentOf.encompassingEncounter.location.healthCareFacility.serviceProviderOrganization.name</t>
+  </si>
+  <si>
+    <t>Tentatively mapped the encounterParticipant -&gt; location -&gt; healthCareFacility -&gt; serviceProviderOrganization -&gt; name</t>
   </si>
   <si>
     <t>"request" : {
@@ -2411,9 +2938,6 @@
   </si>
   <si>
     <t>Path to get 'active'</t>
-  </si>
-  <si>
-    <t>identifier -&gt; value</t>
   </si>
   <si>
     <t>Document.author.assignedAuthor.representedOrganization.id.extension</t>
@@ -2482,9 +3006,6 @@
   </si>
   <si>
     <t>Path to get Identifier code and value</t>
-  </si>
-  <si>
-    <t>identifier -&gt; system</t>
   </si>
   <si>
     <t>"http://www.scn.ny.gov/"</t>
@@ -2896,6 +3417,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"item" : [
               {
                 "</t>
@@ -3111,6 +3639,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"</t>
     </r>
     <r>
@@ -3140,6 +3675,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"subject": {
             "</t>
     </r>
@@ -3168,6 +3710,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"encounter" : {
         "</t>
     </r>
@@ -3196,6 +3745,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"item" : [
           {
             "</t>
@@ -4057,7 +4613,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4084,9 +4640,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4623,7 +5176,7 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -4802,7 +5355,7 @@
       <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -4813,7 +5366,7 @@
       <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -4895,7 +5448,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>380</v>
+        <v>427</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -4909,7 +5462,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>381</v>
+        <v>428</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -4933,7 +5486,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>382</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -4945,10 +5498,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -5076,60 +5629,60 @@
         <v>65</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" ht="60" spans="2:4">
-      <c r="B12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" ht="30" spans="2:4">
+    <row r="13" ht="60" spans="2:4">
       <c r="B13" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" ht="60" spans="2:5">
+    <row r="14" ht="30" spans="2:4">
       <c r="B14" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15" ht="60" spans="2:5">
+      <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" ht="120" spans="2:4">
+    <row r="16" spans="2:4">
       <c r="B16" s="3" t="s">
         <v>80</v>
       </c>
@@ -5140,207 +5693,207 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" ht="120" spans="2:4">
       <c r="B17" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" ht="90" spans="2:5">
+    <row r="24" spans="2:4">
       <c r="B24" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" ht="90" spans="2:5">
+      <c r="B25" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" ht="30" spans="2:4">
+    <row r="26" spans="2:4">
       <c r="B26" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="2:4">
+      <c r="D26" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" ht="30" spans="2:4">
       <c r="B27" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" ht="30" spans="2:4">
+    <row r="28" spans="2:4">
       <c r="B28" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" ht="30" spans="2:4">
       <c r="B29" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" ht="30" spans="2:4">
+        <v>114</v>
+      </c>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="2:4">
       <c r="B31" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="2:4">
+        <v>105</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" ht="30" spans="2:4">
       <c r="B32" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" ht="30" spans="2:4">
+    <row r="33" spans="2:4">
       <c r="B33" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" ht="30" spans="2:4">
       <c r="B34" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" ht="30" spans="2:4">
+        <v>119</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" ht="120" spans="2:5">
+        <v>120</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" ht="30" spans="2:4">
       <c r="B37" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="C37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" ht="120" spans="2:5">
       <c r="B38" s="3" t="s">
@@ -5353,61 +5906,60 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" ht="120" spans="2:5">
       <c r="B39" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="5"/>
+      <c r="E39" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" ht="195" spans="2:5">
+    <row r="43" spans="2:4">
       <c r="B43" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" ht="195" spans="2:5">
       <c r="B44" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
         <v>138</v>
       </c>
@@ -5416,162 +5968,163 @@
       </c>
     </row>
     <row r="45" ht="195" spans="2:5">
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E45" s="3" t="s">
+    </row>
+    <row r="46" ht="195" spans="2:5">
+      <c r="B46" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="46" customFormat="1" spans="2:5">
-      <c r="B46" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="3"/>
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" ht="150" spans="2:5">
-      <c r="B50" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="5" t="s">
+    <row r="50" customFormat="1" spans="2:5">
+      <c r="B50" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="3" t="s">
+      <c r="D50" s="5"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" ht="150" spans="2:5">
+      <c r="B51" s="5" t="s">
         <v>152</v>
       </c>
       <c r="C51" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D51" s="5"/>
-    </row>
-    <row r="52" customFormat="1" spans="2:5">
+      <c r="E51" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
       <c r="B52" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>127</v>
+        <v>155</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="3"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="3"/>
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="3"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C56" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>161</v>
       </c>
       <c r="D56" s="5"/>
-    </row>
-    <row r="57" ht="180" spans="2:5">
-      <c r="B57" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="C57" s="5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="58" ht="75" spans="2:4">
-      <c r="B58" s="3" t="s">
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" ht="180" spans="2:5">
+      <c r="B58" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="59" ht="255" spans="2:5">
+      <c r="E58" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" ht="75" spans="2:4">
       <c r="B59" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="60" ht="135" spans="2:5">
+    <row r="60" ht="255" spans="2:5">
       <c r="B60" s="3" t="s">
         <v>170</v>
       </c>
@@ -5582,48 +6135,59 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" ht="30" spans="2:3">
+    <row r="61" ht="135" spans="2:5">
       <c r="B61" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>54</v>
+      <c r="D61" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="62" ht="30" spans="2:3">
       <c r="B62" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" ht="30" spans="2:3">
       <c r="B63" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D63" s="6" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="64" ht="43" customHeight="1" spans="2:4">
+    <row r="64" spans="2:4">
       <c r="B64" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D64" s="6"/>
+      <c r="D64" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" ht="43" customHeight="1" spans="2:4">
+      <c r="B65" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D65" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D64:D65"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -5679,7 +6243,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -5707,183 +6271,183 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:3">
       <c r="B9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" ht="105" spans="2:5">
       <c r="B11" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="1" ht="43" customHeight="1" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="3"/>
@@ -5948,7 +6512,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5960,7 +6524,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -5982,7 +6546,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -5996,168 +6560,168 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D8" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:4">
       <c r="B19" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C19" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:4">
       <c r="B20" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D21" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" ht="46" customHeight="1" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D23" s="6"/>
     </row>
@@ -6173,19 +6737,19 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D12"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="30.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="42.2857142857143" style="3" customWidth="1"/>
     <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="47.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="53" customWidth="1"/>
     <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6219,7 +6783,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6231,7 +6795,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6253,136 +6817,308 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" ht="105" spans="2:5">
-      <c r="B8" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="5" t="s">
+    <row r="7" customFormat="1" ht="90" spans="2:6">
+      <c r="B7" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="9" ht="120" spans="2:4">
+      <c r="D7" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E7" t="s">
+        <v>270</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="1" ht="30" spans="2:6">
+      <c r="B8" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>269</v>
+        <v>186</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="10" ht="30" spans="2:3">
+        <v>274</v>
+      </c>
+      <c r="D9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" ht="105" spans="2:5">
       <c r="B10" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
+        <v>278</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" ht="60" spans="2:4">
+        <v>282</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" customFormat="1" ht="30" spans="2:3">
+        <v>284</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" ht="120" spans="2:5">
       <c r="B13" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E13" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="2:5">
+      <c r="B14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="2:5">
+      <c r="B15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" ht="30" spans="2:5">
+      <c r="B16" t="s">
+        <v>297</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" ht="60" spans="2:4">
+      <c r="B17" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="14" ht="60" spans="2:4">
-      <c r="B14" t="s">
-        <v>277</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="15" ht="30" spans="2:3">
-      <c r="B15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="16" ht="75" spans="2:5">
-      <c r="B16" t="s">
-        <v>282</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E16" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="17" customFormat="1" spans="2:4">
-      <c r="B17" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
-      <c r="B18" s="3" t="s">
+      <c r="C17" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" ht="30" spans="2:3">
+      <c r="B18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" ht="60" spans="2:4">
+      <c r="B19" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" ht="30" spans="2:3">
+      <c r="B20" t="s">
+        <v>303</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" ht="45" spans="2:5">
+      <c r="B21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" ht="30" spans="2:5">
+      <c r="B22" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E22" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" ht="45" spans="2:3">
+      <c r="B23" t="s">
+        <v>312</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" ht="45" spans="2:5">
+      <c r="B24" t="s">
+        <v>314</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" ht="105" spans="2:5">
+      <c r="B25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" ht="75" spans="2:5">
+      <c r="B26" t="s">
+        <v>320</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" ht="30" spans="2:5">
+      <c r="B27" t="s">
+        <v>324</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" ht="60" spans="2:5">
+      <c r="B28" t="s">
+        <v>327</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="29" customFormat="1" ht="45" spans="2:5">
+      <c r="B29" t="s">
+        <v>331</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="30" customFormat="1" spans="2:4">
+      <c r="B30" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D18" s="6"/>
+      <c r="C30" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
+      <c r="B31" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D31" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D17:D18"/>
+  <mergeCells count="2">
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -6438,7 +7174,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>287</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -6468,7 +7204,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>288</v>
+        <v>337</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6476,136 +7212,136 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>290</v>
+        <v>339</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>291</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" ht="135" spans="2:5">
       <c r="B8" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>293</v>
+        <v>341</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>295</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>297</v>
+        <v>344</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>298</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="3" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
-        <v>301</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>302</v>
+        <v>349</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>303</v>
+        <v>350</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" ht="105" spans="2:5">
       <c r="B12" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>305</v>
+        <v>352</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>306</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="2:6">
       <c r="B13" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
-        <v>307</v>
+        <v>354</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" customFormat="1" ht="180" spans="2:6">
       <c r="B14" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>309</v>
+        <v>356</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>310</v>
+        <v>357</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" customFormat="1" ht="90" spans="2:6">
       <c r="B15" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>311</v>
+        <v>358</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" customFormat="1" ht="120" spans="2:6">
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>312</v>
+        <v>359</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>313</v>
+        <v>360</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:6">
       <c r="B17" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>314</v>
+        <v>361</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
@@ -6613,10 +7349,10 @@
     </row>
     <row r="18" customFormat="1" ht="30" spans="2:6">
       <c r="B18" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>315</v>
+        <v>362</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
@@ -6624,10 +7360,10 @@
     </row>
     <row r="19" customFormat="1" ht="30" spans="2:6">
       <c r="B19" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>316</v>
+        <v>363</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
@@ -6635,10 +7371,10 @@
     </row>
     <row r="20" customFormat="1" ht="30" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>317</v>
+        <v>364</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
@@ -6646,10 +7382,10 @@
     </row>
     <row r="21" customFormat="1" ht="30" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>318</v>
+        <v>365</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
@@ -6657,21 +7393,21 @@
     </row>
     <row r="22" customFormat="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>319</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>320</v>
+        <v>367</v>
       </c>
       <c r="D23" s="6"/>
     </row>
@@ -6725,7 +7461,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>321</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6734,7 +7470,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6746,7 +7482,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -6768,7 +7504,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>323</v>
+        <v>370</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6782,157 +7518,157 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D8" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>324</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D19" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>325</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D22" s="6"/>
     </row>
@@ -6995,7 +7731,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>326</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7007,7 +7743,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7029,7 +7765,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7037,10 +7773,10 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>328</v>
+        <v>375</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>34</v>
@@ -7048,10 +7784,10 @@
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>329</v>
+        <v>376</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -7059,123 +7795,123 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>330</v>
+        <v>377</v>
       </c>
       <c r="D9" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>332</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>333</v>
+        <v>380</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>334</v>
+        <v>381</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>335</v>
+        <v>382</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>337</v>
+        <v>384</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>338</v>
+        <v>385</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>339</v>
+        <v>386</v>
       </c>
       <c r="E11" t="s">
-        <v>340</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>341</v>
+        <v>388</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>342</v>
+        <v>389</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>343</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>344</v>
+        <v>391</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>338</v>
+        <v>385</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>345</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>346</v>
+        <v>393</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>347</v>
+        <v>394</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>348</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>349</v>
+        <v>396</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>350</v>
+        <v>397</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>351</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>352</v>
+        <v>399</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>353</v>
+        <v>400</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>354</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>325</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -7230,7 +7966,7 @@
     </row>
     <row r="2" ht="30" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>355</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7239,7 +7975,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>356</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7251,7 +7987,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7273,7 +8009,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>357</v>
+        <v>404</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7281,76 +8017,76 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>358</v>
+        <v>405</v>
       </c>
       <c r="D7" t="s">
-        <v>359</v>
+        <v>406</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>360</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" ht="45" spans="2:5">
       <c r="B8" t="s">
-        <v>361</v>
+        <v>408</v>
       </c>
       <c r="C8" t="s">
-        <v>362</v>
+        <v>409</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>363</v>
+        <v>410</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>364</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" ht="45" spans="2:5">
       <c r="B9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>365</v>
+        <v>412</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" ht="45" spans="2:5">
       <c r="B10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>366</v>
+        <v>413</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>337</v>
+        <v>384</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>367</v>
+        <v>414</v>
       </c>
       <c r="E11" t="s">
-        <v>340</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>368</v>
+        <v>415</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>369</v>
+        <v>416</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
@@ -7359,10 +8095,10 @@
     </row>
     <row r="13" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>370</v>
+        <v>417</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
@@ -7371,10 +8107,10 @@
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>371</v>
+        <v>418</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
@@ -7383,10 +8119,10 @@
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" t="s">
-        <v>349</v>
+        <v>396</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
@@ -7395,10 +8131,10 @@
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>372</v>
+        <v>419</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>338</v>
+        <v>385</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
@@ -7407,10 +8143,10 @@
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>373</v>
+        <v>420</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>374</v>
+        <v>421</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" t="s">
@@ -7419,10 +8155,10 @@
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>375</v>
+        <v>422</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>376</v>
+        <v>423</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
@@ -7431,10 +8167,10 @@
     </row>
     <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>377</v>
+        <v>424</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>350</v>
+        <v>397</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" t="s">
@@ -7443,10 +8179,10 @@
     </row>
     <row r="20" customFormat="1" ht="45" spans="2:5">
       <c r="B20" t="s">
-        <v>378</v>
+        <v>425</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>379</v>
+        <v>426</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" t="s">
@@ -7455,21 +8191,21 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>325</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D22" s="6"/>
     </row>

</xml_diff>

<commit_message>
docs: update xslt file to convert ccda codes to corresponding fhir codes #1208
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="437">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -479,12 +479,6 @@
   </si>
   <si>
     <t>"gender" : "male",</t>
-  </si>
-  <si>
-    <t>When code = 'M' then 'male'
-When code = 'F' then 'female'
-Otherwise code.
-Tentatively mapped.</t>
   </si>
   <si>
     <t>birthDate</t>
@@ -568,12 +562,6 @@
         "value" : "555-120-6047",
         "use" : "home"
       }],</t>
-  </si>
-  <si>
-    <t>When use = 'HP' then 'home'
-When use = 'WP' then 'work'
-Otherwise use.
-What are the possible values of telecom -&gt; use? Is it HP, WP etc? or it should be converted to 'home', 'work' etc.?</t>
   </si>
   <si>
     <t>extension -&gt; extension -&gt; url</t>
@@ -1469,7 +1457,7 @@
     <t>Document.authorization.consent.statusCode.code</t>
   </si>
   <si>
-    <t>"status": "completed"</t>
+    <t>"status": "active"</t>
   </si>
   <si>
     <t>scope -&gt; coding -&gt; code</t>
@@ -2965,6 +2953,50 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
+      <t>system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "urn:oid:1.2.840.114350.1.13.570.2.7.2.696570",
+            "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "SCNExample",
+            "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>display</t>
     </r>
     <r>
@@ -2978,8 +3010,29 @@
       <t>" : "Care Ridge"
           }]
         },
-        "system" : "http://www.scn.ny.gov/",
-        "value" : "</t>
+        "system" : "http://www.hl7.org/oid/",
+        "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "</t>
     </r>
     <r>
       <rPr>
@@ -3005,22 +3058,38 @@
     </r>
   </si>
   <si>
-    <t>Path to get Identifier code and value</t>
-  </si>
-  <si>
-    <t>"http://www.scn.ny.gov/"</t>
+    <t xml:space="preserve">Tentatively mapped the identifier -&gt; value.
+</t>
+  </si>
+  <si>
+    <t>"http://www.hl7.org/oid/"</t>
   </si>
   <si>
     <t>Provide the identifier system.</t>
   </si>
   <si>
+    <t>identifier -&gt; type -&gt; coding -&gt; code</t>
+  </si>
+  <si>
+    <t>Path to get Identifier type -&gt; coding -&gt; code</t>
+  </si>
+  <si>
+    <t>identifier -&gt; type -&gt; coding -&gt; system</t>
+  </si>
+  <si>
+    <t>Document.author.assignedAuthor.representedOrganization.id.root</t>
+  </si>
+  <si>
+    <t>Tentatively mapped Identifier type -&gt; coding -&gt; system</t>
+  </si>
+  <si>
     <t>identifier -&gt; type -&gt; coding -&gt; display</t>
   </si>
   <si>
     <t>Document.author.assignedAuthor.representedOrganization.name</t>
   </si>
   <si>
-    <t>Tentatively mapped the identifier type display.</t>
+    <t>Tentatively mapped the identifier -&gt; type -&gt; coding -&gt; display.</t>
   </si>
   <si>
     <t>name</t>
@@ -3091,28 +3160,7 @@
         <scheme val="minor"/>
       </rPr>
       <t>"telecom" : [{
-      "system" : "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>phone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",
+      "system" : "phone",
       "</t>
     </r>
     <r>
@@ -3244,6 +3292,7 @@
   </si>
   <si>
     <t>"address" : [{
+       "use": "home",
         "text" : "111 Care Ridge St, Plainview, NY 11803",
         "line" : ["111 Care Ridge St"],
         "city" : "Plainview",
@@ -3253,6 +3302,12 @@
       }]</t>
   </si>
   <si>
+    <t>address -&gt; use</t>
+  </si>
+  <si>
+    <t>Document.author.assignedAuthor.representedOrganization.addr.use</t>
+  </si>
+  <si>
     <t>Document.author.assignedAuthor.representedOrganization.addr.streetAddressLine</t>
   </si>
   <si>
@@ -3284,6 +3339,104 @@
   </si>
   <si>
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/shinny-observation-sexual-orientation"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"category" : [{
+        "coding" : [{
+          "system" : "http://hl7.org/fhir/us/sdoh-clinicalcare/CodeSystem/SDOHCC-CodeSystemTemporaryCodes",
+          "code" : "housing-instability",
+          "display" : "Housing Instability"
+        }]
+      },
+      {
+        "coding" : [{
+          "system" : "http://terminology.hl7.org/CodeSystem/observation-category",
+         "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>social-history</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",
+          "display": "Social History"
+        }]
+      },
+      {
+        "coding" : [{
+          "system" : "http://terminology.hl7.org/CodeSystem/observation-category",
+          "code" : "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>survey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+        }]
+      }],</t>
+    </r>
+  </si>
+  <si>
+    <t>Tentatively mapped the path for 'code' ("social-history").
+Is it needed the  "housing-instability" and "survey" codes in every Observations?</t>
   </si>
   <si>
     <r>
@@ -5176,8 +5329,8 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -5448,7 +5601,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5462,7 +5615,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -5486,7 +5639,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -5500,8 +5653,8 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -5668,7 +5821,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" ht="60" spans="2:5">
+    <row r="15" ht="30" spans="2:4">
       <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
@@ -5678,217 +5831,211 @@
       <c r="D15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" ht="120" spans="2:4">
       <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" ht="75" spans="2:4">
+      <c r="B25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" ht="90" spans="2:5">
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" ht="30" spans="2:4">
       <c r="B27" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D28" s="6"/>
     </row>
     <row r="29" ht="30" spans="2:4">
       <c r="B29" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" ht="30" spans="2:4">
       <c r="B32" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" ht="30" spans="2:4">
       <c r="B34" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" ht="30" spans="2:4">
       <c r="B37" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>77</v>
@@ -5897,97 +6044,97 @@
     </row>
     <row r="38" ht="120" spans="2:5">
       <c r="B38" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="39" ht="120" spans="2:5">
       <c r="B39" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" ht="195" spans="2:5">
       <c r="B44" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="E44" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="45" ht="195" spans="2:5">
       <c r="B45" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" ht="195" spans="2:5">
       <c r="B46" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>34</v>
@@ -5995,160 +6142,160 @@
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
       <c r="B50" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="3"/>
     </row>
     <row r="51" ht="150" spans="2:5">
       <c r="B51" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D52" s="5"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="3"/>
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="3"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="3"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D57" s="5"/>
     </row>
     <row r="58" ht="180" spans="2:5">
       <c r="B58" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="59" ht="75" spans="2:4">
       <c r="B59" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" ht="255" spans="2:5">
       <c r="B60" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="61" ht="135" spans="2:5">
       <c r="B61" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="62" ht="30" spans="2:3">
       <c r="B62" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>54</v>
@@ -6156,29 +6303,29 @@
     </row>
     <row r="63" ht="30" spans="2:3">
       <c r="B63" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="65" ht="43" customHeight="1" spans="2:4">
       <c r="B65" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D65" s="6"/>
     </row>
@@ -6200,7 +6347,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6243,7 +6390,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -6271,183 +6418,183 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="s">
         <v>186</v>
-      </c>
-      <c r="C7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:3">
       <c r="B9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" t="s">
         <v>195</v>
-      </c>
-      <c r="C10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E10" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="11" ht="105" spans="2:5">
       <c r="B11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" t="s">
         <v>205</v>
       </c>
-      <c r="C14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" t="s">
-        <v>207</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" t="s">
-        <v>209</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
+        <v>209</v>
+      </c>
+      <c r="C16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="C16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="C17" t="s">
-        <v>215</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>219</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="1" ht="43" customHeight="1" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="3"/>
@@ -6467,8 +6614,8 @@
   <sheetPr/>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6512,7 +6659,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6524,7 +6671,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6546,7 +6693,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6560,168 +6707,168 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:4">
       <c r="B19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="C19" t="s">
-        <v>254</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:4">
       <c r="B20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" t="s">
         <v>256</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D20" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" t="s">
+        <v>258</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="D21" t="s">
-        <v>260</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" ht="46" customHeight="1" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D23" s="6"/>
     </row>
@@ -6739,8 +6886,8 @@
   <sheetPr/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6783,7 +6930,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6795,7 +6942,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6817,7 +6964,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6825,293 +6972,293 @@
     </row>
     <row r="7" customFormat="1" ht="90" spans="2:6">
       <c r="B7" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E7" t="s">
         <v>268</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" t="s">
-        <v>270</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="1" ht="30" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="D9" t="s">
-        <v>275</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="10" ht="105" spans="2:5">
       <c r="B10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" t="s">
         <v>278</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E10" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" ht="120" spans="2:5">
       <c r="B13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" t="s">
         <v>288</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E13" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" t="s">
         <v>291</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="E14" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:5">
       <c r="B15" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E15" t="s">
         <v>294</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E15" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" t="s">
+        <v>295</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" t="s">
         <v>297</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E16" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="17" customFormat="1" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:4">
       <c r="B19" t="s">
+        <v>298</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:3">
       <c r="B20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:5">
       <c r="B21" t="s">
+        <v>303</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E22" t="s">
         <v>309</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="E22" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="23" ht="45" spans="2:3">
       <c r="B23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" ht="45" spans="2:5">
       <c r="B24" t="s">
+        <v>312</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="25" ht="105" spans="2:5">
       <c r="B25" t="s">
+        <v>315</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="26" ht="75" spans="2:5">
       <c r="B26" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="60" spans="2:5">
       <c r="B28" t="s">
+        <v>325</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="45" spans="2:5">
       <c r="B29" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D31" s="6"/>
     </row>
@@ -7128,10 +7275,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7174,7 +7321,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -7204,7 +7351,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7212,158 +7359,158 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D7" t="s">
+        <v>337</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" ht="165" spans="2:5">
+      <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="8" ht="135" spans="2:5">
-      <c r="B8" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
-      <c r="B11" t="s">
-        <v>349</v>
+      <c r="B11" s="3" t="s">
+        <v>346</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="2:5">
+      <c r="B12" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" ht="105" spans="2:5">
-      <c r="B12" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="D12" s="5" t="s">
+    </row>
+    <row r="13" ht="30" spans="2:5">
+      <c r="B13" t="s">
         <v>352</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="C13" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="13" customFormat="1" spans="2:6">
-      <c r="B13" s="3" t="s">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" ht="105" spans="2:5">
+      <c r="B14" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="2:6">
+      <c r="B15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="1" ht="180" spans="2:6">
+      <c r="B16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" customFormat="1" ht="180" spans="2:6">
-      <c r="B14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" customFormat="1" ht="90" spans="2:6">
-      <c r="B15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" customFormat="1" ht="120" spans="2:6">
-      <c r="B16" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:6">
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" customFormat="1" ht="30" spans="2:6">
+    <row r="18" customFormat="1" ht="135" spans="2:6">
       <c r="B18" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>363</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" customFormat="1" ht="30" spans="2:6">
       <c r="B19" s="3" t="s">
-        <v>90</v>
+        <v>364</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
@@ -7371,10 +7518,10 @@
     </row>
     <row r="20" customFormat="1" ht="30" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
@@ -7382,38 +7529,71 @@
     </row>
     <row r="21" customFormat="1" ht="30" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" customFormat="1" spans="2:4">
+    <row r="22" customFormat="1" ht="30" spans="2:6">
       <c r="B22" s="3" t="s">
-        <v>179</v>
+        <v>89</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" customFormat="1" ht="30" spans="2:6">
+      <c r="B23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" customFormat="1" ht="30" spans="2:6">
+      <c r="B24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" customFormat="1" spans="2:4">
+      <c r="B25" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" ht="46" customHeight="1" spans="2:4">
+      <c r="B26" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="23" customFormat="1" ht="46" customHeight="1" spans="2:4">
-      <c r="B23" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="D23" s="6"/>
+      <c r="C26" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -7425,8 +7605,8 @@
   <sheetPr/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7461,7 +7641,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7470,7 +7650,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7482,7 +7662,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7504,7 +7684,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7518,157 +7698,157 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" ht="390" spans="2:5">
+      <c r="B9" t="s">
         <v>229</v>
       </c>
-      <c r="D8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" ht="375" spans="2:5">
-      <c r="B9" t="s">
-        <v>231</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>232</v>
+        <v>376</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>233</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" t="s">
         <v>256</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D19" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" t="s">
+        <v>258</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="D20" t="s">
-        <v>260</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D22" s="6"/>
     </row>
@@ -7731,7 +7911,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7743,7 +7923,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7765,7 +7945,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7773,10 +7953,10 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>34</v>
@@ -7784,10 +7964,10 @@
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -7795,123 +7975,123 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D9" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="E11" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -7931,7 +8111,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7966,7 +8146,7 @@
     </row>
     <row r="2" ht="30" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7975,7 +8155,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7987,7 +8167,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -8009,7 +8189,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8017,76 +8197,76 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="D7" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" ht="45" spans="2:5">
       <c r="B8" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="C8" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" ht="45" spans="2:5">
       <c r="B9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" ht="45" spans="2:5">
       <c r="B10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="E11" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
@@ -8095,10 +8275,10 @@
     </row>
     <row r="13" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
@@ -8107,10 +8287,10 @@
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
@@ -8119,10 +8299,10 @@
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
@@ -8131,10 +8311,10 @@
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
@@ -8143,10 +8323,10 @@
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" t="s">
@@ -8155,10 +8335,10 @@
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
@@ -8167,10 +8347,10 @@
     </row>
     <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" t="s">
@@ -8179,10 +8359,10 @@
     </row>
     <row r="20" customFormat="1" ht="45" spans="2:5">
       <c r="B20" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" t="s">
@@ -8191,21 +8371,21 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D22" s="6"/>
     </row>

</xml_diff>

<commit_message>
docs: update xslt files to handle the consent resource for the epic ccda files #1233
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="439">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -1457,7 +1457,13 @@
     <t>Document.authorization.consent.statusCode.code</t>
   </si>
   <si>
-    <t>"status": "active"</t>
+    <t>"status": "permit"</t>
+  </si>
+  <si>
+    <t>If the statusCode-&gt;code is other than 'deny' then 'permit' otherwise 'deny'. Only two status are given 'deny' or 'permit'.</t>
+  </si>
+  <si>
+    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with ststusCode -&gt; code as 'deny'.</t>
   </si>
   <si>
     <t>scope -&gt; coding -&gt; code</t>
@@ -4766,7 +4772,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4789,6 +4795,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5329,7 +5338,7 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -5601,7 +5610,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5615,7 +5624,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -5639,7 +5648,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -5935,7 +5944,7 @@
       <c r="C26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -6346,8 +6355,8 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6421,7 +6430,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" ht="45" spans="2:6">
       <c r="B7" t="s">
         <v>184</v>
       </c>
@@ -6431,149 +6440,155 @@
       <c r="D7" t="s">
         <v>186</v>
       </c>
+      <c r="E7" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:3">
       <c r="B9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" ht="105" spans="2:5">
       <c r="B11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -6584,7 +6599,7 @@
         <v>178</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6594,7 +6609,7 @@
         <v>180</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="3"/>
@@ -6659,7 +6674,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6671,7 +6686,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6693,7 +6708,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6707,7 +6722,7 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
@@ -6715,10 +6730,10 @@
         <v>184</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>137</v>
@@ -6726,130 +6741,130 @@
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:4">
       <c r="B19" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:4">
       <c r="B20" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D21" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -6860,7 +6875,7 @@
         <v>178</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" ht="46" customHeight="1" spans="2:4">
@@ -6868,7 +6883,7 @@
         <v>180</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D23" s="6"/>
     </row>
@@ -6930,7 +6945,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6942,7 +6957,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6964,7 +6979,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6972,29 +6987,29 @@
     </row>
     <row r="7" customFormat="1" ht="90" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E7" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="1" ht="30" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -7003,243 +7018,243 @@
         <v>184</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" ht="105" spans="2:5">
       <c r="B10" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E10" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" ht="120" spans="2:5">
       <c r="B13" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E13" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E14" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:5">
       <c r="B15" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E15" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E16" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" customFormat="1" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:4">
       <c r="B19" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:3">
       <c r="B20" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:5">
       <c r="B21" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E22" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" ht="45" spans="2:3">
       <c r="B23" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" ht="45" spans="2:5">
       <c r="B24" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" ht="105" spans="2:5">
       <c r="B25" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" ht="75" spans="2:5">
       <c r="B26" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="60" spans="2:5">
       <c r="B28" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="45" spans="2:5">
       <c r="B29" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:4">
@@ -7250,7 +7265,7 @@
         <v>178</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -7258,7 +7273,7 @@
         <v>180</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D31" s="6"/>
     </row>
@@ -7321,7 +7336,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -7351,7 +7366,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7359,98 +7374,98 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="3" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:5">
       <c r="B13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" ht="105" spans="2:5">
       <c r="B14" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="2:6">
@@ -7462,7 +7477,7 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -7471,13 +7486,13 @@
         <v>97</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -7486,7 +7501,7 @@
         <v>99</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -7497,20 +7512,20 @@
         <v>82</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" customFormat="1" ht="30" spans="2:6">
       <c r="B19" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
@@ -7521,7 +7536,7 @@
         <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
@@ -7532,7 +7547,7 @@
         <v>87</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
@@ -7543,7 +7558,7 @@
         <v>89</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3"/>
@@ -7554,7 +7569,7 @@
         <v>91</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="3"/>
@@ -7565,7 +7580,7 @@
         <v>93</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="3"/>
@@ -7579,7 +7594,7 @@
         <v>178</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -7587,7 +7602,7 @@
         <v>180</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D26" s="6"/>
     </row>
@@ -7641,7 +7656,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7650,7 +7665,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7662,7 +7677,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7684,7 +7699,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7698,7 +7713,7 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
@@ -7706,10 +7721,10 @@
         <v>184</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>137</v>
@@ -7717,119 +7732,119 @@
     </row>
     <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -7840,7 +7855,7 @@
         <v>178</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
@@ -7848,7 +7863,7 @@
         <v>180</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D22" s="6"/>
     </row>
@@ -7911,7 +7926,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7923,7 +7938,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7945,7 +7960,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7953,10 +7968,10 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>34</v>
@@ -7964,10 +7979,10 @@
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -7978,101 +7993,101 @@
         <v>184</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D9" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E11" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -8083,7 +8098,7 @@
         <v>178</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
@@ -8091,7 +8106,7 @@
         <v>180</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -8146,7 +8161,7 @@
     </row>
     <row r="2" ht="30" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8155,7 +8170,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8167,7 +8182,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -8189,7 +8204,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8200,73 +8215,73 @@
         <v>184</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D7" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" ht="45" spans="2:5">
       <c r="B8" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C8" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" ht="45" spans="2:5">
       <c r="B9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" ht="45" spans="2:5">
       <c r="B10" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E11" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
@@ -8275,10 +8290,10 @@
     </row>
     <row r="13" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
@@ -8287,10 +8302,10 @@
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
@@ -8299,10 +8314,10 @@
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
@@ -8311,10 +8326,10 @@
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
@@ -8323,10 +8338,10 @@
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" t="s">
@@ -8335,10 +8350,10 @@
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
@@ -8347,10 +8362,10 @@
     </row>
     <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" t="s">
@@ -8359,10 +8374,10 @@
     </row>
     <row r="20" customFormat="1" ht="45" spans="2:5">
       <c r="B20" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" t="s">
@@ -8377,7 +8392,7 @@
         <v>178</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
@@ -8385,7 +8400,7 @@
         <v>180</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D22" s="6"/>
     </row>

</xml_diff>

<commit_message>
docs: update xslt files to handle the consent state for the epic ccda files #1233
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="8675" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="439">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -1457,13 +1457,10 @@
     <t>Document.authorization.consent.statusCode.code</t>
   </si>
   <si>
-    <t>"status": "permit"</t>
-  </si>
-  <si>
-    <t>If the statusCode-&gt;code is other than 'deny' then 'permit' otherwise 'deny'. Only two status are given 'deny' or 'permit'.</t>
-  </si>
-  <si>
-    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with ststusCode -&gt; code as 'deny'.</t>
+    <t>"status": "active"</t>
+  </si>
+  <si>
+    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with 'ststusCode -&gt; code' as 'completed' and 'act -&gt; code -&gt; code' as 'deny'.</t>
   </si>
   <si>
     <t>scope -&gt; coding -&gt; code</t>
@@ -1677,6 +1674,10 @@
       <t>"
       }</t>
     </r>
+  </si>
+  <si>
+    <t>act -&gt; code -&gt; displayName 
+('deny' or 'permit')</t>
   </si>
   <si>
     <t>patient -&gt; reference</t>
@@ -4772,7 +4773,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4795,9 +4796,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5342,14 +5340,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
     <col min="2" max="2" width="28.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="65.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="73.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="29.447619047619" customWidth="1"/>
-    <col min="6" max="6" width="46.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="73.4259259259259" customWidth="1"/>
+    <col min="5" max="5" width="29.4444444444444" customWidth="1"/>
+    <col min="6" max="6" width="46.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -5398,7 +5396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="75" spans="2:4">
+    <row r="5" ht="57.6" spans="2:4">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -5435,7 +5433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" ht="30" spans="2:3">
+    <row r="9" ht="28.8" spans="2:3">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -5480,7 +5478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" ht="45" spans="2:5">
+    <row r="19" ht="28.8" spans="2:5">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -5491,7 +5489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" ht="45" spans="2:5">
+    <row r="20" ht="28.8" spans="2:5">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -5502,7 +5500,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" ht="45" spans="2:5">
+    <row r="21" ht="28.8" spans="2:5">
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -5513,7 +5511,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" ht="75" spans="2:5">
+    <row r="22" ht="43.2" spans="2:5">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -5524,7 +5522,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" ht="75" spans="2:5">
+    <row r="23" ht="43.2" spans="2:5">
       <c r="B23" t="s">
         <v>43</v>
       </c>
@@ -5535,7 +5533,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" ht="30" spans="2:5">
+    <row r="24" ht="28.8" spans="2:5">
       <c r="B24" t="s">
         <v>45</v>
       </c>
@@ -5543,7 +5541,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" ht="30" spans="2:5">
+    <row r="25" ht="28.8" spans="2:5">
       <c r="B25" t="s">
         <v>47</v>
       </c>
@@ -5569,14 +5567,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="36.2190476190476" customWidth="1"/>
-    <col min="4" max="4" width="54.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="36.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="54.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="34.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="34.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -5629,7 +5627,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" customFormat="1" ht="30" spans="1:6">
+    <row r="5" customFormat="1" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -5666,14 +5664,14 @@
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="41.7809523809524" style="3" customWidth="1"/>
-    <col min="3" max="3" width="63.8857142857143" style="3" customWidth="1"/>
-    <col min="4" max="4" width="81.2857142857143" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.7142857142857" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="41.7777777777778" style="3" customWidth="1"/>
+    <col min="3" max="3" width="63.8888888888889" style="3" customWidth="1"/>
+    <col min="4" max="4" width="81.287037037037" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.712962962963" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -5721,7 +5719,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:5">
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -5741,7 +5739,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" ht="30" spans="2:4">
+    <row r="7" ht="28.8" spans="2:4">
       <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
@@ -5752,7 +5750,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" ht="60" spans="2:5">
+    <row r="8" ht="57.6" spans="2:5">
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
@@ -5808,7 +5806,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" ht="60" spans="2:4">
+    <row r="13" ht="57.6" spans="2:4">
       <c r="B13" s="3" t="s">
         <v>70</v>
       </c>
@@ -5819,7 +5817,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" ht="30" spans="2:4">
+    <row r="14" ht="28.8" spans="2:4">
       <c r="B14" s="3" t="s">
         <v>73</v>
       </c>
@@ -5830,7 +5828,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" ht="30" spans="2:4">
+    <row r="15" spans="2:4">
       <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
@@ -5852,7 +5850,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" ht="120" spans="2:4">
+    <row r="17" ht="115.2" spans="2:4">
       <c r="B17" s="3" t="s">
         <v>82</v>
       </c>
@@ -5926,7 +5924,7 @@
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" ht="75" spans="2:4">
+    <row r="25" ht="72" spans="2:4">
       <c r="B25" s="3" t="s">
         <v>99</v>
       </c>
@@ -5944,11 +5942,11 @@
       <c r="C26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" ht="30" spans="2:4">
+    <row r="27" spans="2:4">
       <c r="B27" s="3" t="s">
         <v>105</v>
       </c>
@@ -5966,7 +5964,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" ht="30" spans="2:4">
+    <row r="29" spans="2:4">
       <c r="B29" s="3" t="s">
         <v>109</v>
       </c>
@@ -5995,7 +5993,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" ht="30" spans="2:4">
+    <row r="32" spans="2:4">
       <c r="B32" s="3" t="s">
         <v>105</v>
       </c>
@@ -6013,7 +6011,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" ht="30" spans="2:4">
+    <row r="34" spans="2:4">
       <c r="B34" s="3" t="s">
         <v>109</v>
       </c>
@@ -6042,7 +6040,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" ht="30" spans="2:4">
+    <row r="37" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>120</v>
       </c>
@@ -6051,7 +6049,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" ht="120" spans="2:5">
+    <row r="38" ht="115.2" spans="2:5">
       <c r="B38" s="3" t="s">
         <v>121</v>
       </c>
@@ -6062,7 +6060,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" ht="120" spans="2:5">
+    <row r="39" ht="115.2" spans="2:5">
       <c r="B39" s="3" t="s">
         <v>124</v>
       </c>
@@ -6109,7 +6107,7 @@
       </c>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" ht="195" spans="2:5">
+    <row r="44" ht="187.2" spans="2:5">
       <c r="B44" s="3" t="s">
         <v>134</v>
       </c>
@@ -6123,7 +6121,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" ht="195" spans="2:5">
+    <row r="45" ht="187.2" spans="2:5">
       <c r="B45" s="3" t="s">
         <v>138</v>
       </c>
@@ -6135,7 +6133,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" ht="195" spans="2:5">
+    <row r="46" ht="187.2" spans="2:5">
       <c r="B46" s="5" t="s">
         <v>141</v>
       </c>
@@ -6189,7 +6187,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" ht="150" spans="2:5">
+    <row r="51" ht="144" spans="2:5">
       <c r="B51" s="5" t="s">
         <v>150</v>
       </c>
@@ -6261,7 +6259,7 @@
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" ht="180" spans="2:5">
+    <row r="58" ht="172.8" spans="2:5">
       <c r="B58" s="5" t="s">
         <v>163</v>
       </c>
@@ -6272,7 +6270,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="59" ht="75" spans="2:4">
+    <row r="59" ht="72" spans="2:4">
       <c r="B59" s="3" t="s">
         <v>166</v>
       </c>
@@ -6280,7 +6278,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="60" ht="255" spans="2:5">
+    <row r="60" ht="244.8" spans="2:5">
       <c r="B60" s="3" t="s">
         <v>168</v>
       </c>
@@ -6291,7 +6289,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" ht="135" spans="2:5">
+    <row r="61" ht="129.6" spans="2:5">
       <c r="B61" s="3" t="s">
         <v>171</v>
       </c>
@@ -6302,7 +6300,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" ht="30" spans="2:3">
+    <row r="62" ht="28.8" spans="2:3">
       <c r="B62" s="3" t="s">
         <v>174</v>
       </c>
@@ -6310,7 +6308,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" ht="30" spans="2:3">
+    <row r="63" ht="28.8" spans="2:3">
       <c r="B63" s="3" t="s">
         <v>175</v>
       </c>
@@ -6355,18 +6353,18 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="63.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="68.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="38.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="57.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="27.8611111111111" customWidth="1"/>
+    <col min="3" max="3" width="63.4259259259259" customWidth="1"/>
+    <col min="4" max="4" width="68.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="50" customWidth="1"/>
+    <col min="6" max="6" width="57.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6411,7 +6409,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="30" spans="2:5">
+    <row r="5" ht="28.8" spans="2:5">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -6430,7 +6428,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" ht="45" spans="2:6">
+    <row r="7" ht="43.2" spans="2:5">
       <c r="B7" t="s">
         <v>184</v>
       </c>
@@ -6440,109 +6438,104 @@
       <c r="D7" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F7" s="8" t="s">
+    </row>
+    <row r="8" ht="115.2" spans="2:5">
+      <c r="B8" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="8" ht="120" spans="2:5">
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>189</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:3">
       <c r="B9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" t="s">
         <v>193</v>
-      </c>
-      <c r="C9" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" t="s">
         <v>195</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>196</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" ht="100.8" spans="2:5">
+      <c r="B11" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="11" ht="105" spans="2:5">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>198</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
         <v>201</v>
-      </c>
-      <c r="C12" t="s">
-        <v>202</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" t="s">
         <v>203</v>
       </c>
-      <c r="C13" t="s">
-        <v>204</v>
-      </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" t="s">
         <v>205</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>206</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" ht="43.2" spans="2:5">
+      <c r="B15" t="s">
         <v>207</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" ht="45" spans="2:5">
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>208</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="16" ht="45" spans="2:5">
+    </row>
+    <row r="16" ht="43.2" spans="2:5">
       <c r="B16" t="s">
         <v>211</v>
       </c>
@@ -6554,7 +6547,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="45" spans="2:5">
+    <row r="17" ht="43.2" spans="2:5">
       <c r="B17" t="s">
         <v>214</v>
       </c>
@@ -6566,7 +6559,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="45" spans="2:5">
+    <row r="18" ht="43.2" spans="2:5">
       <c r="B18" t="s">
         <v>217</v>
       </c>
@@ -6577,10 +6570,10 @@
         <v>219</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" ht="60" spans="2:5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" ht="57.6" spans="2:5">
       <c r="B19" t="s">
         <v>220</v>
       </c>
@@ -6633,14 +6626,14 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="33.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.5740740740741" customWidth="1"/>
     <col min="3" max="3" width="49.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="56.552380952381" customWidth="1"/>
-    <col min="5" max="5" width="53.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="47.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="56.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="53.287037037037" customWidth="1"/>
+    <col min="6" max="6" width="47.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6703,7 +6696,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -6725,7 +6718,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="2:5">
+    <row r="8" ht="28.8" spans="2:5">
       <c r="B8" t="s">
         <v>184</v>
       </c>
@@ -6739,7 +6732,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" ht="375" spans="2:5">
+    <row r="9" ht="316.8" spans="2:5">
       <c r="B9" t="s">
         <v>231</v>
       </c>
@@ -6750,7 +6743,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="10" ht="135" spans="2:4">
+    <row r="10" ht="129.6" spans="2:4">
       <c r="B10" t="s">
         <v>234</v>
       </c>
@@ -6761,7 +6754,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="2:3">
+    <row r="11" ht="28.8" spans="2:3">
       <c r="B11" t="s">
         <v>237</v>
       </c>
@@ -6774,13 +6767,13 @@
         <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E12" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="13" ht="30" spans="2:3">
+    <row r="13" ht="28.8" spans="2:3">
       <c r="B13" t="s">
         <v>241</v>
       </c>
@@ -6788,7 +6781,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" ht="105" spans="2:4">
+    <row r="14" ht="100.8" spans="2:4">
       <c r="B14" s="3" t="s">
         <v>243</v>
       </c>
@@ -6799,7 +6792,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" ht="30" spans="2:3">
+    <row r="15" ht="28.8" spans="2:3">
       <c r="B15" s="3" t="s">
         <v>246</v>
       </c>
@@ -6807,15 +6800,15 @@
         <v>247</v>
       </c>
     </row>
-    <row r="16" ht="30" spans="2:3">
+    <row r="16" ht="28.8" spans="2:3">
       <c r="B16" s="3" t="s">
         <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" ht="75" spans="2:4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" ht="57.6" spans="2:4">
       <c r="B17" t="s">
         <v>249</v>
       </c>
@@ -6826,7 +6819,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" ht="30" spans="2:3">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>251</v>
       </c>
@@ -6834,7 +6827,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" ht="45" spans="2:4">
+    <row r="19" ht="43.2" spans="2:4">
       <c r="B19" t="s">
         <v>253</v>
       </c>
@@ -6845,7 +6838,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" ht="30" spans="2:4">
+    <row r="20" ht="28.8" spans="2:4">
       <c r="B20" t="s">
         <v>256</v>
       </c>
@@ -6905,14 +6898,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="42.2857142857143" style="3" customWidth="1"/>
-    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="35.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="42.287037037037" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73.5740740740741" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="51.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6974,7 +6967,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -6985,7 +6978,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" customFormat="1" ht="90" spans="2:6">
+    <row r="7" customFormat="1" ht="86.4" spans="2:6">
       <c r="B7" s="3" t="s">
         <v>267</v>
       </c>
@@ -7000,7 +6993,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" customFormat="1" ht="30" spans="2:6">
+    <row r="8" customFormat="1" ht="28.8" spans="2:6">
       <c r="B8" s="3" t="s">
         <v>271</v>
       </c>
@@ -7027,7 +7020,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" ht="105" spans="2:5">
+    <row r="10" ht="100.8" spans="2:5">
       <c r="B10" t="s">
         <v>277</v>
       </c>
@@ -7041,7 +7034,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="2:5">
+    <row r="11" ht="28.8" spans="2:5">
       <c r="B11" t="s">
         <v>281</v>
       </c>
@@ -7053,7 +7046,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" ht="30" spans="2:5">
+    <row r="12" ht="28.8" spans="2:5">
       <c r="B12" t="s">
         <v>284</v>
       </c>
@@ -7065,7 +7058,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" ht="120" spans="2:5">
+    <row r="13" ht="115.2" spans="2:5">
       <c r="B13" t="s">
         <v>287</v>
       </c>
@@ -7079,7 +7072,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="14" ht="30" spans="2:5">
+    <row r="14" ht="28.8" spans="2:5">
       <c r="B14" t="s">
         <v>291</v>
       </c>
@@ -7090,7 +7083,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" ht="30" spans="2:5">
+    <row r="15" ht="28.8" spans="2:5">
       <c r="B15" t="s">
         <v>294</v>
       </c>
@@ -7101,7 +7094,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="16" customFormat="1" ht="30" spans="2:5">
+    <row r="16" customFormat="1" ht="28.8" spans="2:5">
       <c r="B16" t="s">
         <v>297</v>
       </c>
@@ -7112,7 +7105,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="60" spans="2:4">
+    <row r="17" customFormat="1" ht="57.6" spans="2:4">
       <c r="B17" t="s">
         <v>249</v>
       </c>
@@ -7123,7 +7116,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="30" spans="2:3">
+    <row r="18" customFormat="1" ht="28.8" spans="2:3">
       <c r="B18" t="s">
         <v>251</v>
       </c>
@@ -7131,7 +7124,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" ht="60" spans="2:4">
+    <row r="19" ht="57.6" spans="2:4">
       <c r="B19" t="s">
         <v>300</v>
       </c>
@@ -7142,7 +7135,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" ht="30" spans="2:3">
+    <row r="20" ht="28.8" spans="2:3">
       <c r="B20" t="s">
         <v>303</v>
       </c>
@@ -7150,7 +7143,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" ht="45" spans="2:5">
+    <row r="21" ht="28.8" spans="2:5">
       <c r="B21" t="s">
         <v>305</v>
       </c>
@@ -7164,7 +7157,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="22" ht="30" spans="2:5">
+    <row r="22" ht="28.8" spans="2:5">
       <c r="B22" t="s">
         <v>309</v>
       </c>
@@ -7175,7 +7168,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="23" ht="45" spans="2:3">
+    <row r="23" ht="43.2" spans="2:3">
       <c r="B23" t="s">
         <v>312</v>
       </c>
@@ -7183,7 +7176,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="24" ht="45" spans="2:5">
+    <row r="24" ht="43.2" spans="2:5">
       <c r="B24" t="s">
         <v>314</v>
       </c>
@@ -7194,7 +7187,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" ht="105" spans="2:5">
+    <row r="25" ht="100.8" spans="2:5">
       <c r="B25" t="s">
         <v>317</v>
       </c>
@@ -7205,7 +7198,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="26" ht="75" spans="2:5">
+    <row r="26" ht="72" spans="2:5">
       <c r="B26" t="s">
         <v>320</v>
       </c>
@@ -7219,7 +7212,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="27" customFormat="1" ht="30" spans="2:5">
+    <row r="27" customFormat="1" ht="28.8" spans="2:5">
       <c r="B27" t="s">
         <v>324</v>
       </c>
@@ -7231,7 +7224,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" customFormat="1" ht="60" spans="2:5">
+    <row r="28" customFormat="1" ht="57.6" spans="2:5">
       <c r="B28" t="s">
         <v>327</v>
       </c>
@@ -7245,7 +7238,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" customFormat="1" ht="45" spans="2:5">
+    <row r="29" customFormat="1" ht="43.2" spans="2:5">
       <c r="B29" t="s">
         <v>331</v>
       </c>
@@ -7296,14 +7289,14 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
     <col min="2" max="2" width="27.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="50.8857142857143" customWidth="1"/>
-    <col min="4" max="4" width="72.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="46.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="45.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="50.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="72.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="46.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="45.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7361,7 +7354,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -7383,7 +7376,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" ht="165" spans="2:5">
+    <row r="8" ht="158.4" spans="2:5">
       <c r="B8" t="s">
         <v>271</v>
       </c>
@@ -7409,7 +7402,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" ht="30" spans="2:5">
+    <row r="10" ht="28.8" spans="2:5">
       <c r="B10" s="3" t="s">
         <v>346</v>
       </c>
@@ -7421,7 +7414,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="2:5">
+    <row r="11" ht="28.8" spans="2:5">
       <c r="B11" s="3" t="s">
         <v>348</v>
       </c>
@@ -7433,7 +7426,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="12" ht="30" spans="2:5">
+    <row r="12" ht="28.8" spans="2:5">
       <c r="B12" s="3" t="s">
         <v>351</v>
       </c>
@@ -7445,7 +7438,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" ht="30" spans="2:5">
+    <row r="13" ht="28.8" spans="2:5">
       <c r="B13" t="s">
         <v>354</v>
       </c>
@@ -7457,7 +7450,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="105" spans="2:5">
+    <row r="14" ht="100.8" spans="2:5">
       <c r="B14" t="s">
         <v>356</v>
       </c>
@@ -7481,7 +7474,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" customFormat="1" ht="180" spans="2:6">
+    <row r="16" customFormat="1" ht="172.8" spans="2:6">
       <c r="B16" s="3" t="s">
         <v>97</v>
       </c>
@@ -7496,7 +7489,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" customFormat="1" ht="30" spans="2:6">
+    <row r="17" customFormat="1" ht="28.8" spans="2:6">
       <c r="B17" s="3" t="s">
         <v>99</v>
       </c>
@@ -7507,7 +7500,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" customFormat="1" ht="135" spans="2:6">
+    <row r="18" customFormat="1" ht="129.6" spans="2:6">
       <c r="B18" s="3" t="s">
         <v>82</v>
       </c>
@@ -7520,7 +7513,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" customFormat="1" ht="30" spans="2:6">
+    <row r="19" customFormat="1" ht="28.8" spans="2:6">
       <c r="B19" s="3" t="s">
         <v>366</v>
       </c>
@@ -7531,7 +7524,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" customFormat="1" ht="30" spans="2:6">
+    <row r="20" customFormat="1" ht="28.8" spans="2:6">
       <c r="B20" s="3" t="s">
         <v>85</v>
       </c>
@@ -7542,7 +7535,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" customFormat="1" ht="30" spans="2:6">
+    <row r="21" customFormat="1" ht="28.8" spans="2:6">
       <c r="B21" s="3" t="s">
         <v>87</v>
       </c>
@@ -7553,7 +7546,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" customFormat="1" ht="30" spans="2:6">
+    <row r="22" customFormat="1" ht="28.8" spans="2:6">
       <c r="B22" s="3" t="s">
         <v>89</v>
       </c>
@@ -7564,7 +7557,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" customFormat="1" ht="30" spans="2:6">
+    <row r="23" customFormat="1" ht="28.8" spans="2:6">
       <c r="B23" s="3" t="s">
         <v>91</v>
       </c>
@@ -7575,7 +7568,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" customFormat="1" ht="30" spans="2:6">
+    <row r="24" customFormat="1" ht="28.8" spans="2:6">
       <c r="B24" s="3" t="s">
         <v>93</v>
       </c>
@@ -7624,12 +7617,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="46.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="46.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -7654,7 +7647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="45" spans="1:1">
+    <row r="2" ht="43.2" spans="1:1">
       <c r="A2" s="4" t="s">
         <v>375</v>
       </c>
@@ -7680,7 +7673,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:6">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -7694,7 +7687,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="30" spans="2:6">
+    <row r="6" ht="28.8" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -7716,7 +7709,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="2:5">
+    <row r="8" ht="28.8" spans="2:5">
       <c r="B8" t="s">
         <v>184</v>
       </c>
@@ -7730,7 +7723,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" ht="390" spans="2:5">
+    <row r="9" ht="331.2" spans="2:5">
       <c r="B9" t="s">
         <v>231</v>
       </c>
@@ -7741,7 +7734,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" ht="135" spans="2:4">
+    <row r="10" ht="129.6" spans="2:4">
       <c r="B10" t="s">
         <v>234</v>
       </c>
@@ -7752,7 +7745,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="2:3">
+    <row r="11" ht="28.8" spans="2:3">
       <c r="B11" t="s">
         <v>237</v>
       </c>
@@ -7765,13 +7758,13 @@
         <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E12" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="13" ht="30" spans="2:3">
+    <row r="13" ht="28.8" spans="2:3">
       <c r="B13" t="s">
         <v>241</v>
       </c>
@@ -7779,7 +7772,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" ht="105" spans="2:4">
+    <row r="14" ht="100.8" spans="2:4">
       <c r="B14" s="3" t="s">
         <v>243</v>
       </c>
@@ -7790,7 +7783,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="15" ht="30" spans="2:3">
+    <row r="15" ht="28.8" spans="2:3">
       <c r="B15" s="3" t="s">
         <v>246</v>
       </c>
@@ -7798,15 +7791,15 @@
         <v>247</v>
       </c>
     </row>
-    <row r="16" ht="30" spans="2:3">
+    <row r="16" ht="28.8" spans="2:3">
       <c r="B16" s="3" t="s">
         <v>248</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" ht="75" spans="2:4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" ht="57.6" spans="2:4">
       <c r="B17" t="s">
         <v>249</v>
       </c>
@@ -7817,7 +7810,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" ht="30" spans="2:3">
+    <row r="18" ht="28.8" spans="2:3">
       <c r="B18" t="s">
         <v>251</v>
       </c>
@@ -7825,7 +7818,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" ht="30" spans="2:4">
+    <row r="19" ht="28.8" spans="2:4">
       <c r="B19" t="s">
         <v>256</v>
       </c>
@@ -7885,12 +7878,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="46.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="46.5740740740741" customWidth="1"/>
+    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -7941,7 +7934,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:6">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -7955,7 +7948,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="30" spans="2:6">
+    <row r="6" ht="28.8" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -7966,7 +7959,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" ht="30" spans="2:5">
+    <row r="7" ht="28.8" spans="2:5">
       <c r="B7" t="s">
         <v>267</v>
       </c>
@@ -7977,7 +7970,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="2:5">
+    <row r="8" ht="28.8" spans="2:5">
       <c r="B8" t="s">
         <v>271</v>
       </c>
@@ -8002,7 +7995,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="10" ht="30" spans="2:5">
+    <row r="10" ht="28.8" spans="2:5">
       <c r="B10" t="s">
         <v>389</v>
       </c>
@@ -8016,7 +8009,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="11" ht="45" spans="2:5">
+    <row r="11" ht="43.2" spans="2:5">
       <c r="B11" t="s">
         <v>393</v>
       </c>
@@ -8030,7 +8023,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="12" ht="45" spans="2:5">
+    <row r="12" ht="43.2" spans="2:5">
       <c r="B12" t="s">
         <v>397</v>
       </c>
@@ -8042,7 +8035,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" ht="45" spans="2:5">
+    <row r="13" ht="43.2" spans="2:5">
       <c r="B13" t="s">
         <v>400</v>
       </c>
@@ -8054,7 +8047,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="14" ht="45" spans="2:5">
+    <row r="14" ht="43.2" spans="2:5">
       <c r="B14" t="s">
         <v>402</v>
       </c>
@@ -8066,7 +8059,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" ht="45" spans="2:5">
+    <row r="15" ht="43.2" spans="2:5">
       <c r="B15" t="s">
         <v>405</v>
       </c>
@@ -8129,13 +8122,13 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="44.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="46.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
-    <col min="5" max="5" width="42.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="44.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="46.5740740740741" customWidth="1"/>
+    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="42.1388888888889" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8159,7 +8152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="30" spans="1:1">
+    <row r="2" ht="28.8" spans="1:1">
       <c r="A2" s="4" t="s">
         <v>411</v>
       </c>
@@ -8185,7 +8178,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:6">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -8199,7 +8192,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="30" spans="2:6">
+    <row r="6" ht="28.8" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -8224,7 +8217,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="8" ht="45" spans="2:5">
+    <row r="8" ht="43.2" spans="2:5">
       <c r="B8" t="s">
         <v>417</v>
       </c>
@@ -8238,7 +8231,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="9" ht="45" spans="2:5">
+    <row r="9" ht="43.2" spans="2:5">
       <c r="B9" t="s">
         <v>249</v>
       </c>
@@ -8250,7 +8243,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="45" spans="2:5">
+    <row r="10" ht="43.2" spans="2:5">
       <c r="B10" t="s">
         <v>253</v>
       </c>
@@ -8262,7 +8255,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="30" spans="2:5">
+    <row r="11" ht="28.8" spans="2:5">
       <c r="B11" t="s">
         <v>393</v>
       </c>
@@ -8276,7 +8269,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="12" ht="30" spans="2:5">
+    <row r="12" ht="28.8" spans="2:5">
       <c r="B12" t="s">
         <v>424</v>
       </c>
@@ -8288,7 +8281,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" ht="30" spans="2:5">
+    <row r="13" ht="28.8" spans="2:5">
       <c r="B13" t="s">
         <v>426</v>
       </c>
@@ -8300,7 +8293,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" ht="30" spans="2:5">
+    <row r="14" ht="28.8" spans="2:5">
       <c r="B14" t="s">
         <v>427</v>
       </c>
@@ -8312,7 +8305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" customFormat="1" ht="30" spans="2:5">
+    <row r="15" customFormat="1" ht="28.8" spans="2:5">
       <c r="B15" t="s">
         <v>405</v>
       </c>
@@ -8324,7 +8317,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" ht="45" spans="2:5">
+    <row r="16" ht="43.2" spans="2:5">
       <c r="B16" t="s">
         <v>428</v>
       </c>
@@ -8336,7 +8329,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" ht="45" spans="2:5">
+    <row r="17" ht="43.2" spans="2:5">
       <c r="B17" t="s">
         <v>429</v>
       </c>
@@ -8348,7 +8341,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" ht="45" spans="2:5">
+    <row r="18" ht="43.2" spans="2:5">
       <c r="B18" t="s">
         <v>431</v>
       </c>
@@ -8360,7 +8353,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" ht="45" spans="2:5">
+    <row r="19" ht="43.2" spans="2:5">
       <c r="B19" t="s">
         <v>433</v>
       </c>
@@ -8372,7 +8365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="45" spans="2:5">
+    <row r="20" customFormat="1" ht="43.2" spans="2:5">
       <c r="B20" t="s">
         <v>434</v>
       </c>

</xml_diff>

<commit_message>
docs: update ccda to fhir conversion specification document #1233
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8675" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="430">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -909,13 +909,21 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
+      <t>Document.recordTarget.patientRole.id.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extension</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">"identifier" : [{
         "type" : {
           "coding" : [{
@@ -953,7 +961,31 @@
     </r>
   </si>
   <si>
-    <t>Path to get the identifier -&gt; system</t>
+    <r>
+      <t>Tentatively mapped the path as 
+"http://www.scn.gov/facility/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Document.recordTarget.patientRole.id.extension&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1240,7 +1272,8 @@
     </r>
   </si>
   <si>
-    <t>Path to get the identifier -&gt; value for "Social Security Number"</t>
+    <t>Path to get the identifier -&gt; value for "Social Security Number".
+Not included in the bundle now.</t>
   </si>
   <si>
     <t>text</t>
@@ -1466,9 +1499,6 @@
     <t>scope -&gt; coding -&gt; code</t>
   </si>
   <si>
-    <t>Document.authorization.consent.entry.act.code.code</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1551,75 +1581,63 @@
     </r>
   </si>
   <si>
-    <t>Tentatively mapped the path.</t>
+    <t>Tentatively provided the fixed value as in the example.</t>
   </si>
   <si>
     <t>scope -&gt; coding -&gt; display</t>
   </si>
   <si>
-    <t>Document.authorization.consent.entry.act.code.displayName</t>
-  </si>
-  <si>
     <t>scope -&gt; coding -&gt; system</t>
   </si>
   <si>
-    <t>"http://terminology.hl7.org/CodeSystem/consentscope"</t>
-  </si>
-  <si>
     <t>Tentatively mapped the system.</t>
   </si>
   <si>
     <t>category -&gt; coding -&gt; code</t>
   </si>
   <si>
-    <t>Document.authorization.consent.code.code</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"category" : [{
-        "coding" : [{
-          "system" : "http://loinc.org",
-          "code" : "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>59284-0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",
-          "display" : "Consent Document"
-        }]
-      },</t>
+    <r>
+      <t>"category": [
+                    {
+                        "coding": [
+                            {
+                                "system": "http://loinc.org",
+                                "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "59284-0",
+                                "display": "Consent Document"
+                            }   ]   },
+                    {
+                        "coding": [
+                            {
+                                "system": "http://terminology.hl7.org/CodeSystem/v3-ActCode",
+                                "code": "IDSCL"
+                            }   ]   }   ]</t>
     </r>
   </si>
   <si>
     <t>category -&gt; coding -&gt; display</t>
   </si>
   <si>
-    <t>Document.authorization.consent.code.displayName</t>
-  </si>
-  <si>
     <t>category -&gt; coding -&gt; system</t>
   </si>
   <si>
@@ -1633,6 +1651,9 @@
   </si>
   <si>
     <t>"dateTime" : "2024-02-23T00:00:00Z",</t>
+  </si>
+  <si>
+    <t>If effectiveTime.value is not available, then current time will be shown.</t>
   </si>
   <si>
     <t>provision -&gt; type</t>
@@ -1705,19 +1726,9 @@
     <t>policy -&gt; authority</t>
   </si>
   <si>
-    <t>Document.authorization.consent.policy.id</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
+    <r>
       <t>"policy" : [{
-        "</t>
+            "</t>
     </r>
     <r>
       <rPr>
@@ -1739,7 +1750,7 @@
         <scheme val="minor"/>
       </rPr>
       <t>" : "urn:uuid:d1eaac1a-22b7-4bb6-9c62-cc95d6fdf1a5"
-      }],</t>
+          }]</t>
     </r>
   </si>
   <si>
@@ -1750,11 +1761,6 @@
         "contentType" : "application/pdf",
         "language" : "en"
       },</t>
-  </si>
-  <si>
-    <t>Path to get the 
-sourceAttachment -&gt; contentType and 
-sourceAttachment -&gt; language</t>
   </si>
   <si>
     <t>"request" : {
@@ -3790,48 +3796,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tentatively mapped the status to 'completed' . </t>
-  </si>
-  <si>
-    <t>questionnaire</t>
-  </si>
-  <si>
-    <t>"Questionnaire/&lt;questionnaireResourceId&gt;"</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>questionnaire</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : "http://shinny.org/us/ny/hrsn/Questionnaire/SHINNYDisablityQuestionnaire",</t>
-    </r>
-  </si>
-  <si>
-    <t>Tentatively mapped the dynamically generated Questionnaire resource id</t>
   </si>
   <si>
     <r>
@@ -5340,14 +5304,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="28.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="65.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="73.4259259259259" customWidth="1"/>
-    <col min="5" max="5" width="29.4444444444444" customWidth="1"/>
-    <col min="6" max="6" width="46.287037037037" customWidth="1"/>
+    <col min="4" max="4" width="73.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="29.447619047619" customWidth="1"/>
+    <col min="6" max="6" width="46.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -5396,7 +5360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="57.6" spans="2:4">
+    <row r="5" ht="75" spans="2:4">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -5433,7 +5397,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" ht="28.8" spans="2:3">
+    <row r="9" ht="30" spans="2:3">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -5478,7 +5442,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" ht="28.8" spans="2:5">
+    <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -5489,7 +5453,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" ht="28.8" spans="2:5">
+    <row r="20" ht="45" spans="2:5">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -5500,7 +5464,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" ht="28.8" spans="2:5">
+    <row r="21" ht="45" spans="2:5">
       <c r="B21" t="s">
         <v>37</v>
       </c>
@@ -5511,7 +5475,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" ht="43.2" spans="2:5">
+    <row r="22" ht="75" spans="2:5">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -5522,7 +5486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" ht="43.2" spans="2:5">
+    <row r="23" ht="75" spans="2:5">
       <c r="B23" t="s">
         <v>43</v>
       </c>
@@ -5533,7 +5497,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" ht="28.8" spans="2:5">
+    <row r="24" ht="30" spans="2:5">
       <c r="B24" t="s">
         <v>45</v>
       </c>
@@ -5541,7 +5505,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" ht="28.8" spans="2:5">
+    <row r="25" ht="30" spans="2:5">
       <c r="B25" t="s">
         <v>47</v>
       </c>
@@ -5567,14 +5531,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="36.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="54.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="36.2190476190476" customWidth="1"/>
+    <col min="4" max="4" width="54.8857142857143" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="34.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="34.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -5608,7 +5572,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5622,12 +5586,12 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" customFormat="1" spans="1:6">
+    <row r="5" customFormat="1" ht="30" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -5646,7 +5610,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -5660,18 +5624,18 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="41.7777777777778" style="3" customWidth="1"/>
-    <col min="3" max="3" width="63.8888888888889" style="3" customWidth="1"/>
-    <col min="4" max="4" width="81.287037037037" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.712962962963" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="41.7809523809524" style="3" customWidth="1"/>
+    <col min="3" max="3" width="63.8857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="81.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.7142857142857" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -5719,7 +5683,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" ht="30" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -5739,7 +5703,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" ht="28.8" spans="2:4">
+    <row r="7" ht="30" spans="2:4">
       <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
@@ -5750,7 +5714,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" ht="57.6" spans="2:5">
+    <row r="8" ht="60" spans="2:5">
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
@@ -5806,7 +5770,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" ht="57.6" spans="2:4">
+    <row r="13" ht="60" spans="2:4">
       <c r="B13" s="3" t="s">
         <v>70</v>
       </c>
@@ -5817,7 +5781,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" ht="28.8" spans="2:4">
+    <row r="14" ht="30" spans="2:4">
       <c r="B14" s="3" t="s">
         <v>73</v>
       </c>
@@ -5828,7 +5792,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" ht="30" spans="2:4">
       <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
@@ -5850,7 +5814,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" ht="115.2" spans="2:4">
+    <row r="17" ht="120" spans="2:4">
       <c r="B17" s="3" t="s">
         <v>82</v>
       </c>
@@ -5924,7 +5888,7 @@
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" ht="72" spans="2:4">
+    <row r="25" ht="75" spans="2:4">
       <c r="B25" s="3" t="s">
         <v>99</v>
       </c>
@@ -5946,7 +5910,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" ht="30" spans="2:4">
       <c r="B27" s="3" t="s">
         <v>105</v>
       </c>
@@ -5964,7 +5928,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" ht="30" spans="2:4">
       <c r="B29" s="3" t="s">
         <v>109</v>
       </c>
@@ -5993,7 +5957,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" ht="30" spans="2:4">
       <c r="B32" s="3" t="s">
         <v>105</v>
       </c>
@@ -6011,7 +5975,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" ht="30" spans="2:4">
       <c r="B34" s="3" t="s">
         <v>109</v>
       </c>
@@ -6040,7 +6004,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" ht="30" spans="2:4">
       <c r="B37" s="3" t="s">
         <v>120</v>
       </c>
@@ -6049,7 +6013,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" ht="115.2" spans="2:5">
+    <row r="38" ht="120" spans="2:5">
       <c r="B38" s="3" t="s">
         <v>121</v>
       </c>
@@ -6060,7 +6024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" ht="115.2" spans="2:5">
+    <row r="39" ht="120" spans="2:5">
       <c r="B39" s="3" t="s">
         <v>124</v>
       </c>
@@ -6107,7 +6071,7 @@
       </c>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" ht="187.2" spans="2:5">
+    <row r="44" ht="195" spans="2:5">
       <c r="B44" s="3" t="s">
         <v>134</v>
       </c>
@@ -6121,27 +6085,29 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" ht="187.2" spans="2:5">
+    <row r="45" ht="195" spans="2:5">
       <c r="B45" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="D45" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E45" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="46" ht="187.2" spans="2:5">
+      <c r="E45" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" ht="195" spans="2:5">
       <c r="B46" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>34</v>
@@ -6149,7 +6115,7 @@
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>128</v>
@@ -6159,60 +6125,60 @@
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
       <c r="B50" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" ht="144" spans="2:5">
+    <row r="51" ht="150" spans="2:5">
       <c r="B51" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D52" s="5"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>128</v>
@@ -6222,117 +6188,117 @@
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="3"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="3"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" ht="172.8" spans="2:5">
+    <row r="58" ht="180" spans="2:5">
       <c r="B58" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" ht="72" spans="2:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" ht="75" spans="2:4">
       <c r="B59" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="60" ht="244.8" spans="2:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" ht="255" spans="2:5">
       <c r="B60" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="61" ht="129.6" spans="2:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" ht="135" spans="2:5">
       <c r="B61" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="62" ht="28.8" spans="2:3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" ht="30" spans="2:3">
       <c r="B62" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" ht="28.8" spans="2:3">
+    <row r="63" ht="30" spans="2:3">
       <c r="B63" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" ht="43" customHeight="1" spans="2:4">
       <c r="B65" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D65" s="6"/>
     </row>
@@ -6353,18 +6319,18 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="27.8611111111111" customWidth="1"/>
-    <col min="3" max="3" width="63.4259259259259" customWidth="1"/>
-    <col min="4" max="4" width="68.8611111111111" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="63.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="68.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
-    <col min="6" max="6" width="57.5740740740741" customWidth="1"/>
+    <col min="6" max="6" width="57.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6397,7 +6363,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -6409,7 +6375,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="28.8" spans="2:5">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -6425,30 +6391,28 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" ht="43.2" spans="2:5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" ht="45" spans="2:5">
       <c r="B7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" ht="115.2" spans="2:5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" ht="120" spans="2:5">
       <c r="B8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" t="s">
         <v>189</v>
       </c>
+      <c r="C8"/>
       <c r="D8" s="5" t="s">
         <v>190</v>
       </c>
@@ -6456,34 +6420,31 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="2:3">
+    <row r="9" customFormat="1" spans="2:5">
       <c r="B9" t="s">
         <v>192</v>
       </c>
-      <c r="C9" t="s">
-        <v>193</v>
+      <c r="C9"/>
+      <c r="E9" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10"/>
+      <c r="E10" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" ht="225" spans="2:5">
+      <c r="B11" t="s">
         <v>195</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C11"/>
+      <c r="D11" s="5" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="11" ht="100.8" spans="2:5">
-      <c r="B11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>191</v>
@@ -6491,118 +6452,118 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>197</v>
+      </c>
+      <c r="C12"/>
+      <c r="E12" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C13" t="s">
+        <v>199</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="2:5">
+      <c r="B14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" t="s">
         <v>202</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E14" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" t="s">
+    </row>
+    <row r="15" ht="45" spans="2:5">
+      <c r="B15" t="s">
         <v>204</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>205</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" ht="43.2" spans="2:5">
-      <c r="B15" t="s">
+      <c r="E15" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" ht="45" spans="2:5">
+      <c r="B16" t="s">
         <v>208</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="C16" t="s">
         <v>209</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="16" ht="43.2" spans="2:5">
-      <c r="B16" t="s">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" ht="45" spans="2:5">
+      <c r="B17" t="s">
         <v>211</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>212</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" ht="43.2" spans="2:5">
-      <c r="B17" t="s">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" ht="45" spans="2:5">
+      <c r="B18" t="s">
         <v>214</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18"/>
+      <c r="D18" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" ht="43.2" spans="2:5">
-      <c r="B18" t="s">
-        <v>217</v>
-      </c>
-      <c r="C18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="19" ht="57.6" spans="2:5">
+    <row r="19" ht="60" spans="2:5">
       <c r="B19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="1" ht="43" customHeight="1" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="3"/>
@@ -6622,18 +6583,18 @@
   <sheetPr/>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="33.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="49.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="56.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="53.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="47.5740740740741" customWidth="1"/>
+    <col min="4" max="4" width="56.552380952381" customWidth="1"/>
+    <col min="5" max="5" width="53.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="47.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6667,7 +6628,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6679,7 +6640,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6696,12 +6657,12 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6715,168 +6676,168 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" ht="28.8" spans="2:5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" ht="316.8" spans="2:5">
+    <row r="9" ht="375" spans="2:5">
       <c r="B9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" ht="135" spans="2:4">
+      <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="5" t="s">
+    </row>
+    <row r="11" ht="30" spans="2:3">
+      <c r="B11" t="s">
         <v>232</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="10" ht="129.6" spans="2:4">
-      <c r="B10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" ht="28.8" spans="2:3">
-      <c r="B11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" ht="30" spans="2:3">
+      <c r="B13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" ht="105" spans="2:4">
+      <c r="B14" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D14" s="5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="13" ht="28.8" spans="2:3">
-      <c r="B13" t="s">
+    <row r="15" ht="30" spans="2:3">
+      <c r="B15" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="14" ht="100.8" spans="2:4">
-      <c r="B14" s="3" t="s">
+    <row r="16" ht="30" spans="2:3">
+      <c r="B16" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="2:4">
+      <c r="B17" t="s">
         <v>244</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="C17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="15" ht="28.8" spans="2:3">
-      <c r="B15" s="3" t="s">
+    <row r="18" ht="30" spans="2:3">
+      <c r="B18" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="16" ht="28.8" spans="2:3">
-      <c r="B16" s="3" t="s">
+    <row r="19" ht="45" spans="2:4">
+      <c r="B19" t="s">
         <v>248</v>
       </c>
-      <c r="C16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" ht="57.6" spans="2:4">
-      <c r="B17" t="s">
+      <c r="C19" t="s">
         <v>249</v>
       </c>
-      <c r="C17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
+    <row r="20" ht="30" spans="2:4">
+      <c r="B20" t="s">
         <v>251</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="19" ht="43.2" spans="2:4">
-      <c r="B19" t="s">
+      <c r="D20" t="s">
         <v>253</v>
-      </c>
-      <c r="C19" t="s">
-        <v>254</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" ht="28.8" spans="2:4">
-      <c r="B20" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D20" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D21" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" ht="46" customHeight="1" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D23" s="6"/>
     </row>
@@ -6898,14 +6859,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="35.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="42.287037037037" style="3" customWidth="1"/>
-    <col min="4" max="4" width="73.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="42.2857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.712962962963" customWidth="1"/>
+    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6938,7 +6899,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6950,7 +6911,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6967,306 +6928,306 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" customFormat="1" ht="86.4" spans="2:6">
+    <row r="7" customFormat="1" ht="90" spans="2:6">
       <c r="B7" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="1" ht="30" spans="2:6">
+      <c r="B8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" t="s">
-        <v>270</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" customFormat="1" ht="28.8" spans="2:6">
-      <c r="B8" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" ht="105" spans="2:5">
+      <c r="B10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>275</v>
       </c>
-      <c r="E9" s="3" t="s">
+    </row>
+    <row r="11" ht="30" spans="2:5">
+      <c r="B11" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="10" ht="100.8" spans="2:5">
-      <c r="B10" t="s">
+      <c r="C11" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="11" ht="28.8" spans="2:5">
-      <c r="B11" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="12" ht="28.8" spans="2:5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" ht="120" spans="2:5">
+      <c r="B13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="E13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="2:5">
+      <c r="B14" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="13" ht="115.2" spans="2:5">
-      <c r="B13" t="s">
+      <c r="C14" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E14" t="s">
         <v>288</v>
       </c>
-      <c r="D13" s="5" t="s">
+    </row>
+    <row r="15" ht="30" spans="2:5">
+      <c r="B15" t="s">
         <v>289</v>
       </c>
-      <c r="E13" t="s">
+      <c r="C15" s="3" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="14" ht="28.8" spans="2:5">
-      <c r="B14" t="s">
+      <c r="E15" t="s">
         <v>291</v>
       </c>
-      <c r="C14" s="3" t="s">
+    </row>
+    <row r="16" customFormat="1" ht="30" spans="2:5">
+      <c r="B16" t="s">
         <v>292</v>
       </c>
-      <c r="E14" t="s">
+      <c r="C16" s="3" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="15" ht="28.8" spans="2:5">
-      <c r="B15" t="s">
+      <c r="E16" t="s">
         <v>294</v>
       </c>
-      <c r="C15" s="3" t="s">
+    </row>
+    <row r="17" customFormat="1" ht="60" spans="2:4">
+      <c r="B17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" ht="30" spans="2:3">
+      <c r="B18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" ht="60" spans="2:4">
+      <c r="B19" t="s">
         <v>295</v>
       </c>
-      <c r="E15" t="s">
+      <c r="C19" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="16" customFormat="1" ht="28.8" spans="2:5">
-      <c r="B16" t="s">
+      <c r="D19" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C16" s="3" t="s">
+    </row>
+    <row r="20" ht="30" spans="2:3">
+      <c r="B20" t="s">
         <v>298</v>
       </c>
-      <c r="E16" t="s">
+      <c r="C20" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="57.6" spans="2:4">
-      <c r="B17" t="s">
-        <v>249</v>
-      </c>
-      <c r="C17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" customFormat="1" ht="28.8" spans="2:3">
-      <c r="B18" t="s">
-        <v>251</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="19" ht="57.6" spans="2:4">
-      <c r="B19" t="s">
+    <row r="21" ht="45" spans="2:5">
+      <c r="B21" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="20" ht="28.8" spans="2:3">
-      <c r="B20" t="s">
+      <c r="E21" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C20" s="3" t="s">
+    </row>
+    <row r="22" ht="30" spans="2:5">
+      <c r="B22" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="21" ht="28.8" spans="2:5">
-      <c r="B21" t="s">
+      <c r="C22" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="E22" t="s">
         <v>306</v>
       </c>
-      <c r="D21" s="5" t="s">
+    </row>
+    <row r="23" ht="45" spans="2:3">
+      <c r="B23" t="s">
         <v>307</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="22" ht="28.8" spans="2:5">
-      <c r="B22" t="s">
+    <row r="24" ht="45" spans="2:5">
+      <c r="B24" t="s">
         <v>309</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" s="3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="23" ht="43.2" spans="2:3">
-      <c r="B23" t="s">
+    <row r="25" ht="105" spans="2:5">
+      <c r="B25" t="s">
         <v>312</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="24" ht="43.2" spans="2:5">
-      <c r="B24" t="s">
+      <c r="E25" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C24" s="3" t="s">
+    </row>
+    <row r="26" ht="75" spans="2:5">
+      <c r="B26" t="s">
         <v>315</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="25" ht="100.8" spans="2:5">
-      <c r="B25" t="s">
+      <c r="D26" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E25" s="3" t="s">
+    </row>
+    <row r="27" customFormat="1" ht="30" spans="2:5">
+      <c r="B27" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="26" ht="72" spans="2:5">
-      <c r="B26" t="s">
+      <c r="C27" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="27" customFormat="1" ht="28.8" spans="2:5">
-      <c r="B27" t="s">
-        <v>324</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>325</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" ht="60" spans="2:5">
+      <c r="B28" t="s">
+        <v>322</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="29" customFormat="1" ht="45" spans="2:5">
+      <c r="B29" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="28" customFormat="1" ht="57.6" spans="2:5">
-      <c r="B28" t="s">
+      <c r="C29" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="29" customFormat="1" ht="43.2" spans="2:5">
-      <c r="B29" t="s">
-        <v>331</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D31" s="6"/>
     </row>
@@ -7289,14 +7250,14 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="50.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="72.8611111111111" customWidth="1"/>
-    <col min="5" max="5" width="46.4259259259259" customWidth="1"/>
-    <col min="6" max="6" width="45.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="50.8857142857143" customWidth="1"/>
+    <col min="4" max="4" width="72.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="46.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="45.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7329,7 +7290,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -7354,12 +7315,12 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7367,98 +7328,98 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D7" t="s">
+        <v>334</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="8" ht="165" spans="2:5">
+      <c r="B8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="D7" t="s">
-        <v>339</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" ht="158.4" spans="2:5">
-      <c r="B8" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="10" ht="28.8" spans="2:5">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" ht="30" spans="2:5">
       <c r="B10" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="11" ht="28.8" spans="2:5">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="11" ht="30" spans="2:5">
       <c r="B11" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="12" ht="28.8" spans="2:5">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="2:5">
       <c r="B12" s="3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" ht="30" spans="2:5">
+      <c r="B13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" ht="105" spans="2:5">
+      <c r="B14" t="s">
+        <v>351</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="13" ht="28.8" spans="2:5">
-      <c r="B13" t="s">
-        <v>354</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" ht="100.8" spans="2:5">
-      <c r="B14" t="s">
-        <v>356</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="2:6">
@@ -7470,110 +7431,110 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" customFormat="1" ht="172.8" spans="2:6">
+    <row r="16" customFormat="1" ht="180" spans="2:6">
       <c r="B16" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" customFormat="1" ht="28.8" spans="2:6">
+    <row r="17" customFormat="1" ht="30" spans="2:6">
       <c r="B17" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" customFormat="1" ht="129.6" spans="2:6">
+    <row r="18" customFormat="1" ht="135" spans="2:6">
       <c r="B18" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" customFormat="1" ht="28.8" spans="2:6">
+    <row r="19" customFormat="1" ht="30" spans="2:6">
       <c r="B19" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" customFormat="1" ht="28.8" spans="2:6">
+    <row r="20" customFormat="1" ht="30" spans="2:6">
       <c r="B20" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" customFormat="1" ht="28.8" spans="2:6">
+    <row r="21" customFormat="1" ht="30" spans="2:6">
       <c r="B21" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" customFormat="1" ht="28.8" spans="2:6">
+    <row r="22" customFormat="1" ht="30" spans="2:6">
       <c r="B22" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" customFormat="1" ht="28.8" spans="2:6">
+    <row r="23" customFormat="1" ht="30" spans="2:6">
       <c r="B23" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" customFormat="1" ht="28.8" spans="2:6">
+    <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="3"/>
@@ -7581,21 +7542,21 @@
     </row>
     <row r="25" customFormat="1" spans="2:4">
       <c r="B25" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B26" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D26" s="6"/>
     </row>
@@ -7617,12 +7578,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="46.8611111111111" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="46.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -7647,9 +7608,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="43.2" spans="1:1">
+    <row r="2" ht="45" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7658,7 +7619,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7670,10 +7631,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -7687,12 +7648,12 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="28.8" spans="2:6">
+    <row r="6" ht="30" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7706,157 +7667,157 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" ht="28.8" spans="2:5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" ht="331.2" spans="2:5">
+    <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" ht="135" spans="2:4">
+      <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="10" ht="129.6" spans="2:4">
-      <c r="B10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" ht="28.8" spans="2:3">
+    </row>
+    <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" ht="30" spans="2:3">
+      <c r="B13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" ht="105" spans="2:4">
+      <c r="B14" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" ht="28.8" spans="2:3">
-      <c r="B13" t="s">
+      <c r="D14" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="2:3">
+      <c r="B15" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="14" ht="100.8" spans="2:4">
-      <c r="B14" s="3" t="s">
+    <row r="16" ht="30" spans="2:3">
+      <c r="B16" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="2:4">
+      <c r="B17" t="s">
         <v>244</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="15" ht="28.8" spans="2:3">
-      <c r="B15" s="3" t="s">
+      <c r="C17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="2:3">
+      <c r="B18" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="16" ht="28.8" spans="2:3">
-      <c r="B16" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" ht="57.6" spans="2:4">
-      <c r="B17" t="s">
-        <v>249</v>
-      </c>
-      <c r="C17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" ht="28.8" spans="2:3">
-      <c r="B18" t="s">
+    <row r="19" ht="30" spans="2:4">
+      <c r="B19" t="s">
         <v>251</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="19" ht="28.8" spans="2:4">
-      <c r="B19" t="s">
-        <v>256</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>257</v>
-      </c>
       <c r="D19" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D20" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D22" s="6"/>
     </row>
@@ -7875,15 +7836,15 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="46.5740740740741" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="46.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -7919,7 +7880,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7931,10 +7892,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -7948,34 +7909,34 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="28.8" spans="2:6">
+    <row r="6" ht="30" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" ht="28.8" spans="2:5">
+    <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="28.8" spans="2:5">
+    <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -7983,123 +7944,123 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D9" t="s">
+        <v>382</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" ht="30" spans="2:5">
+      <c r="B10" t="s">
+        <v>384</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E9" s="3" t="s">
+    </row>
+    <row r="11" ht="45" spans="2:5">
+      <c r="B11" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="10" ht="28.8" spans="2:5">
-      <c r="B10" t="s">
+      <c r="C11" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E11" t="s">
         <v>391</v>
       </c>
-      <c r="E10" s="3" t="s">
+    </row>
+    <row r="12" ht="45" spans="2:5">
+      <c r="B12" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="11" ht="43.2" spans="2:5">
-      <c r="B11" t="s">
+      <c r="C12" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="E11" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="12" ht="43.2" spans="2:5">
-      <c r="B12" t="s">
-        <v>397</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="13" ht="43.2" spans="2:5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="14" ht="43.2" spans="2:5">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="15" ht="43.2" spans="2:5">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D18" s="6"/>
     </row>
@@ -8116,19 +8077,19 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A7" sqref="$A7:$XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="44.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="46.5740740740741" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="42.1388888888889" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="44.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="46.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
+    <col min="5" max="5" width="42.1428571428571" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8152,9 +8113,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="28.8" spans="1:1">
+    <row r="2" ht="30" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8163,7 +8124,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8175,232 +8136,204 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="2:6">
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>408</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="28.8" spans="2:6">
-      <c r="B6" s="3" t="s">
-        <v>15</v>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>185</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="7" ht="45" spans="2:5">
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" ht="45" spans="2:5">
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="30" spans="2:5">
+      <c r="B9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" ht="30" spans="2:5">
+      <c r="B10" t="s">
         <v>415</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="8" ht="43.2" spans="2:5">
-      <c r="B8" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" ht="30" spans="2:5">
+      <c r="B11" t="s">
         <v>417</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" ht="30" spans="2:5">
+      <c r="B12" t="s">
         <v>418</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="9" ht="43.2" spans="2:5">
-      <c r="B9" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="43.2" spans="2:5">
-      <c r="B10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C10" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" ht="28.8" spans="2:5">
-      <c r="B11" t="s">
-        <v>393</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="E11" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="12" ht="28.8" spans="2:5">
-      <c r="B12" t="s">
-        <v>424</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>425</v>
+        <v>242</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" ht="28.8" spans="2:5">
+    <row r="13" customFormat="1" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>426</v>
+        <v>400</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" ht="28.8" spans="2:5">
+    <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>247</v>
+        <v>389</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" customFormat="1" ht="28.8" spans="2:5">
+    <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>405</v>
+        <v>420</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>242</v>
+        <v>421</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" ht="43.2" spans="2:5">
+    <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>394</v>
+        <v>423</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" ht="43.2" spans="2:5">
+    <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>430</v>
+        <v>401</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" ht="43.2" spans="2:5">
+    <row r="18" customFormat="1" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" ht="43.2" spans="2:5">
-      <c r="B19" t="s">
-        <v>433</v>
+    <row r="19" spans="2:4">
+      <c r="B19" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" customFormat="1" ht="43.2" spans="2:5">
-      <c r="B20" t="s">
-        <v>434</v>
+        <v>179</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="20" ht="45" customHeight="1" spans="2:4">
+      <c r="B20" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="22" ht="45" customHeight="1" spans="2:4">
-      <c r="B22" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D22" s="6"/>
+        <v>258</v>
+      </c>
+      <c r="D20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D11:D20"/>
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
docs: update xslt files to ensure single name in fhir bundle patient resource #1332
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="434">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Path to get the extension -&gt; valueString for name -&gt; "middle-name"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If 'Official' name (use='L') is there, print it, otherwise, first name. </t>
   </si>
   <si>
     <t>name -&gt; extension -&gt; url</t>
@@ -909,21 +912,13 @@
   </si>
   <si>
     <r>
-      <t>Document.recordTarget.patientRole.id.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>extension</t>
-    </r>
-  </si>
-  <si>
-    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">"identifier" : [{
         "type" : {
           "coding" : [{
@@ -962,6 +957,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Tentatively mapped the path as 
 "http://www.scn.gov/facility/</t>
     </r>
@@ -1597,6 +1599,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"category": [
                     {
                         "coding": [
@@ -1727,6 +1736,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"policy" : [{
             "</t>
     </r>
@@ -2081,13 +2097,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>"subject": {
             "</t>
     </r>
@@ -2162,6 +2171,17 @@
   </si>
   <si>
     <t>"effectiveDateTime" : "2023-07-12T16:08:00.000Z",</t>
+  </si>
+  <si>
+    <t>If there is no value, current date time will be assigned.</t>
+  </si>
+  <si>
+    <t>performer</t>
+  </si>
+  <si>
+    <t>"performer": [ {
+            "reference": "Organization/UMC20250121T1024400530"
+          } ]</t>
   </si>
   <si>
     <t>issued</t>
@@ -2523,6 +2543,63 @@
   </si>
   <si>
     <t>Tentatively mapped the code -&gt; originalText</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"subject": {
+            "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>": "Patient/N65602CUMC20250121T1024400530",
+            "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" : "Doe Jon"
+          }</t>
+    </r>
   </si>
   <si>
     <t>period -&gt; start</t>
@@ -4057,8 +4134,7 @@
     <t>item -&gt; answer -&gt; valueCoding -&gt; system</t>
   </si>
   <si>
-    <t>Document.component.structuredBody.component.
-section.entry.observation.value.codeSystem</t>
+    <t>http://loinc.org</t>
   </si>
   <si>
     <t>item -&gt; answer -&gt; valueCoding -&gt; code</t>
@@ -4737,7 +4813,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4756,10 +4832,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5572,7 +5654,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5586,7 +5668,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -5610,7 +5692,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -5624,8 +5706,8 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -5642,19 +5724,19 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5714,7 +5796,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" ht="60" spans="2:5">
+    <row r="8" ht="60" spans="2:6">
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
@@ -5727,370 +5809,373 @@
       <c r="E8" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="F8" s="9" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" ht="60" spans="2:4">
       <c r="B13" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:4">
       <c r="B15" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" ht="120" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" ht="75" spans="2:4">
       <c r="B25" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="8" t="s">
         <v>104</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" ht="30" spans="2:4">
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="6"/>
+        <v>107</v>
+      </c>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="6"/>
+        <v>109</v>
+      </c>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" ht="30" spans="2:4">
       <c r="B29" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="6"/>
+        <v>113</v>
+      </c>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32" ht="30" spans="2:4">
       <c r="B32" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="6"/>
+        <v>115</v>
+      </c>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" ht="30" spans="2:4">
       <c r="B34" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="6"/>
+        <v>118</v>
+      </c>
+      <c r="D35" s="7"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" s="6" t="s">
         <v>119</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="37" ht="30" spans="2:4">
       <c r="B37" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" ht="120" spans="2:5">
       <c r="B38" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" ht="120" spans="2:5">
       <c r="B39" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" ht="195" spans="2:5">
       <c r="B44" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" ht="195" spans="2:5">
       <c r="B45" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>140</v>
@@ -6118,7 +6203,7 @@
         <v>145</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="3"/>
@@ -6158,7 +6243,7 @@
         <v>151</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>152</v>
@@ -6181,7 +6266,7 @@
         <v>156</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="3"/>
@@ -6289,7 +6374,7 @@
       <c r="C64" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="7" t="s">
         <v>180</v>
       </c>
     </row>
@@ -6300,7 +6385,7 @@
       <c r="C65" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D65" s="6"/>
+      <c r="D65" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6319,8 +6404,8 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6412,7 +6497,6 @@
       <c r="B8" t="s">
         <v>189</v>
       </c>
-      <c r="C8"/>
       <c r="D8" s="5" t="s">
         <v>190</v>
       </c>
@@ -6424,7 +6508,6 @@
       <c r="B9" t="s">
         <v>192</v>
       </c>
-      <c r="C9"/>
       <c r="E9" s="3" t="s">
         <v>191</v>
       </c>
@@ -6433,7 +6516,6 @@
       <c r="B10" t="s">
         <v>193</v>
       </c>
-      <c r="C10"/>
       <c r="E10" s="1" t="s">
         <v>194</v>
       </c>
@@ -6442,7 +6524,6 @@
       <c r="B11" t="s">
         <v>195</v>
       </c>
-      <c r="C11"/>
       <c r="D11" s="5" t="s">
         <v>196</v>
       </c>
@@ -6454,7 +6535,6 @@
       <c r="B12" t="s">
         <v>197</v>
       </c>
-      <c r="C12"/>
       <c r="E12" s="3" t="s">
         <v>191</v>
       </c>
@@ -6526,7 +6606,6 @@
       <c r="B18" t="s">
         <v>214</v>
       </c>
-      <c r="C18"/>
       <c r="D18" s="5" t="s">
         <v>215</v>
       </c>
@@ -6552,7 +6631,7 @@
       <c r="C20" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>218</v>
       </c>
       <c r="E20" s="3"/>
@@ -6565,7 +6644,7 @@
       <c r="C21" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
@@ -6581,10 +6660,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6690,7 +6769,7 @@
         <v>225</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
@@ -6799,7 +6878,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" ht="30" spans="2:4">
+    <row r="20" ht="30" spans="2:5">
       <c r="B20" t="s">
         <v>251</v>
       </c>
@@ -6809,41 +6888,55 @@
       <c r="D20" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="E20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" ht="45" spans="2:4">
       <c r="B21" t="s">
-        <v>254</v>
-      </c>
-      <c r="D21" t="s">
         <v>255</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" t="s">
+        <v>258</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="23" ht="46" customHeight="1" spans="2:4">
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" ht="46" customHeight="1" spans="2:4">
+      <c r="B24" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="6"/>
+      <c r="C24" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D23:D24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -6876,7 +6969,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -6899,7 +6992,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6911,7 +7004,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6933,7 +7026,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6941,29 +7034,29 @@
     </row>
     <row r="7" customFormat="1" ht="90" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E7" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="1" ht="30" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -6972,98 +7065,98 @@
         <v>185</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D9" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" ht="105" spans="2:5">
       <c r="B10" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" ht="120" spans="2:5">
       <c r="B13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E14" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:5">
       <c r="B15" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E15" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E16" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" customFormat="1" ht="60" spans="2:4">
@@ -7074,7 +7167,7 @@
         <v>209</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="30" spans="2:3">
@@ -7087,128 +7180,128 @@
     </row>
     <row r="19" ht="60" spans="2:4">
       <c r="B19" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:3">
       <c r="B20" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:5">
       <c r="B21" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E22" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" ht="45" spans="2:3">
       <c r="B23" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" ht="45" spans="2:5">
       <c r="B24" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" ht="105" spans="2:5">
       <c r="B25" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" ht="75" spans="2:5">
       <c r="B26" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="60" spans="2:5">
       <c r="B28" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="45" spans="2:5">
       <c r="B29" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:4">
@@ -7218,8 +7311,8 @@
       <c r="C30" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>329</v>
+      <c r="D30" s="7" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -7227,9 +7320,9 @@
         <v>181</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D31" s="6"/>
+        <v>334</v>
+      </c>
+      <c r="D31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7290,7 +7383,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -7320,7 +7413,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7328,134 +7421,134 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D7" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="3" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" ht="105" spans="2:5">
       <c r="B14" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="2:6">
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" customFormat="1" ht="180" spans="2:6">
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:6">
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -7463,23 +7556,23 @@
     </row>
     <row r="18" customFormat="1" ht="135" spans="2:6">
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" customFormat="1" ht="30" spans="2:6">
       <c r="B19" s="3" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
@@ -7487,10 +7580,10 @@
     </row>
     <row r="20" customFormat="1" ht="30" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
@@ -7498,10 +7591,10 @@
     </row>
     <row r="21" customFormat="1" ht="30" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
@@ -7509,10 +7602,10 @@
     </row>
     <row r="22" customFormat="1" ht="30" spans="2:6">
       <c r="B22" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3"/>
@@ -7520,10 +7613,10 @@
     </row>
     <row r="23" customFormat="1" ht="30" spans="2:6">
       <c r="B23" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="3"/>
@@ -7531,10 +7624,10 @@
     </row>
     <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="3"/>
@@ -7547,8 +7640,8 @@
       <c r="C25" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>368</v>
+      <c r="D25" s="7" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -7556,9 +7649,9 @@
         <v>181</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="D26" s="6"/>
+        <v>373</v>
+      </c>
+      <c r="D26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7610,7 +7703,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7631,7 +7724,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7653,7 +7746,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7681,7 +7774,7 @@
         <v>225</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" ht="390" spans="2:5">
@@ -7689,10 +7782,10 @@
         <v>226</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
@@ -7741,7 +7834,7 @@
         <v>239</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
@@ -7768,7 +7861,7 @@
         <v>209</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
@@ -7792,13 +7885,13 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D20" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -7808,8 +7901,8 @@
       <c r="C21" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>376</v>
+      <c r="D21" s="7" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
@@ -7817,9 +7910,9 @@
         <v>181</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="6"/>
+        <v>261</v>
+      </c>
+      <c r="D22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7880,7 +7973,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7892,7 +7985,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7914,7 +8007,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7922,10 +8015,10 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>34</v>
@@ -7933,10 +8026,10 @@
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>34</v>
@@ -7947,101 +8040,101 @@
         <v>185</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D9" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="E11" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -8051,8 +8144,8 @@
       <c r="C17" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>376</v>
+      <c r="D17" s="7" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
@@ -8060,9 +8153,9 @@
         <v>181</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="6"/>
+        <v>261</v>
+      </c>
+      <c r="D18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8080,7 +8173,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="$A7:$XFD7"/>
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8115,7 +8208,7 @@
     </row>
     <row r="2" ht="30" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8124,7 +8217,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8136,7 +8229,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" ht="30" spans="2:6">
@@ -8144,7 +8237,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -8155,13 +8248,13 @@
         <v>185</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="D6" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" ht="45" spans="2:5">
@@ -8172,7 +8265,7 @@
         <v>209</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -8184,30 +8277,30 @@
         <v>249</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" ht="30" spans="2:5">
       <c r="B9" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="E9" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="10" ht="30" spans="2:5">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>415</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>416</v>
+        <v>419</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>420</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
@@ -8216,7 +8309,7 @@
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>239</v>
@@ -8228,7 +8321,7 @@
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>242</v>
@@ -8240,7 +8333,7 @@
     </row>
     <row r="13" customFormat="1" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>237</v>
@@ -8252,10 +8345,10 @@
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
@@ -8264,10 +8357,10 @@
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
@@ -8276,10 +8369,10 @@
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
@@ -8288,10 +8381,10 @@
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" t="s">
@@ -8300,10 +8393,10 @@
     </row>
     <row r="18" customFormat="1" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
@@ -8317,8 +8410,8 @@
       <c r="C19" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>376</v>
+      <c r="D19" s="7" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="20" ht="45" customHeight="1" spans="2:4">
@@ -8326,15 +8419,18 @@
         <v>181</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>261</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D9:D18"/>
     <mergeCell ref="D19:D20"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" display="http://loinc.org"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
docs: update ccd to fhir conversion document #1355
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Bundle" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="436">
   <si>
     <t>FHIR Resource</t>
   </si>
@@ -137,6 +137,43 @@
     <t>Document.authorization.consent</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with 'ststusCode.code' as 'completed' and 'act.code.code' as 'deny'.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> files, should it take from Observation with code "105511-0", if  no consent sentcion is present?</t>
+    </r>
+  </si>
+  <si>
     <t>Observation (Sexual orientation)</t>
   </si>
   <si>
@@ -195,21 +232,69 @@
     </r>
   </si>
   <si>
-    <t>Tentatively mapped</t>
+    <r>
+      <t xml:space="preserve">Tentatively mapped.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> files, there is no section with LOINC code = '76690-7'. So no Sexual Orientation resource included.</t>
+    </r>
   </si>
   <si>
     <t>Observation</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Document.component.structuredBody.component.section.entry.observation
+      <t>Document.component.structuredBody.component.section[code=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>29762-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">].entry.observation
 where </t>
     </r>
     <r>
@@ -235,6 +320,63 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Tentatively mapped from Social History Section[code=29762-2]. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> files, mapped from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Procedures Section[code=47519-4] for Medent files.</t>
+    </r>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
@@ -248,15 +390,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Document.component.structuredBody.component.section.entry.observation
-where Document.component.structuredBody.component.section.templateId. root = '</t>
+      <t>Document.component.structuredBody.component.section.entry.observation where Document.component.structuredBody.component.section.templateId. root = '</t>
     </r>
     <r>
       <rPr>
@@ -288,15 +422,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Document.component.structuredBody.component.section.entry.observation
-where Document.component.structuredBody.component.section.templateId. root other than  '</t>
+      <t>Document.component.structuredBody.component.section.entry.observation where Document.component.structuredBody.component.section.templateId. root other than  '</t>
     </r>
     <r>
       <rPr>
@@ -1071,6 +1197,9 @@
     </r>
   </si>
   <si>
+    <t>Tentatively mapped</t>
+  </si>
+  <si>
     <t>identifier (MA) -&gt; type -&gt; coding -&gt; system</t>
   </si>
   <si>
@@ -1495,7 +1624,7 @@
     <t>"status": "active"</t>
   </si>
   <si>
-    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with 'ststusCode -&gt; code' as 'completed' and 'act -&gt; code -&gt; code' as 'deny'.</t>
+    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with 'ststusCode.code' as 'completed' and 'act.code.code' as 'deny'.</t>
   </si>
   <si>
     <t>scope -&gt; coding -&gt; code</t>
@@ -2097,6 +2226,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"subject": {
             "</t>
     </r>
@@ -2543,63 +2679,6 @@
   </si>
   <si>
     <t>Tentatively mapped the code -&gt; originalText</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"subject": {
-            "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>reference</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>": "Patient/N65602CUMC20250121T1024400530",
-            "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>display</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" : "Doe Jon"
-          }</t>
-    </r>
   </si>
   <si>
     <t>period -&gt; start</t>
@@ -4189,7 +4268,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4352,6 +4431,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4813,7 +4907,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4841,11 +4935,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5382,8 +5479,8 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -5392,7 +5489,7 @@
     <col min="2" max="2" width="28.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="65.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="73.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="29.447619047619" customWidth="1"/>
+    <col min="5" max="5" width="61.2857142857143" customWidth="1"/>
     <col min="6" max="6" width="46.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5516,83 +5613,86 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" ht="75" spans="2:5">
       <c r="B18" t="s">
         <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>31</v>
       </c>
+      <c r="E18" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" ht="45" spans="2:5">
-      <c r="B19" t="s">
-        <v>32</v>
+      <c r="B19" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
         <v>34</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" ht="45" spans="2:5">
       <c r="B20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" ht="45" spans="2:5">
+        <v>37</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" ht="75" spans="2:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" ht="60" spans="2:5">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" ht="75" spans="2:5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" ht="60" spans="2:5">
       <c r="B23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" ht="30" spans="2:5">
+    </row>
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" ht="30" spans="2:5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -5610,7 +5710,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -5645,7 +5745,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:6">
@@ -5654,7 +5754,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5668,7 +5768,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -5679,11 +5779,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -5692,7 +5792,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -5706,8 +5806,8 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -5751,7 +5851,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -5762,7 +5862,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:5">
@@ -5771,10 +5871,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -5782,608 +5882,608 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" ht="30" spans="2:4">
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" ht="60" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" ht="60" spans="2:4">
       <c r="B13" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:4">
       <c r="B15" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" ht="120" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" ht="75" spans="2:4">
       <c r="B25" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" ht="30" spans="2:4">
       <c r="B27" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D28" s="7"/>
     </row>
     <row r="29" ht="30" spans="2:4">
       <c r="B29" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" ht="30" spans="2:4">
       <c r="B32" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D33" s="7"/>
     </row>
     <row r="34" ht="30" spans="2:4">
       <c r="B34" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" ht="30" spans="2:4">
       <c r="B37" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D37" s="7"/>
     </row>
     <row r="38" ht="120" spans="2:5">
       <c r="B38" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" ht="120" spans="2:5">
       <c r="B39" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" ht="195" spans="2:5">
       <c r="B44" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" ht="195" spans="2:5">
       <c r="B45" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" ht="195" spans="2:5">
       <c r="B46" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
       <c r="B50" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="3"/>
     </row>
     <row r="51" ht="150" spans="2:5">
       <c r="B51" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D52" s="5"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="3"/>
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="3"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="3"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D57" s="5"/>
     </row>
     <row r="58" ht="180" spans="2:5">
       <c r="B58" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" ht="75" spans="2:4">
       <c r="B59" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" ht="255" spans="2:5">
       <c r="B60" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" ht="135" spans="2:5">
       <c r="B61" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" ht="30" spans="2:3">
       <c r="B62" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" ht="30" spans="2:3">
       <c r="B63" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" ht="43" customHeight="1" spans="2:4">
       <c r="B65" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D65" s="7"/>
     </row>
@@ -6404,8 +6504,8 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6414,7 +6514,7 @@
     <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="63.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="68.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="50" customWidth="1"/>
+    <col min="5" max="5" width="52.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="57.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6448,7 +6548,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -6468,7 +6568,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -6476,173 +6576,174 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" ht="45" spans="2:5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" ht="45" spans="2:6">
       <c r="B7" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>188</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:5">
       <c r="B9" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" ht="225" spans="2:5">
       <c r="B11" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="1" ht="43" customHeight="1" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="3"/>
@@ -6662,8 +6763,8 @@
   <sheetPr/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6698,7 +6799,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6707,7 +6808,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6719,7 +6820,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -6728,11 +6829,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -6741,7 +6842,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6749,188 +6850,188 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:4">
       <c r="B19" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:5">
       <c r="B20" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D20" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E20" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:4">
       <c r="B21" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>256</v>
+        <v>215</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D22" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" ht="46" customHeight="1" spans="2:4">
       <c r="B24" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D24" s="7"/>
     </row>
@@ -6949,7 +7050,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6992,7 +7093,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7004,7 +7105,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7013,11 +7114,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -7026,7 +7127,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7034,293 +7135,293 @@
     </row>
     <row r="7" customFormat="1" ht="90" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E7" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="1" ht="30" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D9" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" ht="105" spans="2:5">
       <c r="B10" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E10" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" ht="120" spans="2:5">
       <c r="B13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E13" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E14" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:5">
       <c r="B15" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E15" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E16" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" customFormat="1" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:4">
       <c r="B19" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:3">
       <c r="B20" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:5">
       <c r="B21" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E22" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" ht="45" spans="2:3">
       <c r="B23" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" ht="45" spans="2:5">
       <c r="B24" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" ht="105" spans="2:5">
       <c r="B25" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" ht="75" spans="2:5">
       <c r="B26" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" customFormat="1" ht="60" spans="2:5">
       <c r="B28" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="45" spans="2:5">
       <c r="B29" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="2:4">
       <c r="B30" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D31" s="7"/>
     </row>
@@ -7340,7 +7441,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7383,7 +7484,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -7400,11 +7501,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -7413,7 +7514,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7421,134 +7522,134 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D7" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="3" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="3" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:5">
       <c r="B13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>351</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" ht="105" spans="2:5">
       <c r="B14" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="2:6">
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" customFormat="1" ht="180" spans="2:6">
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:6">
       <c r="B17" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -7556,23 +7657,23 @@
     </row>
     <row r="18" customFormat="1" ht="135" spans="2:6">
       <c r="B18" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" customFormat="1" ht="30" spans="2:6">
       <c r="B19" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
@@ -7580,10 +7681,10 @@
     </row>
     <row r="20" customFormat="1" ht="30" spans="2:6">
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
@@ -7591,10 +7692,10 @@
     </row>
     <row r="21" customFormat="1" ht="30" spans="2:6">
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
@@ -7602,10 +7703,10 @@
     </row>
     <row r="22" customFormat="1" ht="30" spans="2:6">
       <c r="B22" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3"/>
@@ -7613,10 +7714,10 @@
     </row>
     <row r="23" customFormat="1" ht="30" spans="2:6">
       <c r="B23" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="3"/>
@@ -7624,10 +7725,10 @@
     </row>
     <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="3"/>
@@ -7635,21 +7736,21 @@
     </row>
     <row r="25" customFormat="1" spans="2:4">
       <c r="B25" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B26" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D26" s="7"/>
     </row>
@@ -7668,7 +7769,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7703,7 +7804,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7712,7 +7813,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7724,7 +7825,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7733,11 +7834,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -7746,7 +7847,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -7754,163 +7855,163 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D19" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D20" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D22" s="7"/>
     </row>
@@ -7929,7 +8030,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7964,7 +8065,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -7973,7 +8074,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7985,7 +8086,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -7994,11 +8095,11 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -8007,7 +8108,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8015,145 +8116,145 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E11" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D18" s="7"/>
     </row>
@@ -8173,7 +8274,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8208,7 +8309,7 @@
     </row>
     <row r="2" ht="30" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8217,7 +8318,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8229,7 +8330,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" ht="30" spans="2:6">
@@ -8237,7 +8338,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -8245,181 +8346,181 @@
     </row>
     <row r="6" spans="2:5">
       <c r="B6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D6" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" ht="45" spans="2:5">
       <c r="B7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" ht="45" spans="2:5">
       <c r="B8" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C8" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" ht="30" spans="2:5">
       <c r="B9" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E9" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" customFormat="1" ht="30" spans="2:5">
       <c r="B13" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" ht="45" customHeight="1" spans="2:4">
       <c r="B20" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D20" s="7"/>
     </row>

</xml_diff>

<commit_message>
docs: update the CCD to FHIR conversion spec to incorporate the logic for getting the CIN, MRN and SSN of Patient resource #1355
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="439">
   <si>
     <t>FHIR Resource Element column</t>
   </si>
@@ -141,6 +141,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Document.componentOf.encompassingEncounter.
 If it is not present in the CCDA file, the encounter details will be taken from the first occurance of the Document.component.structuredBody.component.section[code[@code='</t>
     </r>
@@ -490,6 +497,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Document.component.structuredBody.component.section[code[@code='</t>
     </r>
     <r>
@@ -758,7 +772,7 @@
     <t>extension -&gt; extension -&gt; url</t>
   </si>
   <si>
-    <t>"ombCategory"</t>
+    <t>"ombCategory" or "detailed"</t>
   </si>
   <si>
     <r>
@@ -807,6 +821,9 @@
     </r>
   </si>
   <si>
+    <t>If the race codes are in any one from the list (1002-5, 2028-9, 2054-5, 2076-8, 2106-3, UNK, ASKU), the url will be 'ombCategory', otherwise 'detailed'.</t>
+  </si>
+  <si>
     <t>extension -&gt; extension -&gt; valueCoding -&gt; system</t>
   </si>
   <si>
@@ -846,6 +863,9 @@
         "url" : "http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity"      },</t>
   </si>
   <si>
+    <t>If the ethnicity codes are in any one from the list (2135-2, 2186-5, UNK, ASKU), the url will be 'ombCategory', otherwise 'detailed'.</t>
+  </si>
+  <si>
     <t>Document.recordTarget.patientRole.patient.ethnicGroupCode.codeSystem</t>
   </si>
   <si>
@@ -1027,19 +1047,12 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Document.recordTarget.patientRole.id.</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1117,23 +1130,13 @@
       </rPr>
       <t xml:space="preserve"> CCDA files, 
 'id.extension', only if assigningAuthorityName="EPI" and root="1.2.840.114350.1.13.570.2.7.5.737384.14" or root != "1.2.840.114350.1.1".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
+For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1143,30 +1146,39 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CCDA files,
-'id.extension', if assigningAuthorityName is not set.
-For other CCDA files,
-'id.extension', if assigningAuthorityName is not set.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
         <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
+      <t xml:space="preserve"> and all other CCDA files,
+the first occurance of 'id.extension', if root is not '2.16.840.1.113883.4.1' and extension is not in the SSN format.</t>
     </r>
   </si>
   <si>
     <t>identifier (MR) -&gt; system</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Document.recordTarget.patientRole.id.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extension</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1215,13 +1227,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Tentatively mapped the path as 
 "http://www.scn.gov/facility/</t>
     </r>
@@ -1425,77 +1430,8 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Epic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CCDA files, 
-'id.extension', only if assigningAuthorityName="EPI" and root="1.2.840.114350.1.1".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Medent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CCDA files,
-'id.extension', if assigningAuthorityName="EPI".
-For other CCDA files,
-'id.extension', if assigningAuthorityName="EPI".</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>The value is reading from the header 'X-TechBD-CIN'
 The format of MA should be 2 letters, 5 digits, 1 letter (e.g., AB12345C)</t>
-    </r>
   </si>
   <si>
     <t>identifier (MA) -&gt; system</t>
@@ -1606,7 +1542,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">For </t>
+      <t>The extension value only if root</t>
     </r>
     <r>
       <rPr>
@@ -1617,7 +1553,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Epic</t>
+      <t xml:space="preserve"> is '2.16.840.1.113883.4.1'</t>
     </r>
     <r>
       <rPr>
@@ -1627,54 +1563,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> CCDA files, 
-'id.extension', only if assigningAuthorityName="JMR123"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Medent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CCDA files,
-'id.extension', if assigningAuthorityName="JMR123".
-For other CCDA files,
-'id.extension', if assigningAuthorityName="JMR123".</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The format of SS value should be xxx-xx-xxxx.</t>
+      <t xml:space="preserve"> and if that is not present then the extension in the form of xxx-xx-xxxx</t>
     </r>
   </si>
   <si>
@@ -2189,6 +2078,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">The Observations are taken from:
 For </t>
     </r>
@@ -2762,6 +2658,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">The Encounter details are taken from </t>
     </r>
     <r>
@@ -3475,10 +3378,14 @@
     <t>identifier (TAX) -&gt; value</t>
   </si>
   <si>
-    <t>Document.author.assignedAuthor.representedOrganization.id.extension</t>
-  </si>
-  <si>
-    <r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"identifier" : [{
         "type" : {
           "coding" : [{
@@ -3535,7 +3442,7 @@
     </r>
   </si>
   <si>
-    <t>Only if id.assigningAuthorityName='TAX'.</t>
+    <t>The value is reading from the header 'X-TechBD-OrgTIN'</t>
   </si>
   <si>
     <t>identifier (TAX) -&gt; system</t>
@@ -3562,10 +3469,14 @@
     <t>identifier (NPI) -&gt; value</t>
   </si>
   <si>
-    <t>Document.author.assignedAuthor.id.extension</t>
-  </si>
-  <si>
-    <r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"identifier" : [{
         "type" : {
           "coding" : [{
@@ -3622,7 +3533,7 @@
     </r>
   </si>
   <si>
-    <t>Only if id.root = '2.16.840.1.113883.4.6'.</t>
+    <t>The value is reading from the header 'X-TechBD-OrgNPI'</t>
   </si>
   <si>
     <t>identifier (NPI) -&gt; system</t>
@@ -4115,6 +4026,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">For </t>
     </r>
     <r>
@@ -4177,6 +4095,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"encounter": {
             "</t>
     </r>
@@ -4208,6 +4133,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"performedPeriod" : {
         "</t>
     </r>
@@ -5263,7 +5195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5814,7 +5746,7 @@
   <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -5935,7 +5867,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5947,7 +5879,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -5969,7 +5901,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -5977,145 +5909,145 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D18" s="11"/>
     </row>
@@ -6135,7 +6067,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6256,7 +6188,7 @@
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6338,7 +6270,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6396,7 +6328,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:5">
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>18</v>
@@ -6615,7 +6547,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" ht="45" spans="2:5">
       <c r="B26" s="4" t="s">
         <v>106</v>
       </c>
@@ -6625,44 +6557,47 @@
       <c r="D26" s="17" t="s">
         <v>108</v>
       </c>
+      <c r="E26" s="18" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="27" ht="30" spans="2:4">
       <c r="B27" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D28" s="11"/>
     </row>
     <row r="29" ht="30" spans="2:4">
       <c r="B29" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" ht="45" spans="2:5">
       <c r="B31" s="4" t="s">
         <v>106</v>
       </c>
@@ -6670,59 +6605,62 @@
         <v>107</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" ht="30" spans="2:4">
       <c r="B32" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D32" s="11"/>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D33" s="11"/>
     </row>
     <row r="34" ht="30" spans="2:4">
       <c r="B34" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" ht="30" spans="2:4">
       <c r="B37" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>81</v>
@@ -6731,260 +6669,261 @@
     </row>
     <row r="38" ht="120" spans="2:5">
       <c r="B38" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" ht="120" spans="2:5">
       <c r="B39" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D42" s="9"/>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D43" s="9"/>
     </row>
     <row r="44" ht="195" spans="2:5">
       <c r="B44" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" ht="195" spans="2:5">
       <c r="B45" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" ht="195" spans="2:5">
       <c r="B46" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="4"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="4"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
       <c r="B50" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" ht="195" spans="2:5">
+    <row r="51" ht="150" spans="2:5">
       <c r="B51" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>139</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="4" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D52" s="9"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="4" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="4"/>
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="4"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="4"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D57" s="9"/>
     </row>
     <row r="58" ht="180" spans="2:5">
       <c r="B58" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" ht="75" spans="2:4">
       <c r="B59" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" ht="255" spans="2:5">
       <c r="B60" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" ht="135" spans="2:5">
       <c r="B61" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" ht="30" spans="2:3">
       <c r="B62" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>57</v>
@@ -6992,29 +6931,29 @@
     </row>
     <row r="63" ht="30" spans="2:3">
       <c r="B63" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" ht="43" customHeight="1" spans="2:4">
       <c r="B65" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D65" s="11"/>
     </row>
@@ -7079,7 +7018,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -7107,174 +7046,174 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" ht="45" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" ht="225" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D14" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C15" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" s="5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" s="5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="1" ht="43" customHeight="1" spans="2:6">
       <c r="B21" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="4"/>
@@ -7333,7 +7272,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7346,7 +7285,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7358,7 +7297,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7380,7 +7319,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7394,191 +7333,191 @@
         <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:4">
       <c r="B19" s="5" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C19" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D20" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E20" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:4">
       <c r="B21" s="5" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D22" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" ht="46" customHeight="1" spans="2:4">
       <c r="B24" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D24" s="11"/>
     </row>
@@ -7636,7 +7575,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7647,7 +7586,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7659,7 +7598,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7681,7 +7620,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7689,262 +7628,262 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" ht="105" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" ht="30" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="14" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" ht="120" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E12" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E14" t="s">
         <v>294</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="E14" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="60" spans="2:4">
       <c r="B15" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:3">
       <c r="B16" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" ht="60" spans="2:5">
       <c r="B23" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" ht="75" spans="2:5">
       <c r="B24" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" customFormat="1" ht="30" spans="2:5">
       <c r="B25" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="60" spans="2:5">
       <c r="B26" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:4">
       <c r="B28" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B29" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D29" s="11"/>
     </row>
@@ -7965,7 +7904,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8008,7 +7947,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -8038,7 +7977,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8046,144 +7985,140 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D7" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>336</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>337</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="4" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="4" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="4" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="1" ht="165" spans="2:5">
       <c r="B13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>348</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:5">
       <c r="B17" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" ht="30" spans="2:5">
       <c r="B18" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" ht="105" spans="2:5">
       <c r="B19" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -8195,7 +8130,7 @@
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -8204,13 +8139,13 @@
         <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F21" s="4"/>
     </row>
@@ -8219,7 +8154,7 @@
         <v>103</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -8230,20 +8165,20 @@
         <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="4"/>
@@ -8254,7 +8189,7 @@
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="4"/>
@@ -8265,7 +8200,7 @@
         <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="4"/>
@@ -8276,7 +8211,7 @@
         <v>93</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="4"/>
@@ -8287,7 +8222,7 @@
         <v>95</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="4"/>
@@ -8298,7 +8233,7 @@
         <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="4"/>
@@ -8306,21 +8241,21 @@
     </row>
     <row r="30" customFormat="1" spans="2:4">
       <c r="B30" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B31" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D31" s="11"/>
     </row>
@@ -8374,7 +8309,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8383,7 +8318,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8395,7 +8330,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -8417,7 +8352,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8431,157 +8366,157 @@
         <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" s="5" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D19" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D20" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D22" s="11"/>
     </row>
@@ -8638,7 +8573,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -8649,7 +8584,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8661,7 +8596,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -8683,7 +8618,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8691,128 +8626,128 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="2:5">
       <c r="B11" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E11" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" customFormat="1" ht="60" spans="2:4">
       <c r="B12" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" customFormat="1" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" customFormat="1" ht="45" spans="2:4">
       <c r="B14" s="5" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" ht="60" spans="2:4">
       <c r="B15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="2:4">
       <c r="B17" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B18" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D18" s="11"/>
     </row>

</xml_diff>

<commit_message>
docs: update CCDA FHIR conversion document with changes in Patient, Encounter, Sexual Orientation and Observation resources #1355
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="442">
   <si>
     <t>FHIR Resource Element column</t>
   </si>
@@ -1047,6 +1047,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Document.recordTarget.patientRole.id.</t>
     </r>
     <r>
@@ -1107,6 +1114,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">For </t>
     </r>
     <r>
@@ -1157,28 +1171,6 @@
   </si>
   <si>
     <t>identifier (MR) -&gt; system</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Document.recordTarget.patientRole.id.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>extension</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1226,31 +1218,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Tentatively mapped the path as 
-"http://www.scn.gov/facility/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;Document.recordTarget.patientRole.id.extension&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
+    <t>Get from the header variable `X-TechBD-Facility-ID`</t>
   </si>
   <si>
     <r>
@@ -1542,6 +1510,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>The extension value only if root</t>
     </r>
     <r>
@@ -1784,10 +1759,13 @@
     <t>"status": "active"</t>
   </si>
   <si>
-    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with 'ststusCode.code' as 'completed' and 'act.code.code' as 'deny'.</t>
+    <t>If there is no consent sentcion in the CCDA XML file, the Consent resource will be generated with 'consent.statusCode.code' as 'completed' and 'consent.code.displayName' as 'deny'.</t>
   </si>
   <si>
     <t>scope -&gt; coding -&gt; code</t>
+  </si>
+  <si>
+    <t>"treatment"</t>
   </si>
   <si>
     <r>
@@ -1878,7 +1856,13 @@
     <t>scope -&gt; coding -&gt; display</t>
   </si>
   <si>
+    <t>"Treatment"</t>
+  </si>
+  <si>
     <t>scope -&gt; coding -&gt; system</t>
+  </si>
+  <si>
+    <t>"http://terminology.hl7.org/CodeSystem/consentscope"</t>
   </si>
   <si>
     <t>Tentatively mapped the system.</t>
@@ -1957,7 +1941,7 @@
     <t>provision -&gt; type</t>
   </si>
   <si>
-    <t>Document.authorization.consent.provision.type</t>
+    <t>Document.authorization.consent.code.displayName</t>
   </si>
   <si>
     <r>
@@ -1995,8 +1979,7 @@
     </r>
   </si>
   <si>
-    <t>act -&gt; code -&gt; displayName 
-('deny' or 'permit')</t>
+    <t>consent -&gt; code -&gt; displayName will be 'deny' or 'permit'.</t>
   </si>
   <si>
     <t>patient -&gt; reference</t>
@@ -2022,6 +2005,9 @@
   </si>
   <si>
     <t>policy -&gt; authority</t>
+  </si>
+  <si>
+    <t>"urn:uuid:d1eaac1a-22b7-4bb6-9c62-cc95d6fdf1a5"</t>
   </si>
   <si>
     <r>
@@ -2622,13 +2608,113 @@
     <t>effectiveDateTime</t>
   </si>
   <si>
-    <t>effectiveTime.value</t>
-  </si>
-  <si>
     <t>"effectiveDateTime" : "2023-07-12T16:08:00.000Z",</t>
   </si>
   <si>
-    <t>If there is no value, current date time will be assigned.</t>
+    <r>
+      <t>First check the value from entryRelationship.observation.effectiveTime. 
+for</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Document.component.section.entry.observation.entryRelationship.observation.entryRelationship.observation.effectiveTime
+for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Document.component.section.entry.observation.entryRelationship.observation.effectiveTime
+If that is not valued, then use the same timestamp that is used in the Encounter FHIR resource:
+for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Document.componentOf.encompassingEncounter.effectiveTime
+for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Document.component.section.entry.encounter.effectiveTime
+If that is not valued, then use the same timestamp that is used in the meta.lastUpdated.</t>
+    </r>
   </si>
   <si>
     <t>performer</t>
@@ -2833,9 +2919,6 @@
     <t>type -&gt; coding -&gt; code</t>
   </si>
   <si>
-    <t>code.translation.code</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2939,7 +3022,7 @@
     </r>
   </si>
   <si>
-    <t>Tentatively mapped the code -&gt; translation -&gt; code</t>
+    <t>Get from the header variable `X-TechBD-Encounter-Type`</t>
   </si>
   <si>
     <t>type -&gt; coding -&gt; display</t>
@@ -4013,6 +4096,18 @@
   <si>
     <t>Document.component.structuredBody.component.
 section.entry.observation.value.displayName</t>
+  </si>
+  <si>
+    <t>Document.component.structuredBody.component.
+section.entry.observation.value.codeSystem</t>
+  </si>
+  <si>
+    <t>It will be added by checking the codeSystem.
+IF '2.16.840.1.113883.6.96' THEN http://snomed.info/sct
+IF '2.16.840.1.113883.6.1' THEN http://loinc.org
+IF '2.16.840.1.113883.6.12' THEN http://www.ama-assn.org/go/cpt
+IF '2.16.840.1.113883.6.285' THEN http://www.cms.gov/Medicare/Coding/HCPCSReleaseCodeSets
+IF '2.16.840.1.113883.6.90' THEN http://hl7.org/fhir/sid/icd-10-cm</t>
   </si>
   <si>
     <t>Document.component.structuredBody.component.
@@ -4662,7 +4757,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4670,7 +4765,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5186,6 +5281,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5194,9 +5292,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5745,8 +5840,8 @@
   <sheetPr/>
   <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -5867,7 +5962,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5879,7 +5974,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -5901,7 +5996,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -5909,145 +6004,145 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D9" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D18" s="11"/>
     </row>
@@ -6269,8 +6364,8 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6554,10 +6649,10 @@
       <c r="C26" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="8" t="s">
         <v>109</v>
       </c>
     </row>
@@ -6607,7 +6702,7 @@
       <c r="D31" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="8" t="s">
         <v>119</v>
       </c>
     </row>
@@ -6735,7 +6830,7 @@
       <c r="D44" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="16" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6743,33 +6838,31 @@
       <c r="B45" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="E45" s="16" t="s">
         <v>146</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="46" ht="195" spans="2:5">
       <c r="B46" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="E46" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>134</v>
@@ -6779,58 +6872,58 @@
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="4"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
       <c r="B50" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="4"/>
     </row>
     <row r="51" ht="150" spans="2:5">
       <c r="B51" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="16" t="s">
         <v>159</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="D52" s="9"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>134</v>
@@ -6840,90 +6933,90 @@
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="4"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="4"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="D57" s="9"/>
     </row>
     <row r="58" ht="180" spans="2:5">
       <c r="B58" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>141</v>
       </c>
       <c r="D58" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E58" s="16" t="s">
         <v>172</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="59" ht="75" spans="2:4">
       <c r="B59" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="60" ht="255" spans="2:5">
       <c r="B60" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="E60" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="61" ht="135" spans="2:5">
       <c r="B61" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D61" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="E61" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="62" ht="30" spans="2:3">
       <c r="B62" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>57</v>
@@ -6931,29 +7024,29 @@
     </row>
     <row r="63" ht="30" spans="2:3">
       <c r="B63" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="D64" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="65" ht="43" customHeight="1" spans="2:4">
       <c r="B65" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="D65" s="11"/>
     </row>
@@ -6975,7 +7068,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6983,7 +7076,7 @@
     <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="63.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="68.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="70.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="52.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="57.5714285714286" customWidth="1"/>
   </cols>
@@ -7018,7 +7111,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -7046,26 +7139,29 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" ht="60" spans="2:6">
+      <c r="B7" s="5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" ht="45" spans="2:6">
-      <c r="B7" s="5" t="s">
+      <c r="C7" t="s">
         <v>192</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>193</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
         <v>196</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -7079,24 +7175,30 @@
       <c r="B9" s="5" t="s">
         <v>199</v>
       </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
       <c r="E9" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" ht="225" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>198</v>
@@ -7104,7 +7206,7 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>198</v>
@@ -7112,10 +7214,10 @@
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>198</v>
@@ -7123,62 +7225,65 @@
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
-      <c r="B15" t="s">
-        <v>211</v>
+      <c r="B15" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C16" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>221</v>
+        <v>223</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>198</v>
@@ -7186,10 +7291,10 @@
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>198</v>
@@ -7197,23 +7302,23 @@
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D20" s="11" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" customFormat="1" ht="43" customHeight="1" spans="2:6">
+    <row r="21" customFormat="1" ht="60" customHeight="1" spans="2:6">
       <c r="B21" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="4"/>
@@ -7233,8 +7338,8 @@
   <sheetPr/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7272,12 +7377,12 @@
         <v>42</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1"/>
@@ -7285,7 +7390,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7297,7 +7402,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7319,7 +7424,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7333,191 +7438,189 @@
         <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" ht="375" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:3">
       <c r="B16" s="4" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C16" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:4">
       <c r="B19" s="5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" ht="315" spans="2:5">
       <c r="B20" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>264</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="C20" s="4"/>
       <c r="D20" t="s">
-        <v>265</v>
-      </c>
-      <c r="E20" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="21" ht="45" spans="2:4">
       <c r="B21" s="5" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D22" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D23" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" ht="46" customHeight="1" spans="2:4">
       <c r="B24" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D24" s="11"/>
     </row>
@@ -7537,7 +7640,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -7575,7 +7678,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7586,7 +7689,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7598,7 +7701,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7620,7 +7723,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7628,262 +7731,260 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" ht="105" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" ht="30" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="14" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" ht="120" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>289</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="E11" s="10" t="s">
         <v>291</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E12" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E14" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="60" spans="2:4">
       <c r="B15" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:3">
       <c r="B16" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" ht="60" spans="2:5">
       <c r="B23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" ht="75" spans="2:5">
       <c r="B24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" customFormat="1" ht="30" spans="2:5">
       <c r="B25" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="60" spans="2:5">
       <c r="B26" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:4">
       <c r="B28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D28" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B29" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D29" s="11"/>
     </row>
@@ -7947,7 +8048,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -7977,7 +8078,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7985,50 +8086,50 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="E8" s="15" t="s">
         <v>341</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>134</v>
@@ -8038,49 +8139,49 @@
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="1" ht="165" spans="2:5">
       <c r="B13" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="E13" s="15" t="s">
         <v>351</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>134</v>
@@ -8090,35 +8191,35 @@
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:5">
       <c r="B17" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" ht="30" spans="2:5">
       <c r="B18" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" ht="105" spans="2:5">
       <c r="B19" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -8130,7 +8231,7 @@
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -8139,13 +8240,13 @@
         <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F21" s="4"/>
     </row>
@@ -8154,7 +8255,7 @@
         <v>103</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -8165,20 +8266,20 @@
         <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="4"/>
@@ -8189,7 +8290,7 @@
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="4"/>
@@ -8200,7 +8301,7 @@
         <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="4"/>
@@ -8211,7 +8312,7 @@
         <v>93</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="4"/>
@@ -8222,7 +8323,7 @@
         <v>95</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="4"/>
@@ -8233,7 +8334,7 @@
         <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="4"/>
@@ -8241,21 +8342,21 @@
     </row>
     <row r="30" customFormat="1" spans="2:4">
       <c r="B30" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D30" s="11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B31" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D31" s="11"/>
     </row>
@@ -8273,8 +8374,8 @@
   <sheetPr/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8309,7 +8410,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8318,7 +8419,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8330,7 +8431,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -8352,7 +8453,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8366,157 +8467,160 @@
         <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="2:3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="16" ht="165" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C16" t="s">
-        <v>206</v>
+        <v>258</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D19" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D20" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D21" s="11" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D22" s="11"/>
     </row>
@@ -8573,7 +8677,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -8584,7 +8688,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8596,7 +8700,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -8618,7 +8722,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8626,128 +8730,128 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E9" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="2:5">
       <c r="B11" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" customFormat="1" ht="60" spans="2:4">
       <c r="B12" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" customFormat="1" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" customFormat="1" ht="45" spans="2:4">
       <c r="B14" s="5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C14" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" ht="60" spans="2:4">
       <c r="B15" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="2:4">
       <c r="B17" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B18" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D18" s="11"/>
     </row>

</xml_diff>

<commit_message>
docs: update CCDA to FHIR Conversion Spec document with consent resource and organization name changes for Epic and Medenat CCDA files #1367
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1" activeTab="7"/>
+    <workbookView windowWidth="23040" windowHeight="9120" tabRatio="709" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="443">
   <si>
     <t>FHIR Resource Element column</t>
   </si>
@@ -1744,6 +1744,55 @@
     <t>"http://shinny.org/us/ny/hrsn/Patient/&lt;patientResourceId&gt;"</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCDS, if the consent document (authorization.consent with code.code = '59284-0') is present, then a consent resource with provition.type = "permit" will be generated and if no consent document is present, then a consent resource with provition.type = "deny" will be generated.
+For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCDS, if there is an entry in the Procedures section with a consent question (`entry.observation.entryRelationship.observation with code = "105511-0"`) and answer (`entry.observation.entryRelationship.observation.value`), then if the `entry.observation.entryRelationship.observation.value.displayName = "Yes"` then, a consent resource with provition.type = "permit" will be generated. Otherwise, a consent resource with provition.type = "deny" will be generated.
+</t>
+    </r>
+  </si>
+  <si>
     <t>"Consent"</t>
   </si>
   <si>
@@ -2612,6 +2661,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>First check the value from entryRelationship.observation.effectiveTime. 
 for</t>
     </r>
@@ -4757,7 +4813,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4765,7 +4821,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5235,7 +5291,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5281,14 +5337,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5844,15 +5903,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.88571428571429" style="20"/>
-    <col min="2" max="2" width="35.2190476190476" customWidth="1"/>
+    <col min="1" max="1" width="8.88888888888889" style="21"/>
+    <col min="2" max="2" width="35.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="92.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="20">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -5863,7 +5922,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="20">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -5874,7 +5933,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="20">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -5885,10 +5944,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="20">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -5896,10 +5955,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="20">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
@@ -5921,12 +5980,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="46.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="46.5740740740741" customWidth="1"/>
+    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -5962,7 +6021,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5974,10 +6033,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="5" ht="30" spans="1:6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>18</v>
@@ -5991,34 +6050,34 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" ht="30" spans="2:6">
+    <row r="6" ht="28.8" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" ht="30" spans="2:5">
+    <row r="7" ht="28.8" spans="2:5">
       <c r="B7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="2:5">
+    <row r="8" ht="28.8" spans="2:5">
       <c r="B8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>150</v>
@@ -6026,104 +6085,104 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="10" ht="30" spans="2:5">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" ht="28.8" spans="2:5">
       <c r="B10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="11" ht="45" spans="2:5">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="11" ht="43.2" spans="2:5">
       <c r="B11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="12" ht="45" spans="2:5">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="12" ht="43.2" spans="2:5">
       <c r="B12" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="13" ht="45" spans="2:5">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="13" ht="43.2" spans="2:5">
       <c r="B13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="14" ht="45" spans="2:5">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="14" ht="43.2" spans="2:5">
       <c r="B14" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="15" ht="45" spans="2:5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="15" ht="43.2" spans="2:5">
       <c r="B15" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -6134,7 +6193,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
@@ -6142,7 +6201,7 @@
         <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D18" s="11"/>
     </row>
@@ -6165,14 +6224,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
     <col min="2" max="2" width="28.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="65.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="46.2190476190476" customWidth="1"/>
-    <col min="5" max="5" width="61.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="46.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="46.2222222222222" customWidth="1"/>
+    <col min="5" max="5" width="61.287037037037" customWidth="1"/>
+    <col min="6" max="6" width="46.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6221,7 +6280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="90" spans="2:4">
+    <row r="5" ht="86.4" spans="2:4">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -6258,7 +6317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" ht="30" spans="2:3">
+    <row r="9" ht="28.8" spans="2:3">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -6279,7 +6338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" ht="75" spans="2:3">
+    <row r="16" ht="72" spans="2:3">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -6295,7 +6354,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" ht="75" spans="2:5">
+    <row r="18" ht="72" spans="2:5">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -6306,7 +6365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" ht="45" spans="2:5">
+    <row r="19" ht="43.2" spans="2:5">
       <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
@@ -6317,7 +6376,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" ht="45" spans="2:5">
+    <row r="20" ht="43.2" spans="2:5">
       <c r="B20" t="s">
         <v>42</v>
       </c>
@@ -6328,7 +6387,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" ht="60" spans="2:5">
+    <row r="21" ht="43.2" spans="2:5">
       <c r="B21" t="s">
         <v>45</v>
       </c>
@@ -6339,14 +6398,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" ht="30" spans="2:5">
+    <row r="22" ht="28.8" spans="2:5">
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="20" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6368,14 +6427,14 @@
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="41.7809523809524" style="4" customWidth="1"/>
-    <col min="3" max="3" width="63.8857142857143" style="4" customWidth="1"/>
-    <col min="4" max="4" width="81.2857142857143" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.4285714285714" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="41.7777777777778" style="4" customWidth="1"/>
+    <col min="3" max="3" width="63.8888888888889" style="4" customWidth="1"/>
+    <col min="4" max="4" width="81.287037037037" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.4259259259259" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6443,7 +6502,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" ht="30" spans="2:4">
+    <row r="7" ht="28.8" spans="2:4">
       <c r="B7" s="4" t="s">
         <v>56</v>
       </c>
@@ -6454,7 +6513,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" ht="60" spans="2:6">
+    <row r="8" ht="57.6" spans="2:6">
       <c r="B8" s="4" t="s">
         <v>59</v>
       </c>
@@ -6513,7 +6572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" ht="60" spans="2:4">
+    <row r="13" ht="57.6" spans="2:4">
       <c r="B13" s="4" t="s">
         <v>74</v>
       </c>
@@ -6524,7 +6583,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" ht="30" spans="2:4">
+    <row r="14" ht="28.8" spans="2:4">
       <c r="B14" s="4" t="s">
         <v>77</v>
       </c>
@@ -6535,7 +6594,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" ht="30" spans="2:4">
+    <row r="15" spans="2:4">
       <c r="B15" s="4" t="s">
         <v>80</v>
       </c>
@@ -6557,7 +6616,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" ht="120" spans="2:4">
+    <row r="17" ht="115.2" spans="2:4">
       <c r="B17" s="4" t="s">
         <v>86</v>
       </c>
@@ -6631,7 +6690,7 @@
       </c>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" ht="75" spans="2:4">
+    <row r="25" ht="72" spans="2:4">
       <c r="B25" s="4" t="s">
         <v>103</v>
       </c>
@@ -6642,21 +6701,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" ht="45" spans="2:5">
+    <row r="26" ht="43.2" spans="2:5">
       <c r="B26" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" ht="30" spans="2:4">
+    <row r="27" spans="2:4">
       <c r="B27" s="4" t="s">
         <v>110</v>
       </c>
@@ -6674,7 +6733,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" ht="30" spans="2:4">
+    <row r="29" spans="2:4">
       <c r="B29" s="4" t="s">
         <v>114</v>
       </c>
@@ -6692,7 +6751,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" ht="45" spans="2:5">
+    <row r="31" ht="43.2" spans="2:5">
       <c r="B31" s="4" t="s">
         <v>106</v>
       </c>
@@ -6706,7 +6765,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" ht="30" spans="2:4">
+    <row r="32" spans="2:4">
       <c r="B32" s="4" t="s">
         <v>110</v>
       </c>
@@ -6724,7 +6783,7 @@
       </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" ht="30" spans="2:4">
+    <row r="34" spans="2:4">
       <c r="B34" s="4" t="s">
         <v>114</v>
       </c>
@@ -6753,7 +6812,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" ht="30" spans="2:4">
+    <row r="37" spans="2:4">
       <c r="B37" s="4" t="s">
         <v>126</v>
       </c>
@@ -6762,7 +6821,7 @@
       </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" ht="120" spans="2:5">
+    <row r="38" ht="115.2" spans="2:5">
       <c r="B38" s="4" t="s">
         <v>127</v>
       </c>
@@ -6773,7 +6832,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" ht="120" spans="2:5">
+    <row r="39" ht="115.2" spans="2:5">
       <c r="B39" s="4" t="s">
         <v>130</v>
       </c>
@@ -6820,7 +6879,7 @@
       </c>
       <c r="D43" s="9"/>
     </row>
-    <row r="44" ht="195" spans="2:5">
+    <row r="44" ht="187.2" spans="2:5">
       <c r="B44" s="6" t="s">
         <v>140</v>
       </c>
@@ -6830,11 +6889,11 @@
       <c r="D44" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" ht="195" spans="2:5">
+    <row r="45" ht="187.2" spans="2:5">
       <c r="B45" s="6" t="s">
         <v>144</v>
       </c>
@@ -6842,11 +6901,11 @@
       <c r="D45" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="46" ht="195" spans="2:5">
+    <row r="46" ht="187.2" spans="2:5">
       <c r="B46" s="6" t="s">
         <v>147</v>
       </c>
@@ -6900,7 +6959,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" ht="150" spans="2:5">
+    <row r="51" ht="144" spans="2:5">
       <c r="B51" s="9" t="s">
         <v>157</v>
       </c>
@@ -6908,7 +6967,7 @@
       <c r="D51" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="15" t="s">
         <v>159</v>
       </c>
     </row>
@@ -6970,7 +7029,7 @@
       </c>
       <c r="D57" s="9"/>
     </row>
-    <row r="58" ht="180" spans="2:5">
+    <row r="58" ht="172.8" spans="2:5">
       <c r="B58" s="9" t="s">
         <v>170</v>
       </c>
@@ -6980,11 +7039,11 @@
       <c r="D58" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="59" ht="75" spans="2:4">
+    <row r="59" ht="72" spans="2:4">
       <c r="B59" s="4" t="s">
         <v>173</v>
       </c>
@@ -6992,7 +7051,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" ht="255" spans="2:5">
+    <row r="60" ht="244.8" spans="2:5">
       <c r="B60" s="4" t="s">
         <v>175</v>
       </c>
@@ -7003,7 +7062,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" ht="135" spans="2:5">
+    <row r="61" ht="129.6" spans="2:5">
       <c r="B61" s="4" t="s">
         <v>178</v>
       </c>
@@ -7014,7 +7073,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" ht="30" spans="2:3">
+    <row r="62" ht="28.8" spans="2:3">
       <c r="B62" s="4" t="s">
         <v>181</v>
       </c>
@@ -7022,7 +7081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" ht="30" spans="2:3">
+    <row r="63" ht="28.8" spans="2:3">
       <c r="B63" s="4" t="s">
         <v>182</v>
       </c>
@@ -7067,18 +7126,18 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="63.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="70.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="52.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="57.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="27.8611111111111" customWidth="1"/>
+    <col min="3" max="3" width="63.4259259259259" customWidth="1"/>
+    <col min="4" max="4" width="70.712962962963" customWidth="1"/>
+    <col min="5" max="5" width="52.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="57.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7101,17 +7160,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" ht="74" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="B2" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -7139,165 +7203,165 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" ht="60" spans="2:6">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" ht="57.6" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" ht="120" spans="2:5">
+    <row r="8" ht="115.2" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:5">
       <c r="B9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="C9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" ht="225" spans="2:5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" ht="201.6" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="14" ht="30" spans="2:5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" ht="28.8" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" ht="45" spans="2:5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" ht="43.2" spans="2:5">
       <c r="B15" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="16" ht="45" spans="2:5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" ht="43.2" spans="2:5">
       <c r="B16" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" ht="45" spans="2:5">
+    <row r="17" ht="43.2" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" ht="45" spans="2:5">
+    <row r="18" ht="43.2" spans="2:5">
       <c r="B18" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" ht="60" spans="2:5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" ht="57.6" spans="2:5">
       <c r="B19" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -7308,7 +7372,7 @@
         <v>185</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -7318,14 +7382,15 @@
         <v>187</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7342,14 +7407,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="33.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.5740740740741" customWidth="1"/>
     <col min="3" max="3" width="49.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="56.552380952381" customWidth="1"/>
-    <col min="5" max="5" width="53.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="47.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="56.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="53.287037037037" customWidth="1"/>
+    <col min="6" max="6" width="47.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7377,12 +7442,12 @@
         <v>42</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="17"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1"/>
@@ -7390,7 +7455,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7402,7 +7467,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7419,12 +7484,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7438,170 +7503,170 @@
         <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" ht="375" spans="2:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" ht="316.8" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" ht="135" spans="2:5">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" ht="129.6" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="14" ht="105" spans="2:4">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" ht="100.8" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" ht="30" spans="2:3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" ht="28.8" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="2:3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" ht="28.8" spans="2:3">
       <c r="B16" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C16" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" ht="75" spans="2:4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" ht="57.6" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" ht="30" spans="2:3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" ht="45" spans="2:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" ht="43.2" spans="2:4">
       <c r="B19" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" ht="315" spans="2:5">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" ht="259.2" spans="2:5">
       <c r="B20" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" t="s">
-        <v>267</v>
-      </c>
-      <c r="E20" s="16" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="21" ht="45" spans="2:4">
+      <c r="E20" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" ht="43.2" spans="2:4">
       <c r="B21" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -7612,7 +7677,7 @@
         <v>185</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" ht="46" customHeight="1" spans="2:4">
@@ -7620,7 +7685,7 @@
         <v>187</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D24" s="11"/>
     </row>
@@ -7643,14 +7708,14 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="42.2857142857143" style="4" customWidth="1"/>
-    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="35.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="42.287037037037" style="4" customWidth="1"/>
+    <col min="4" max="4" width="73.5740740740741" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="51.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7678,7 +7743,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7689,7 +7754,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7701,7 +7766,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7718,12 +7783,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7731,241 +7796,240 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="8" ht="105" spans="2:5">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" ht="100.8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" ht="30" spans="2:5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" ht="28.8" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="11" ht="120" spans="2:5">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" ht="115.2" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>291</v>
+      </c>
       <c r="D11" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="E11" s="16" t="s">
         <v>292</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="15" customFormat="1" ht="60" spans="2:4">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" ht="57.6" spans="2:4">
       <c r="B15" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" customFormat="1" ht="30" spans="2:3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" ht="28.8" spans="2:3">
       <c r="B16" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" ht="60" spans="2:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" ht="57.6" spans="2:4">
       <c r="B17" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" ht="45" spans="2:5">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" ht="28.8" spans="2:5">
       <c r="B19" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="22" ht="30" spans="2:5">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" ht="28.8" spans="2:5">
       <c r="B22" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="23" ht="60" spans="2:5">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" ht="57.6" spans="2:5">
       <c r="B23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="24" ht="75" spans="2:5">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" ht="72" spans="2:5">
       <c r="B24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="25" customFormat="1" ht="30" spans="2:5">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" ht="28.8" spans="2:5">
       <c r="B25" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="26" customFormat="1" ht="60" spans="2:5">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" ht="57.6" spans="2:5">
       <c r="B26" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="27" customFormat="1" ht="30" spans="2:5">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" ht="28.8" spans="2:5">
       <c r="B27" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:4">
@@ -7976,7 +8040,7 @@
         <v>185</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -7984,7 +8048,7 @@
         <v>187</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D29" s="11"/>
     </row>
@@ -8008,14 +8072,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
     <col min="2" max="2" width="27.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="50.8857142857143" customWidth="1"/>
-    <col min="4" max="4" width="72.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="46.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="45.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="50.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="72.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="46.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="45.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -8048,7 +8112,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -8073,12 +8137,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8086,50 +8150,50 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="8" ht="165" spans="2:5">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" ht="158.4" spans="2:5">
       <c r="B8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="E8" s="16" t="s">
         <v>342</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" ht="30" spans="2:5">
+    <row r="10" ht="28.8" spans="2:5">
       <c r="B10" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" ht="30" spans="2:5">
+    <row r="11" ht="28.8" spans="2:5">
       <c r="B11" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>134</v>
@@ -8137,51 +8201,51 @@
       <c r="D11" s="9"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" ht="30" spans="2:5">
+    <row r="12" ht="28.8" spans="2:5">
       <c r="B12" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" customFormat="1" ht="165" spans="2:5">
+    <row r="13" customFormat="1" ht="158.4" spans="2:5">
       <c r="B13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="E13" s="16" t="s">
         <v>352</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" customFormat="1" ht="30" spans="2:5">
+    <row r="15" customFormat="1" ht="28.8" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" customFormat="1" ht="30" spans="2:5">
+    <row r="16" customFormat="1" ht="28.8" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>134</v>
@@ -8189,37 +8253,37 @@
       <c r="D16" s="9"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" customFormat="1" ht="30" spans="2:5">
+    <row r="17" customFormat="1" ht="28.8" spans="2:5">
       <c r="B17" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" ht="30" spans="2:5">
+    <row r="18" ht="28.8" spans="2:5">
       <c r="B18" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" ht="105" spans="2:5">
+    <row r="19" ht="100.8" spans="2:5">
       <c r="B19" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -8231,110 +8295,110 @@
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" customFormat="1" ht="180" spans="2:6">
+    <row r="21" customFormat="1" ht="172.8" spans="2:6">
       <c r="B21" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" customFormat="1" ht="30" spans="2:6">
+    <row r="22" customFormat="1" ht="28.8" spans="2:6">
       <c r="B22" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" customFormat="1" ht="135" spans="2:6">
+    <row r="23" customFormat="1" ht="129.6" spans="2:6">
       <c r="B23" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" customFormat="1" ht="30" spans="2:6">
+    <row r="24" customFormat="1" ht="28.8" spans="2:6">
       <c r="B24" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" customFormat="1" ht="30" spans="2:6">
+    <row r="25" customFormat="1" ht="28.8" spans="2:6">
       <c r="B25" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" customFormat="1" ht="30" spans="2:6">
+    <row r="26" customFormat="1" ht="28.8" spans="2:6">
       <c r="B26" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" customFormat="1" ht="30" spans="2:6">
+    <row r="27" customFormat="1" ht="28.8" spans="2:6">
       <c r="B27" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" customFormat="1" ht="30" spans="2:6">
+    <row r="28" customFormat="1" ht="28.8" spans="2:6">
       <c r="B28" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" customFormat="1" ht="30" spans="2:6">
+    <row r="29" customFormat="1" ht="28.8" spans="2:6">
       <c r="B29" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="4"/>
@@ -8348,7 +8412,7 @@
         <v>185</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -8356,7 +8420,7 @@
         <v>187</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D31" s="11"/>
     </row>
@@ -8374,16 +8438,16 @@
   <sheetPr/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
-    <col min="3" max="3" width="46.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="46.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -8408,9 +8472,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="45" spans="1:1">
+    <row r="2" ht="43.2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8419,7 +8483,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8431,10 +8495,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="5" ht="30" spans="1:6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>18</v>
@@ -8448,12 +8512,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" ht="30" spans="2:6">
+    <row r="6" ht="28.8" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8467,141 +8531,141 @@
         <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" ht="30" spans="2:5">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" ht="28.8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" ht="390" spans="2:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" ht="331.2" spans="2:5">
       <c r="B9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="10" ht="135" spans="2:4">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="10" ht="129.6" spans="2:4">
       <c r="B10" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="11" ht="30" spans="2:3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" ht="28.8" spans="2:3">
       <c r="B11" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="13" ht="30" spans="2:3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="13" ht="28.8" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="14" ht="105" spans="2:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" ht="100.8" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="15" ht="30" spans="2:3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="15" ht="28.8" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="16" ht="165" spans="2:5">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" ht="158.4" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="E16" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="17" ht="75" spans="2:4">
+      <c r="E16" s="15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="17" ht="57.6" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" ht="30" spans="2:3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" ht="28.8" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" ht="30" spans="2:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" ht="28.8" spans="2:4">
       <c r="B19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D20" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -8612,7 +8676,7 @@
         <v>185</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
@@ -8620,7 +8684,7 @@
         <v>187</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D22" s="11"/>
     </row>
@@ -8642,14 +8706,14 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="42.2857142857143" style="4" customWidth="1"/>
-    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="35.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="42.287037037037" style="4" customWidth="1"/>
+    <col min="4" max="4" width="73.5740740740741" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="51.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -8677,7 +8741,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -8688,7 +8752,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8700,7 +8764,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -8717,12 +8781,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
+    <row r="6" customFormat="1" ht="28.8" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8730,109 +8794,109 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="8" ht="120" spans="2:5">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" ht="115.2" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="2:5">
       <c r="B11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E11" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" ht="60" spans="2:4">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" ht="57.6" spans="2:4">
       <c r="B12" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" customFormat="1" ht="30" spans="2:3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" ht="28.8" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" customFormat="1" ht="45" spans="2:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" ht="43.2" spans="2:4">
       <c r="B14" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="15" ht="60" spans="2:4">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="15" ht="57.6" spans="2:4">
       <c r="B15" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="2:4">
@@ -8843,7 +8907,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -8851,7 +8915,7 @@
         <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D18" s="11"/>
     </row>

</xml_diff>

<commit_message>
docs: update CCDA to FHIR conversion spec with lattest changes made to consent, observation and encounter resources #1604
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120" tabRatio="709" firstSheet="1" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="446">
   <si>
     <t>FHIR Resource Element column</t>
   </si>
@@ -1745,6 +1745,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">For </t>
     </r>
     <r>
@@ -1794,6 +1801,9 @@
   </si>
   <si>
     <t>"Consent"</t>
+  </si>
+  <si>
+    <t>Unique 64-character SHA-256 Consent resource ID is generated using the Patient MRN, Patient CIN, current timestamp, and the text content of the resource (if present) in the CCDA XML file.</t>
   </si>
   <si>
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/shinny-Consent"</t>
@@ -2568,6 +2578,21 @@
     </r>
   </si>
   <si>
+    <t>If `entryRelationship.observation.value.translation.code` is one of "X-SDOH-FLO-1570000066-Patient-unable-to-answer" or "X-SDOH-FLO-1570000066-Patient-declined" then, `dataAbsentReason` element will be added instead of 'valueCodeableConcept'.  
+"dataAbsentReason": {
+                "coding": [
+                    {
+                        "system": "http://terminology.hl7.org/CodeSystem/data-absent-reason",
+                        "code": "asked-declined",
+                        "display": "Asked But Declined"
+                    }
+                ]
+            }
+The 'code' mapping for dataAbsebtReason' is as follows:
+"X-SDOH-FLO-1570000066-Patient-unable-to-answer" -&gt; "asked-unknown"
+"X-SDOH-FLO-1570000066-Patient-declined" -&gt; "asked-declined"</t>
+  </si>
+  <si>
     <t>valueCodeableConcept -&gt; coding -&gt; display</t>
   </si>
   <si>
@@ -2858,6 +2883,54 @@
   </si>
   <si>
     <t>"id" : "EncounterExample",</t>
+  </si>
+  <si>
+    <r>
+      <t>If the encompassingEncounter section is present in the CCDA XML file (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCDA files), a 64-character SHA-256 Encounter resource ID is generated from the Patient MRN, Patient CIN, effectiveTime, and the text content of the encompassingEncounter section (if any).
+Otherwise (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCDA files), the ID is generated from the Patient MRN, Patient CIN, effectiveTime, and the text content of the first occurrence of the encounter section (if any).</t>
+    </r>
   </si>
   <si>
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/shinny-encounter"</t>
@@ -3699,10 +3772,41 @@
     <t>name</t>
   </si>
   <si>
-    <t>Document.author.assignedAuthor.representedOrganization.name</t>
-  </si>
-  <si>
     <t>"name" : "Care Ridge SCN",</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For Epic CCD files, Document.author.assignedAuthor.representedOrganization.name.
+For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCD files, encounter.participant.participantRole.playingEntity.name with participant typeCode="LOC" and participantRole classCode="SDLOC".</t>
+    </r>
   </si>
   <si>
     <t>type -&gt; code</t>
@@ -4813,7 +4917,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4821,7 +4925,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4835,7 +4939,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4845,6 +4949,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5167,7 +5277,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5191,16 +5301,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -5209,89 +5319,89 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5340,14 +5450,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5903,15 +6019,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.88888888888889" style="21"/>
-    <col min="2" max="2" width="35.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="8.88571428571429" style="23"/>
+    <col min="2" max="2" width="35.2190476190476" customWidth="1"/>
     <col min="3" max="3" width="92.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="21">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -5922,7 +6038,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="21">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -5933,7 +6049,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="21">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -5944,10 +6060,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="21">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -5955,10 +6071,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="21">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
@@ -5980,12 +6096,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="46.5740740740741" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="46.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -6021,7 +6137,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6033,10 +6149,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>18</v>
@@ -6050,34 +6166,34 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" ht="28.8" spans="2:6">
+    <row r="6" ht="30" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" ht="28.8" spans="2:5">
+    <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" ht="28.8" spans="2:5">
+    <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>150</v>
@@ -6085,104 +6201,104 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="D9" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="10" ht="28.8" spans="2:5">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="11" ht="43.2" spans="2:5">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="12" ht="43.2" spans="2:5">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="13" ht="43.2" spans="2:5">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="14" ht="43.2" spans="2:5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="15" ht="43.2" spans="2:5">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -6193,7 +6309,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
@@ -6201,7 +6317,7 @@
         <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D18" s="11"/>
     </row>
@@ -6220,18 +6336,18 @@
   <sheetPr/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="28.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="65.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="46.2222222222222" customWidth="1"/>
-    <col min="5" max="5" width="61.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="46.287037037037" customWidth="1"/>
+    <col min="4" max="4" width="46.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="61.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="46.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6280,7 +6396,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="86.4" spans="2:4">
+    <row r="5" ht="90" spans="2:4">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -6317,7 +6433,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" ht="28.8" spans="2:3">
+    <row r="9" ht="30" spans="2:3">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -6338,7 +6454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" ht="72" spans="2:3">
+    <row r="16" ht="75" spans="2:3">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -6354,7 +6470,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" ht="72" spans="2:5">
+    <row r="18" ht="75" spans="2:5">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -6365,7 +6481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" ht="43.2" spans="2:5">
+    <row r="19" ht="45" spans="2:5">
       <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
@@ -6376,7 +6492,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" ht="43.2" spans="2:5">
+    <row r="20" ht="45" spans="2:5">
       <c r="B20" t="s">
         <v>42</v>
       </c>
@@ -6387,7 +6503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" ht="43.2" spans="2:5">
+    <row r="21" ht="60" spans="2:5">
       <c r="B21" t="s">
         <v>45</v>
       </c>
@@ -6398,14 +6514,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" ht="28.8" spans="2:5">
+    <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="22" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6423,18 +6539,18 @@
   <sheetPr/>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="41.7777777777778" style="4" customWidth="1"/>
-    <col min="3" max="3" width="63.8888888888889" style="4" customWidth="1"/>
-    <col min="4" max="4" width="81.287037037037" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.4259259259259" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="41.7809523809524" style="4" customWidth="1"/>
+    <col min="3" max="3" width="63.8857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="81.2857142857143" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.4285714285714" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -6502,7 +6618,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" ht="28.8" spans="2:4">
+    <row r="7" ht="30" spans="2:4">
       <c r="B7" s="4" t="s">
         <v>56</v>
       </c>
@@ -6513,7 +6629,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" ht="57.6" spans="2:6">
+    <row r="8" ht="60" spans="2:6">
       <c r="B8" s="4" t="s">
         <v>59</v>
       </c>
@@ -6572,7 +6688,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" ht="57.6" spans="2:4">
+    <row r="13" ht="60" spans="2:4">
       <c r="B13" s="4" t="s">
         <v>74</v>
       </c>
@@ -6583,7 +6699,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" ht="28.8" spans="2:4">
+    <row r="14" ht="30" spans="2:4">
       <c r="B14" s="4" t="s">
         <v>77</v>
       </c>
@@ -6594,7 +6710,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" ht="30" spans="2:4">
       <c r="B15" s="4" t="s">
         <v>80</v>
       </c>
@@ -6616,7 +6732,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" ht="115.2" spans="2:4">
+    <row r="17" ht="120" spans="2:4">
       <c r="B17" s="4" t="s">
         <v>86</v>
       </c>
@@ -6690,7 +6806,7 @@
       </c>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" ht="72" spans="2:4">
+    <row r="25" ht="75" spans="2:4">
       <c r="B25" s="4" t="s">
         <v>103</v>
       </c>
@@ -6701,21 +6817,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" ht="43.2" spans="2:5">
+    <row r="26" ht="45" spans="2:5">
       <c r="B26" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" ht="30" spans="2:4">
       <c r="B27" s="4" t="s">
         <v>110</v>
       </c>
@@ -6733,7 +6849,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" ht="30" spans="2:4">
       <c r="B29" s="4" t="s">
         <v>114</v>
       </c>
@@ -6751,7 +6867,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" ht="43.2" spans="2:5">
+    <row r="31" ht="45" spans="2:5">
       <c r="B31" s="4" t="s">
         <v>106</v>
       </c>
@@ -6765,7 +6881,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" ht="30" spans="2:4">
       <c r="B32" s="4" t="s">
         <v>110</v>
       </c>
@@ -6783,7 +6899,7 @@
       </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" ht="30" spans="2:4">
       <c r="B34" s="4" t="s">
         <v>114</v>
       </c>
@@ -6812,7 +6928,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" ht="30" spans="2:4">
       <c r="B37" s="4" t="s">
         <v>126</v>
       </c>
@@ -6821,7 +6937,7 @@
       </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" ht="115.2" spans="2:5">
+    <row r="38" ht="120" spans="2:5">
       <c r="B38" s="4" t="s">
         <v>127</v>
       </c>
@@ -6832,7 +6948,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" ht="115.2" spans="2:5">
+    <row r="39" ht="120" spans="2:5">
       <c r="B39" s="4" t="s">
         <v>130</v>
       </c>
@@ -6879,7 +6995,7 @@
       </c>
       <c r="D43" s="9"/>
     </row>
-    <row r="44" ht="187.2" spans="2:5">
+    <row r="44" ht="195" spans="2:5">
       <c r="B44" s="6" t="s">
         <v>140</v>
       </c>
@@ -6893,7 +7009,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" ht="187.2" spans="2:5">
+    <row r="45" ht="195" spans="2:5">
       <c r="B45" s="6" t="s">
         <v>144</v>
       </c>
@@ -6905,7 +7021,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" ht="187.2" spans="2:5">
+    <row r="46" ht="195" spans="2:5">
       <c r="B46" s="6" t="s">
         <v>147</v>
       </c>
@@ -6959,7 +7075,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" ht="144" spans="2:5">
+    <row r="51" ht="150" spans="2:5">
       <c r="B51" s="9" t="s">
         <v>157</v>
       </c>
@@ -7029,7 +7145,7 @@
       </c>
       <c r="D57" s="9"/>
     </row>
-    <row r="58" ht="172.8" spans="2:5">
+    <row r="58" ht="180" spans="2:5">
       <c r="B58" s="9" t="s">
         <v>170</v>
       </c>
@@ -7043,7 +7159,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" ht="72" spans="2:4">
+    <row r="59" ht="75" spans="2:4">
       <c r="B59" s="4" t="s">
         <v>173</v>
       </c>
@@ -7051,7 +7167,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" ht="244.8" spans="2:5">
+    <row r="60" ht="255" spans="2:5">
       <c r="B60" s="4" t="s">
         <v>175</v>
       </c>
@@ -7062,7 +7178,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" ht="129.6" spans="2:5">
+    <row r="61" ht="135" spans="2:5">
       <c r="B61" s="4" t="s">
         <v>178</v>
       </c>
@@ -7073,7 +7189,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" ht="28.8" spans="2:3">
+    <row r="62" ht="30" spans="2:3">
       <c r="B62" s="4" t="s">
         <v>181</v>
       </c>
@@ -7081,7 +7197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" ht="28.8" spans="2:3">
+    <row r="63" ht="30" spans="2:3">
       <c r="B63" s="4" t="s">
         <v>182</v>
       </c>
@@ -7124,20 +7240,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="27.8611111111111" customWidth="1"/>
-    <col min="3" max="3" width="63.4259259259259" customWidth="1"/>
-    <col min="4" max="4" width="70.712962962963" customWidth="1"/>
-    <col min="5" max="5" width="52.4259259259259" customWidth="1"/>
-    <col min="6" max="6" width="57.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="63.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="70.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="52.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="57.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7164,11 +7280,11 @@
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="4" t="s">
@@ -7178,14 +7294,18 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" ht="60" spans="2:7">
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
@@ -7203,165 +7323,165 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" ht="57.6" spans="2:6">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" ht="60" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" ht="115.2" spans="2:5">
+    <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:5">
       <c r="B9" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="C9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" ht="201.6" spans="2:5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" ht="225" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" ht="28.8" spans="2:5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" ht="43.2" spans="2:5">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" ht="45" spans="2:5">
       <c r="B15" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" ht="43.2" spans="2:5">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" ht="45" spans="2:5">
       <c r="B16" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" ht="43.2" spans="2:5">
+    <row r="17" ht="45" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" ht="43.2" spans="2:5">
+    <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" ht="57.6" spans="2:5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" ht="60" spans="2:5">
       <c r="B19" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -7372,7 +7492,7 @@
         <v>185</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -7382,7 +7502,7 @@
         <v>187</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="4"/>
@@ -7403,18 +7523,18 @@
   <sheetPr/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="33.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="49.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="56.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="53.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="47.5740740740741" customWidth="1"/>
+    <col min="4" max="4" width="56.552380952381" customWidth="1"/>
+    <col min="5" max="5" width="53.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="47.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7442,12 +7562,12 @@
         <v>42</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1"/>
@@ -7455,7 +7575,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7467,7 +7587,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7484,12 +7604,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7503,170 +7623,173 @@
         <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" ht="316.8" spans="2:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" ht="375" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="10" ht="129.6" spans="2:5">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" ht="135" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="14" ht="100.8" spans="2:4">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" ht="390" spans="2:6">
       <c r="B14" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" ht="28.8" spans="2:3">
+        <v>257</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="16" ht="28.8" spans="2:3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" ht="30" spans="2:3">
       <c r="B16" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" ht="57.6" spans="2:4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" ht="43.2" spans="2:4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" ht="45" spans="2:4">
       <c r="B19" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" ht="259.2" spans="2:5">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" ht="315" spans="2:5">
       <c r="B20" s="5" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="21" ht="43.2" spans="2:4">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" ht="45" spans="2:4">
       <c r="B21" s="5" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -7677,7 +7800,7 @@
         <v>185</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" ht="46" customHeight="1" spans="2:4">
@@ -7685,7 +7808,7 @@
         <v>187</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D24" s="11"/>
     </row>
@@ -7705,17 +7828,17 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="35.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="42.287037037037" style="4" customWidth="1"/>
-    <col min="4" max="4" width="73.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="42.2857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.712962962963" customWidth="1"/>
+    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -7743,7 +7866,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7754,10 +7877,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" ht="135" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -7766,7 +7889,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>279</v>
+        <v>281</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7783,12 +7909,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7796,240 +7922,240 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D7" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" ht="100.8" spans="2:5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" ht="105" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="9" ht="28.8" spans="2:5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" ht="30" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="14" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" ht="115.2" spans="2:5">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" ht="120" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>293</v>
+        <v>295</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E12" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E14" t="s">
         <v>299</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="E14" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="15" customFormat="1" ht="57.6" spans="2:4">
+    </row>
+    <row r="15" customFormat="1" ht="60" spans="2:4">
       <c r="B15" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" customFormat="1" ht="28.8" spans="2:3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" ht="30" spans="2:3">
       <c r="B16" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" ht="57.6" spans="2:4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="19" ht="28.8" spans="2:5">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="22" ht="28.8" spans="2:5">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="23" ht="57.6" spans="2:5">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" ht="60" spans="2:5">
       <c r="B23" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" ht="72" spans="2:5">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" ht="75" spans="2:5">
       <c r="B24" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="25" customFormat="1" ht="28.8" spans="2:5">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" ht="30" spans="2:5">
       <c r="B25" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" customFormat="1" ht="57.6" spans="2:5">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" ht="60" spans="2:5">
       <c r="B26" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="27" customFormat="1" ht="28.8" spans="2:5">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:4">
@@ -8040,7 +8166,7 @@
         <v>185</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -8048,7 +8174,7 @@
         <v>187</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D29" s="11"/>
     </row>
@@ -8072,14 +8198,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="50.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="72.8611111111111" customWidth="1"/>
-    <col min="5" max="5" width="46.4259259259259" customWidth="1"/>
-    <col min="6" max="6" width="45.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="50.8857142857143" customWidth="1"/>
+    <col min="4" max="4" width="72.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="46.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="45.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -8112,7 +8238,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -8137,12 +8263,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8150,50 +8276,50 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D7" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" ht="158.4" spans="2:5">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" ht="28.8" spans="2:5">
+    <row r="10" ht="30" spans="2:5">
       <c r="B10" s="4" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" ht="28.8" spans="2:5">
+    <row r="11" ht="30" spans="2:5">
       <c r="B11" s="4" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>134</v>
@@ -8201,51 +8327,51 @@
       <c r="D11" s="9"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" ht="28.8" spans="2:5">
+    <row r="12" ht="30" spans="2:5">
       <c r="B12" s="4" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" customFormat="1" ht="158.4" spans="2:5">
+    <row r="13" customFormat="1" ht="165" spans="2:5">
       <c r="B13" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" customFormat="1" ht="28.8" spans="2:5">
+    <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" customFormat="1" ht="28.8" spans="2:5">
+    <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>134</v>
@@ -8253,37 +8379,37 @@
       <c r="D16" s="9"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" customFormat="1" ht="28.8" spans="2:5">
+    <row r="17" customFormat="1" ht="30" spans="2:5">
       <c r="B17" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" ht="28.8" spans="2:5">
+    <row r="18" ht="120" spans="2:5">
       <c r="B18" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>362</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" ht="100.8" spans="2:5">
+        <v>365</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" ht="105" spans="2:5">
       <c r="B19" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
@@ -8295,110 +8421,110 @@
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" customFormat="1" ht="172.8" spans="2:6">
+    <row r="21" customFormat="1" ht="180" spans="2:6">
       <c r="B21" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" customFormat="1" ht="28.8" spans="2:6">
+    <row r="22" customFormat="1" ht="30" spans="2:6">
       <c r="B22" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" customFormat="1" ht="129.6" spans="2:6">
+    <row r="23" customFormat="1" ht="135" spans="2:6">
       <c r="B23" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" customFormat="1" ht="28.8" spans="2:6">
+    <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="4" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" customFormat="1" ht="28.8" spans="2:6">
+    <row r="25" customFormat="1" ht="30" spans="2:6">
       <c r="B25" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" customFormat="1" ht="28.8" spans="2:6">
+    <row r="26" customFormat="1" ht="30" spans="2:6">
       <c r="B26" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" customFormat="1" ht="28.8" spans="2:6">
+    <row r="27" customFormat="1" ht="30" spans="2:6">
       <c r="B27" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" customFormat="1" ht="28.8" spans="2:6">
+    <row r="28" customFormat="1" ht="30" spans="2:6">
       <c r="B28" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" customFormat="1" ht="28.8" spans="2:6">
+    <row r="29" customFormat="1" ht="30" spans="2:6">
       <c r="B29" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="4"/>
@@ -8412,7 +8538,7 @@
         <v>185</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -8420,7 +8546,7 @@
         <v>187</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D31" s="11"/>
     </row>
@@ -8438,16 +8564,16 @@
   <sheetPr/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="46.8611111111111" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.8857142857143" customWidth="1"/>
+    <col min="3" max="3" width="46.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
     <col min="5" max="5" width="41.3333333333333" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
@@ -8472,9 +8598,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="43.2" spans="1:1">
+    <row r="2" ht="45" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8483,7 +8609,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8495,10 +8621,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>18</v>
@@ -8512,12 +8638,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" ht="28.8" spans="2:6">
+    <row r="6" ht="30" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8531,141 +8657,141 @@
         <v>58</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" ht="28.8" spans="2:5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" ht="331.2" spans="2:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="10" ht="129.6" spans="2:4">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" ht="135" spans="2:4">
       <c r="B10" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" ht="28.8" spans="2:3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" ht="30" spans="2:3">
       <c r="B11" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="13" ht="28.8" spans="2:3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="14" ht="100.8" spans="2:4">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" ht="105" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="15" ht="28.8" spans="2:3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="16" ht="158.4" spans="2:5">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="16" ht="165" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="17" ht="57.6" spans="2:4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" ht="28.8" spans="2:3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" ht="28.8" spans="2:4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D20" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -8676,7 +8802,7 @@
         <v>185</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
@@ -8684,7 +8810,7 @@
         <v>187</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D22" s="11"/>
     </row>
@@ -8706,14 +8832,14 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="35.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="42.287037037037" style="4" customWidth="1"/>
-    <col min="4" max="4" width="73.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="42.2857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.712962962963" customWidth="1"/>
+    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -8741,7 +8867,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -8752,7 +8878,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8764,7 +8890,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -8781,12 +8907,12 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="1" ht="28.8" spans="2:6">
+    <row r="6" customFormat="1" ht="30" spans="2:6">
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8794,109 +8920,109 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D7" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" ht="115.2" spans="2:5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="2:5">
       <c r="B11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E11" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" ht="57.6" spans="2:4">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" ht="60" spans="2:4">
       <c r="B12" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="13" customFormat="1" ht="28.8" spans="2:3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" customFormat="1" ht="43.2" spans="2:4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" ht="45" spans="2:4">
       <c r="B14" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C14" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="15" ht="57.6" spans="2:4">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" ht="60" spans="2:4">
       <c r="B15" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="2:4">
@@ -8907,7 +9033,7 @@
         <v>185</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -8915,7 +9041,7 @@
         <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D18" s="11"/>
     </row>

</xml_diff>

<commit_message>
docs: add observation grouper resource details
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Patient" sheetId="1" r:id="rId3"/>
     <sheet name="Consent" sheetId="3" r:id="rId4"/>
     <sheet name="Observation" sheetId="4" r:id="rId5"/>
-    <sheet name="Encounter" sheetId="5" r:id="rId6"/>
-    <sheet name="Organization" sheetId="6" r:id="rId7"/>
-    <sheet name="Sexual Orientation" sheetId="8" r:id="rId8"/>
-    <sheet name="Procedure" sheetId="13" r:id="rId9"/>
-    <sheet name="Questionnaire" sheetId="9" r:id="rId10"/>
+    <sheet name="Observation Grouper" sheetId="14" r:id="rId6"/>
+    <sheet name="Encounter" sheetId="5" r:id="rId7"/>
+    <sheet name="Organization" sheetId="6" r:id="rId8"/>
+    <sheet name="Sexual Orientation" sheetId="8" r:id="rId9"/>
+    <sheet name="Procedure" sheetId="13" r:id="rId10"/>
+    <sheet name="Questionnaire" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="454">
   <si>
     <t>FHIR Resource Element column</t>
   </si>
@@ -493,43 +494,7 @@
     <t>Path to get the resource</t>
   </si>
   <si>
-    <t>Procedure</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Document.component.structuredBody.component.section[code[@code='</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>47519-4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']]/.entry.procedure</t>
-    </r>
-  </si>
-  <si>
-    <t>It is done only for Medent CCDA files.</t>
+    <t>Observation (Observation Grouper)</t>
   </si>
   <si>
     <t>"Patient"</t>
@@ -2824,6 +2789,187 @@
     <t>"http://shinny.org/us/ny/hrsn/Observation/&lt;observationResourceId&gt;"</t>
   </si>
   <si>
+    <t>Tentatively mapped to the fixed value, "en"</t>
+  </si>
+  <si>
+    <t>It will list the categories present in all the observations.</t>
+  </si>
+  <si>
+    <t>"category": [
+                    {
+                        "coding": [
+                            {
+                                "system": "http://hl7.org/fhir/us/sdoh-clinicalcare/CodeSystem/SDOHCC-CodeSystemTemporaryCodes",
+                                "code": "financial-insecurity",
+                                "display": "Financial Insecurity"
+                            },
+                            {
+                                "system": "http://hl7.org/fhir/us/sdoh-clinicalcare/CodeSystem/SDOHCC-CodeSystemTemporaryCodes",
+                                "code": "sdoh-category-unspecified",
+                                "display": "SDOH Category Unspecified"
+                            }
+                        ]
+                    },
+                    {
+                        "coding": [
+                            {
+                                "system": "http://terminology.hl7.org/CodeSystem/observation-category",
+                                "code": "social-history"
+                            }
+                        ]
+                    },
+                    {
+                        "coding": [
+                            {
+                                "system": "http://terminology.hl7.org/CodeSystem/observation-category",
+                                "code": "survey"
+                            }
+                        ]
+                    }
+                ],</t>
+  </si>
+  <si>
+    <r>
+      <t>"code": {
+                    "coding": [
+                        {
+                            "system": "http://loinc.org",
+                            "code": "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>96777-8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",
+                            "display": "Accountable health communities (AHC) health-related social needs screening (HRSN) tool"
+                        }
+                    ]
+                },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> files, "96777-8".
+For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> files, if any value is set in the header variable, `</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X-TechBD-Screening-Code`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, other wise, "100698-0" as the default value.  
+If the screening code is one of ('NYSAHCHRSN', 'NYS-AHC-HRSN'), then the constant value is given: 
+{
+   "code": "100698-0",
+    "system": "http://loinc.org",
+    "display": "Social Determinants of Health screening report Document"
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>Tentatively mapped to the current date time.</t>
+  </si>
+  <si>
+    <t>hasMember</t>
+  </si>
+  <si>
+    <t>"hasMember": [
+          {
+            "reference": "Observation/&lt;observation.id&gt;"
+          },
+          {
+             "reference": "Observation/&lt;observation.id&gt;"
+          },
+          {
+             "reference": "Observation/&lt;observation.id&gt;"
+          }
+        ]</t>
+  </si>
+  <si>
+    <t>Included references to all the Observation resources.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2886,6 +3032,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>If the encompassingEncounter section is present in the CCDA XML file (</t>
     </r>
     <r>
@@ -4280,8 +4433,16 @@
     }</t>
   </si>
   <si>
-    <r>
-      <rPr>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is now removed from the FHIR bundle.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
         <sz val="11"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -4293,6 +4454,7 @@
     <r>
       <rPr>
         <b/>
+        <strike/>
         <sz val="11"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -4303,6 +4465,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -4314,6 +4477,7 @@
     <r>
       <rPr>
         <b/>
+        <strike/>
         <sz val="11"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -4324,6 +4488,7 @@
     </r>
     <r>
       <rPr>
+        <strike/>
         <sz val="11"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
@@ -4713,7 +4878,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4915,9 +5080,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.25"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4931,9 +5111,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <strike/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5456,7 +5645,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6093,6 +6282,238 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="42.2857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="53" customWidth="1"/>
+    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="34" customHeight="1" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" customFormat="1" spans="2:3">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" customFormat="1" ht="30" spans="2:6">
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>415</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" ht="120" spans="2:5">
+      <c r="B8" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E9" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="2:5">
+      <c r="B11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" ht="60" spans="2:4">
+      <c r="B12" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" ht="30" spans="2:3">
+      <c r="B13" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" ht="45" spans="2:4">
+      <c r="B14" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" ht="60" spans="2:4">
+      <c r="B15" t="s">
+        <v>418</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="2:4">
+      <c r="B17" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
+      <c r="B18" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D18" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D17:D18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6137,7 +6558,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6149,7 +6570,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -6158,11 +6579,11 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -6171,7 +6592,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -6179,145 +6600,145 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="D9" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" ht="45" customHeight="1" spans="2:4">
       <c r="B18" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D18" s="11"/>
     </row>
@@ -6336,8 +6757,8 @@
   <sheetPr/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6515,15 +6936,11 @@
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
-      <c r="B22" t="s">
+      <c r="B22" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>50</v>
-      </c>
+      <c r="C22"/>
+      <c r="E22" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6584,7 +7001,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -6595,7 +7012,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6604,10 +7021,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -6615,613 +7032,613 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" ht="30" spans="2:4">
       <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" ht="60" spans="2:6">
       <c r="B8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="F8" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" ht="60" spans="2:4">
       <c r="B13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:4">
       <c r="B14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:4">
       <c r="B15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="17" ht="120" spans="2:4">
       <c r="B17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19" s="9"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D24" s="9"/>
     </row>
     <row r="25" ht="75" spans="2:4">
       <c r="B25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="26" ht="45" spans="2:5">
       <c r="B26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="E26" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="27" ht="30" spans="2:4">
       <c r="B27" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" s="11"/>
     </row>
     <row r="29" ht="30" spans="2:4">
       <c r="B29" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D30" s="11"/>
     </row>
     <row r="31" ht="45" spans="2:5">
       <c r="B31" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" ht="30" spans="2:4">
       <c r="B32" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D32" s="11"/>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D33" s="11"/>
     </row>
     <row r="34" ht="30" spans="2:4">
       <c r="B34" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" ht="30" spans="2:4">
       <c r="B37" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D37" s="11"/>
     </row>
     <row r="38" ht="120" spans="2:5">
       <c r="B38" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="39" ht="120" spans="2:5">
       <c r="B39" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D42" s="9"/>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D43" s="9"/>
     </row>
     <row r="44" ht="195" spans="2:5">
       <c r="B44" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="E44" s="15" t="s">
         <v>141</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="45" ht="195" spans="2:5">
       <c r="B45" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" ht="195" spans="2:5">
       <c r="B46" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="E46" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="2:5">
       <c r="B47" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="4"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
       <c r="B49" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="4"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
       <c r="B50" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="4"/>
     </row>
     <row r="51" ht="150" spans="2:5">
       <c r="B51" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D52" s="9"/>
     </row>
     <row r="53" customFormat="1" spans="2:5">
       <c r="B53" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="4"/>
     </row>
     <row r="54" customFormat="1" spans="2:5">
       <c r="B54" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="4"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
       <c r="B55" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="4"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
       <c r="B56" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D57" s="9"/>
     </row>
     <row r="58" ht="180" spans="2:5">
       <c r="B58" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E58" s="15" t="s">
         <v>170</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="59" ht="75" spans="2:4">
       <c r="B59" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" ht="255" spans="2:5">
       <c r="B60" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="61" ht="135" spans="2:5">
       <c r="B61" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="62" ht="30" spans="2:3">
       <c r="B62" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" ht="30" spans="2:3">
       <c r="B63" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="65" ht="43" customHeight="1" spans="2:4">
       <c r="B65" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D65" s="11"/>
     </row>
@@ -7281,7 +7698,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -7291,7 +7708,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" ht="60" spans="2:7">
@@ -7302,7 +7719,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
@@ -7315,7 +7732,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -7323,186 +7740,186 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" ht="60" spans="2:6">
       <c r="B7" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" t="s">
         <v>193</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="D7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" ht="120" spans="2:5">
       <c r="B8" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="C10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="11" ht="225" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:5">
       <c r="B14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" t="s">
         <v>211</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="D14" t="s">
-        <v>213</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="16" ht="45" spans="2:5">
       <c r="B16" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="C16" t="s">
-        <v>220</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" ht="45" spans="2:5">
       <c r="B17" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="C17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" ht="45" spans="2:5">
       <c r="B18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C18" t="s">
-        <v>226</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>227</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" ht="60" spans="2:5">
       <c r="B19" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="1" ht="60" customHeight="1" spans="2:6">
       <c r="B21" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="4"/>
@@ -7524,6 +7941,310 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="33.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="49.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="56.552380952381" customWidth="1"/>
+    <col min="5" max="5" width="53.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="47.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="110" customHeight="1" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" customFormat="1" ht="30" spans="2:6">
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" ht="375" spans="2:5">
+      <c r="B9" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" ht="135" spans="2:5">
+      <c r="B10" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" ht="390" spans="2:6">
+      <c r="B14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="2:3">
+      <c r="B15" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" ht="30" spans="2:3">
+      <c r="B16" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="2:4">
+      <c r="B17" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="2:3">
+      <c r="B18" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" ht="45" spans="2:4">
+      <c r="B19" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C19" t="s">
+        <v>265</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" ht="315" spans="2:5">
+      <c r="B20" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" ht="45" spans="2:4">
+      <c r="B21" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" ht="46" customHeight="1" spans="2:4">
+      <c r="B24" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D24" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D23:D24"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7562,7 +8283,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7575,7 +8296,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7587,7 +8308,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7596,11 +8317,11 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -7609,7 +8330,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7617,212 +8338,183 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>236</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" ht="409.5" spans="2:5">
+      <c r="B9" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" ht="375" spans="2:5">
-      <c r="B9" s="5" t="s">
-        <v>240</v>
+      <c r="C9" t="s">
+        <v>278</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="180" spans="2:5">
+      <c r="B10" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="10" ht="135" spans="2:5">
-      <c r="B10" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="D10" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>246</v>
+        <v>280</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" ht="75" spans="2:4">
       <c r="B13" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="14" ht="390" spans="2:6">
-      <c r="B14" s="4" t="s">
-        <v>255</v>
+        <v>260</v>
+      </c>
+      <c r="C13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="2:3">
+      <c r="B14" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" ht="30" spans="2:3">
-      <c r="B15" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" ht="30" spans="2:3">
-      <c r="B16" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" ht="75" spans="2:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" ht="45" spans="2:4">
+      <c r="B15" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" t="s">
+        <v>265</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" ht="315" spans="2:5">
+      <c r="B16" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" t="s">
+        <v>268</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" ht="45" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="18" ht="30" spans="2:3">
-      <c r="B18" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="19" ht="45" spans="2:4">
-      <c r="B19" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C19" t="s">
-        <v>267</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="20" ht="315" spans="2:5">
-      <c r="B20" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" t="s">
         <v>270</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="C17" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="21" ht="45" spans="2:4">
-      <c r="B21" s="5" t="s">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
         <v>272</v>
       </c>
+      <c r="D18" t="s">
+        <v>273</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" ht="165" spans="2:5">
+      <c r="B19" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="E19" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" ht="46" customHeight="1" spans="2:4">
+      <c r="B21" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="C21" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" t="s">
-        <v>274</v>
-      </c>
-      <c r="D22" t="s">
-        <v>275</v>
-      </c>
-      <c r="E22" s="7" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="24" ht="46" customHeight="1" spans="2:4">
-      <c r="B24" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D24" s="11"/>
+      <c r="D21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F29"/>
@@ -7866,7 +8558,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -7877,7 +8569,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" ht="135" spans="1:5">
@@ -7889,10 +8581,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
@@ -7901,11 +8593,11 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -7914,7 +8606,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -7922,259 +8614,259 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" ht="105" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" ht="30" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="14" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" ht="120" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="E12" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="E14" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="60" spans="2:4">
       <c r="B15" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:3">
       <c r="B16" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" ht="60" spans="2:4">
       <c r="B17" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" ht="45" spans="2:5">
       <c r="B19" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
       <c r="B22" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" ht="60" spans="2:5">
       <c r="B23" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" ht="75" spans="2:5">
       <c r="B24" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" customFormat="1" ht="30" spans="2:5">
       <c r="B25" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" customFormat="1" ht="60" spans="2:5">
       <c r="B26" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:5">
       <c r="B27" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="2:4">
       <c r="B28" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B29" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="D29" s="11"/>
     </row>
@@ -8189,7 +8881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F31"/>
@@ -8238,7 +8930,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -8255,11 +8947,11 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -8268,7 +8960,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8276,176 +8968,176 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="D7" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" ht="165" spans="2:5">
       <c r="B8" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="4" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="4" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="4" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="1" ht="165" spans="2:5">
       <c r="B13" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:5">
       <c r="B17" s="4" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" ht="120" spans="2:5">
       <c r="B18" s="5" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="9" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" ht="105" spans="2:5">
       <c r="B19" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="1" ht="180" spans="2:6">
       <c r="B21" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="F21" s="4"/>
     </row>
     <row r="22" customFormat="1" ht="30" spans="2:6">
       <c r="B22" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -8453,23 +9145,23 @@
     </row>
     <row r="23" customFormat="1" ht="135" spans="2:6">
       <c r="B23" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" customFormat="1" ht="30" spans="2:6">
       <c r="B24" s="4" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="4"/>
@@ -8477,10 +9169,10 @@
     </row>
     <row r="25" customFormat="1" ht="30" spans="2:6">
       <c r="B25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="4"/>
@@ -8488,10 +9180,10 @@
     </row>
     <row r="26" customFormat="1" ht="30" spans="2:6">
       <c r="B26" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="4"/>
@@ -8499,10 +9191,10 @@
     </row>
     <row r="27" customFormat="1" ht="30" spans="2:6">
       <c r="B27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="4"/>
@@ -8510,10 +9202,10 @@
     </row>
     <row r="28" customFormat="1" ht="30" spans="2:6">
       <c r="B28" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="4"/>
@@ -8521,10 +9213,10 @@
     </row>
     <row r="29" customFormat="1" ht="30" spans="2:6">
       <c r="B29" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="4"/>
@@ -8532,21 +9224,21 @@
     </row>
     <row r="30" customFormat="1" spans="2:4">
       <c r="B30" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" customFormat="1" ht="46" customHeight="1" spans="2:4">
       <c r="B31" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D31" s="11"/>
     </row>
@@ -8559,7 +9251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F22"/>
@@ -8600,7 +9292,7 @@
     </row>
     <row r="2" ht="45" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8609,7 +9301,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8621,7 +9313,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
@@ -8630,11 +9322,11 @@
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -8643,7 +9335,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -8651,166 +9343,166 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" ht="390" spans="2:5">
       <c r="B9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" ht="135" spans="2:4">
       <c r="B10" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>243</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="11" ht="30" spans="2:3">
       <c r="B11" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:3">
       <c r="B13" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" ht="105" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:3">
       <c r="B15" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" ht="165" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" ht="75" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" ht="30" spans="2:3">
       <c r="B18" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:4">
       <c r="B19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="D19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" t="s">
+        <v>273</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="D20" t="s">
-        <v>275</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" ht="45" customHeight="1" spans="2:4">
       <c r="B22" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D22" s="11"/>
     </row>
@@ -8821,236 +9513,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="35.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="42.2857142857143" style="4" customWidth="1"/>
-    <col min="4" max="4" width="73.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="51.7142857142857" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" ht="20" customHeight="1" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>403</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" customFormat="1" spans="2:3">
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="5" customFormat="1" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" customFormat="1" ht="30" spans="2:6">
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D7" t="s">
-        <v>407</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" ht="120" spans="2:5">
-      <c r="B8" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="11" customFormat="1" spans="2:5">
-      <c r="B11" t="s">
-        <v>252</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E11" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" ht="60" spans="2:4">
-      <c r="B12" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" customFormat="1" ht="30" spans="2:3">
-      <c r="B13" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="14" customFormat="1" ht="45" spans="2:4">
-      <c r="B14" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C14" t="s">
-        <v>267</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="15" ht="60" spans="2:4">
-      <c r="B15" t="s">
-        <v>410</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" t="s">
-        <v>412</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="17" customFormat="1" spans="2:4">
-      <c r="B17" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
-      <c r="B18" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="D18" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D17:D18"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update ccda to fhir conversion specification document with changes in encounter status #1901
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="709" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12180" tabRatio="709" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="455">
   <si>
     <t>FHIR Resource Element column</t>
   </si>
@@ -2358,8 +2358,8 @@
     </r>
   </si>
   <si>
-    <t>Tentatively mapped the 'code' (eg. "housing-instability") from the mapping to question codes from IG.
-Is it needed the  "social-history" and "survey" codes in every Observations?</t>
+    <t xml:space="preserve">Tentatively mapped the 'code' (eg. "housing-instability") from the mapping to question codes from IG.
+</t>
   </si>
   <si>
     <t>code -&gt; coding -&gt; code</t>
@@ -2830,6 +2830,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"code": {
                     "coding": [
                         {
@@ -2864,6 +2871,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>For</t>
     </r>
     <r>
@@ -3092,7 +3106,54 @@
     <t>"status" : "finished",</t>
   </si>
   <si>
-    <t>Path to get the status</t>
+    <r>
+      <t xml:space="preserve">For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCDA files:
+Document.component.structuredBody.component.section.entry.encounter.statusCode.code
+For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CCDA files:
+Document.component.structuredBody.component.section.entry.encounter.entryRelationship.act.entryRelationship.observation.statusCode.code</t>
+    </r>
   </si>
   <si>
     <t>class -&gt; code</t>
@@ -4437,6 +4498,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">This is now removed from the FHIR bundle.
 </t>
     </r>
@@ -4509,6 +4577,9 @@
   </si>
   <si>
     <t>"status" : "completed",</t>
+  </si>
+  <si>
+    <t>Path to get the status</t>
   </si>
   <si>
     <t>Tentatively mapped the code -&gt;  displayName</t>
@@ -5080,16 +5151,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.25"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5105,7 +5169,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5123,6 +5187,13 @@
       <strike/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.25"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5590,7 +5661,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5644,9 +5715,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6210,13 +6278,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.88571428571429" style="23"/>
+    <col min="1" max="1" width="8.88571428571429" style="22"/>
     <col min="2" max="2" width="35.2190476190476" customWidth="1"/>
     <col min="3" max="3" width="92.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="23">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -6227,7 +6295,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -6238,7 +6306,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -6249,10 +6317,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -6260,10 +6328,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>5</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
@@ -6382,7 +6450,7 @@
         <v>415</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>292</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" ht="120" spans="2:5">
@@ -6426,7 +6494,7 @@
         <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" customFormat="1" ht="60" spans="2:4">
@@ -6456,23 +6524,23 @@
         <v>265</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" ht="60" spans="2:4">
       <c r="B15" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>311</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>314</v>
@@ -6486,7 +6554,7 @@
         <v>183</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -6494,7 +6562,7 @@
         <v>185</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D18" s="11"/>
     </row>
@@ -6558,7 +6626,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6592,7 +6660,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -6600,10 +6668,10 @@
     </row>
     <row r="7" ht="30" spans="2:5">
       <c r="B7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>148</v>
@@ -6611,10 +6679,10 @@
     </row>
     <row r="8" ht="30" spans="2:5">
       <c r="B8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>148</v>
@@ -6625,101 +6693,101 @@
         <v>191</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:5">
       <c r="B11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" ht="45" spans="2:5">
       <c r="B12" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" ht="45" spans="2:5">
       <c r="B13" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" ht="45" spans="2:5">
       <c r="B14" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" ht="45" spans="2:5">
       <c r="B15" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -6758,7 +6826,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -6936,11 +7004,10 @@
       </c>
     </row>
     <row r="22" ht="30" spans="2:5">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C22"/>
-      <c r="E22" s="22"/>
+      <c r="E22" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7241,7 +7308,7 @@
       <c r="C26" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="20" t="s">
         <v>106</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -7697,11 +7764,11 @@
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="4" t="s">
@@ -7718,11 +7785,11 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="5" t="s">
@@ -7941,7 +8008,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8244,7 +8311,7 @@
   <sheetPr/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8477,7 +8544,7 @@
       <c r="B19" t="s">
         <v>283</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="4" t="s">
         <v>284</v>
       </c>
       <c r="E19" t="s">
@@ -8519,8 +8586,8 @@
   <sheetPr/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8612,17 +8679,15 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" ht="120" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>235</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="D7" t="s">
         <v>291</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="15" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>